<commit_message>
Dejando paths lindos para correr main
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -1,14 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb563583\GitHub\VEN\data_management\management\4. income imputation\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09DCB80-4004-41E3-AD9F-FD7DFE04CABF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="91">
   <si>
     <t>2019</t>
   </si>
@@ -303,7 +297,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -565,14 +559,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -872,7 +858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView showGridLines="false" tabSelected="true" workbookViewId="0">
@@ -905,10 +891,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="22">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C4" s="22">
-        <v>1.4713175731525872</v>
+        <v>1.4365152919369786</v>
       </c>
     </row>
     <row r="5" ht="29">
@@ -916,10 +902,10 @@
         <v>62</v>
       </c>
       <c r="B5" s="22">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="C5" s="22">
-        <v>2.6946602744255248</v>
+        <v>2.7494593759654</v>
       </c>
     </row>
     <row r="6" ht="29">
@@ -927,10 +913,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="22">
-        <v>1528</v>
+        <v>1671</v>
       </c>
       <c r="C6" s="22">
-        <v>12.630186807736814</v>
+        <v>12.905468025949954</v>
       </c>
     </row>
     <row r="7">
@@ -949,10 +935,10 @@
         <v>65</v>
       </c>
       <c r="B8" s="23">
-        <v>1854</v>
+        <v>2027</v>
       </c>
       <c r="C8" s="22">
-        <v>15.324847082162341</v>
+        <v>15.654927401915353</v>
       </c>
     </row>
     <row r="9">
@@ -960,10 +946,10 @@
         <v>66</v>
       </c>
       <c r="B9" s="22">
-        <v>9995</v>
+        <v>10658</v>
       </c>
       <c r="C9" s="22">
-        <v>82.616961481236572</v>
+        <v>82.313870868087733</v>
       </c>
     </row>
     <row r="10">
@@ -971,7 +957,7 @@
         <v>67</v>
       </c>
       <c r="B10" s="25">
-        <v>12098</v>
+        <v>12948</v>
       </c>
       <c r="C10" s="25">
         <v>100</v>
@@ -987,10 +973,10 @@
         <v>69</v>
       </c>
       <c r="B15" s="22">
-        <v>21776</v>
+        <v>23404</v>
       </c>
       <c r="C15" s="22">
-        <v>369.96262317363232</v>
+        <v>374.16466826538766</v>
       </c>
     </row>
     <row r="16" ht="29">
@@ -1001,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="22">
-        <v>0.11892626571525654</v>
+        <v>0.11191047162270183</v>
       </c>
     </row>
     <row r="17" ht="29">
@@ -1012,7 +998,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="22">
-        <v>0.3058103975535168</v>
+        <v>0.28776978417266186</v>
       </c>
     </row>
     <row r="18">
@@ -1034,7 +1020,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="22">
-        <v>0.42473666326877335</v>
+        <v>0.3996802557953637</v>
       </c>
     </row>
     <row r="20">
@@ -1042,10 +1028,10 @@
         <v>66</v>
       </c>
       <c r="B20" s="22">
-        <v>5797</v>
+        <v>6160</v>
       </c>
       <c r="C20" s="22">
-        <v>98.487937478763172</v>
+        <v>98.481215027977626</v>
       </c>
     </row>
     <row r="21" ht="29">
@@ -1053,7 +1039,7 @@
         <v>72</v>
       </c>
       <c r="B21" s="25">
-        <v>5886</v>
+        <v>6255</v>
       </c>
       <c r="C21" s="25">
         <v>100</v>
@@ -1072,7 +1058,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="22">
-        <v>1.8382352941176472</v>
+        <v>1.6816143497757847</v>
       </c>
     </row>
     <row r="27" ht="29">
@@ -1080,10 +1066,10 @@
         <v>75</v>
       </c>
       <c r="B27" s="22">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C27" s="22">
-        <v>1.9607843137254901</v>
+        <v>2.2421524663677128</v>
       </c>
     </row>
     <row r="28">
@@ -1094,7 +1080,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="22">
-        <v>0.24509803921568626</v>
+        <v>0.22421524663677131</v>
       </c>
     </row>
     <row r="29">
@@ -1102,10 +1088,10 @@
         <v>76</v>
       </c>
       <c r="B29" s="23">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C29" s="22">
-        <v>2.2058823529411766</v>
+        <v>2.4663677130044843</v>
       </c>
     </row>
     <row r="30">
@@ -1113,10 +1099,10 @@
         <v>66</v>
       </c>
       <c r="B30" s="22">
-        <v>783</v>
+        <v>855</v>
       </c>
       <c r="C30" s="22">
-        <v>95.955882352941174</v>
+        <v>95.852017937219742</v>
       </c>
     </row>
     <row r="31">
@@ -1124,7 +1110,7 @@
         <v>77</v>
       </c>
       <c r="B31" s="25">
-        <v>816</v>
+        <v>892</v>
       </c>
       <c r="C31" s="25">
         <v>100</v>
@@ -1140,10 +1126,10 @@
         <v>79</v>
       </c>
       <c r="B36" s="22">
-        <v>23602</v>
+        <v>25088</v>
       </c>
       <c r="C36" s="22">
-        <v>317.829248586049</v>
+        <v>314.26781911562068</v>
       </c>
     </row>
     <row r="37" ht="29">
@@ -1151,10 +1137,10 @@
         <v>80</v>
       </c>
       <c r="B37" s="22">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C37" s="22">
-        <v>0.60597899272825206</v>
+        <v>0.71401728673431042</v>
       </c>
     </row>
     <row r="38">
@@ -1169,10 +1155,10 @@
         <v>76</v>
       </c>
       <c r="B39" s="23">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C39" s="22">
-        <v>0.60597899272825206</v>
+        <v>0.71401728673431042</v>
       </c>
     </row>
     <row r="40">
@@ -1180,10 +1166,10 @@
         <v>66</v>
       </c>
       <c r="B40" s="22">
-        <v>7375</v>
+        <v>7919</v>
       </c>
       <c r="C40" s="22">
-        <v>99.313223808241318</v>
+        <v>99.19829637980709</v>
       </c>
     </row>
     <row r="41" ht="29">
@@ -1191,7 +1177,7 @@
         <v>81</v>
       </c>
       <c r="B41" s="25">
-        <v>7426</v>
+        <v>7983</v>
       </c>
       <c r="C41" s="25">
         <v>100</v>
@@ -1208,7 +1194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showGridLines="false" workbookViewId="0">
@@ -1245,7 +1231,7 @@
     </row>
     <row r="4" s="13" customFormat="true" ht="12">
       <c r="B4" s="14">
-        <v>31.445523193096008</v>
+        <v>31.277750370004931</v>
       </c>
       <c r="C4" s="14">
         <v>48</v>
@@ -1256,7 +1242,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="5">
-        <v>68.554476806903992</v>
+        <v>68.722249629995076</v>
       </c>
       <c r="C5" s="5">
         <v>52</v>
@@ -1275,7 +1261,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="5">
-        <v>0.37756202804746497</v>
+        <v>0.34533793783917122</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -1287,7 +1273,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="5">
-        <v>12.513484358144552</v>
+        <v>12.530833744449927</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -1299,7 +1285,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="5">
-        <v>22.491909385113267</v>
+        <v>22.792303897385299</v>
       </c>
       <c r="C9" s="5">
         <v>0</v>
@@ -1311,7 +1297,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="5">
-        <v>23.247033441208199</v>
+        <v>23.038973852984707</v>
       </c>
       <c r="C10" s="5">
         <v>4</v>
@@ -1323,7 +1309,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="5">
-        <v>19.741100323624593</v>
+        <v>19.980266403552047</v>
       </c>
       <c r="C11" s="5">
         <v>16</v>
@@ -1335,7 +1321,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="5">
-        <v>14.724919093851133</v>
+        <v>14.50419338924519</v>
       </c>
       <c r="C12" s="5">
         <v>36</v>
@@ -1347,7 +1333,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="5">
-        <v>6.9039913700107869</v>
+        <v>6.8080907745436612</v>
       </c>
       <c r="C13" s="5">
         <v>44</v>
@@ -1367,7 +1353,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="5">
-        <v>23.408845738942826</v>
+        <v>24.124321657622101</v>
       </c>
       <c r="C15" s="5">
         <v>36</v>
@@ -1379,7 +1365,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="5">
-        <v>33.117583603020492</v>
+        <v>32.807104094721261</v>
       </c>
       <c r="C16" s="5">
         <v>20</v>
@@ -1391,7 +1377,7 @@
         <v>54</v>
       </c>
       <c r="B17" s="5">
-        <v>29.935275080906148</v>
+        <v>29.551060680809076</v>
       </c>
       <c r="C17" s="5">
         <v>8</v>
@@ -1403,7 +1389,7 @@
         <v>58</v>
       </c>
       <c r="B18" s="5">
-        <v>10.841423948220065</v>
+        <v>10.853478046373951</v>
       </c>
       <c r="C18" s="5">
         <v>12</v>
@@ -1415,7 +1401,7 @@
         <v>55</v>
       </c>
       <c r="B19" s="5">
-        <v>2.535059331175836</v>
+        <v>2.5160335471139614</v>
       </c>
       <c r="C19" s="5">
         <v>24</v>
@@ -1427,7 +1413,7 @@
         <v>56</v>
       </c>
       <c r="B20" s="5">
-        <v>0.16181229773462785</v>
+        <v>0.1480019733596448</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -1447,7 +1433,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="5">
-        <v>0.37756202804746497</v>
+        <v>0.34533793783917122</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -1459,7 +1445,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="17">
-        <v>0.16181229773462785</v>
+        <v>0.1480019733596448</v>
       </c>
       <c r="C23" s="17">
         <v>0</v>
@@ -1471,7 +1457,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="5">
-        <v>26.375404530744333</v>
+        <v>26.985693142575233</v>
       </c>
       <c r="C24" s="5">
         <v>48</v>
@@ -1483,7 +1469,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="5">
-        <v>48.2740021574973</v>
+        <v>48.001973359644794</v>
       </c>
       <c r="C25" s="5">
         <v>16</v>
@@ -1495,7 +1481,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="5">
-        <v>5.2319309600862995</v>
+        <v>5.1307350764676869</v>
       </c>
       <c r="C26" s="5">
         <v>4</v>
@@ -1507,7 +1493,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="5">
-        <v>14.347357065803667</v>
+        <v>14.208189442525901</v>
       </c>
       <c r="C27" s="5">
         <v>20</v>
@@ -1519,7 +1505,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="5">
-        <v>0.3236245954692557</v>
+        <v>0.39467192895905284</v>
       </c>
       <c r="C28" s="5">
         <v>0</v>
@@ -1531,7 +1517,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="5">
-        <v>4.9083063646170437</v>
+        <v>4.7853971386285155</v>
       </c>
       <c r="C29" s="5">
         <v>12</v>
@@ -1551,7 +1537,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="5">
-        <v>4.4768069039913696</v>
+        <v>4.3413912185495809</v>
       </c>
       <c r="C31" s="5">
         <v>0</v>
@@ -1563,7 +1549,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="5">
-        <v>3.8834951456310676</v>
+        <v>4.1440552540700546</v>
       </c>
       <c r="C32" s="5">
         <v>0</v>
@@ -1575,7 +1561,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="5">
-        <v>11.596548004314995</v>
+        <v>11.001480019733597</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
@@ -1587,7 +1573,7 @@
         <v>39</v>
       </c>
       <c r="B34" s="5">
-        <v>72.545846817691469</v>
+        <v>73.162308830784411</v>
       </c>
       <c r="C34" s="5">
         <v>4</v>
@@ -1599,7 +1585,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5">
-        <v>0.3236245954692557</v>
+        <v>0.39467192895905284</v>
       </c>
       <c r="C35" s="5">
         <v>0</v>
@@ -1611,7 +1597,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="5">
-        <v>4.1531823085221147</v>
+        <v>4.0453872718302915</v>
       </c>
       <c r="C36" s="5">
         <v>0</v>
@@ -1623,7 +1609,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="5">
-        <v>2.8586839266450914</v>
+        <v>2.7133695115934877</v>
       </c>
       <c r="C37" s="5">
         <v>0</v>
@@ -1635,7 +1621,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="5">
-        <v>0.16181229773462785</v>
+        <v>0.19733596447952642</v>
       </c>
       <c r="C38" s="5">
         <v>92</v>
@@ -1655,7 +1641,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="5">
-        <v>17.637540453074433</v>
+        <v>18.697582634435125</v>
       </c>
       <c r="C40" s="5">
         <v>0</v>
@@ -1667,7 +1653,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="17">
-        <v>0.70118662351672068</v>
+        <v>0.64134188455846086</v>
       </c>
       <c r="C41" s="17">
         <v>0</v>
@@ -1679,7 +1665,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5">
-        <v>1.8338727076591153</v>
+        <v>1.6773556980759743</v>
       </c>
       <c r="C42" s="5">
         <v>4</v>
@@ -1692,7 +1678,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="5">
-        <v>1.2405609492988134</v>
+        <v>1.1840157868771584</v>
       </c>
       <c r="C43" s="5">
         <v>0</v>
@@ -1704,7 +1690,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="5">
-        <v>6.1488673139158578</v>
+        <v>5.920078934385792</v>
       </c>
       <c r="C44" s="5">
         <v>0</v>
@@ -1716,7 +1702,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="5">
-        <v>20.819848975188783</v>
+        <v>20.720276270350272</v>
       </c>
       <c r="C45" s="5">
         <v>0</v>
@@ -1728,7 +1714,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="5">
-        <v>12.459546925566343</v>
+        <v>12.530833744449927</v>
       </c>
       <c r="C46" s="5">
         <v>0</v>
@@ -1740,7 +1726,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="5">
-        <v>2.9665587918015102</v>
+        <v>2.8120374938332513</v>
       </c>
       <c r="C47" s="5">
         <v>0</v>
@@ -1752,7 +1738,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="5">
-        <v>6.0409924487594395</v>
+        <v>5.8214109521460289</v>
       </c>
       <c r="C48" s="5">
         <v>0</v>
@@ -1764,7 +1750,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="5">
-        <v>29.989212513484357</v>
+        <v>29.797730636408488</v>
       </c>
       <c r="C49" s="5">
         <v>4</v>
@@ -1776,7 +1762,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="5">
-        <v>0.16181229773462785</v>
+        <v>0.19733596447952642</v>
       </c>
       <c r="C50" s="5">
         <v>92</v>
@@ -1796,7 +1782,7 @@
         <v>37</v>
       </c>
       <c r="B52" s="5">
-        <v>19.579288025889969</v>
+        <v>18.894918598914654</v>
       </c>
       <c r="C52" s="5">
         <v>16</v>
@@ -1808,7 +1794,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="17">
-        <v>80.420711974110034</v>
+        <v>81.105081401085343</v>
       </c>
       <c r="C53" s="17">
         <v>84</v>
@@ -2028,7 +2014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2108,13 +2094,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>2028753.8251743021</v>
+        <v>2013340.0766250594</v>
       </c>
       <c r="C4" s="7">
         <v>251904.90625</v>
       </c>
       <c r="D4" s="7">
-        <v>453428.84375</v>
+        <v>454765.71875</v>
       </c>
       <c r="E4" s="7">
         <v>1000000</v>
@@ -2126,22 +2112,22 @@
         <v>4030478.5</v>
       </c>
       <c r="H4" s="7">
-        <v>2032165.1573092239</v>
+        <v>2016833.1326708435</v>
       </c>
       <c r="I4" s="7">
         <v>251904.90625</v>
       </c>
       <c r="J4" s="7">
-        <v>468543.125</v>
+        <v>468985.25</v>
       </c>
       <c r="K4" s="7">
-        <v>1000309.25</v>
+        <v>1007619.5625</v>
       </c>
       <c r="L4" s="7">
-        <v>2618299.75</v>
+        <v>2606851.5</v>
       </c>
       <c r="M4" s="8">
-        <v>4101364.75</v>
+        <v>4042826.25</v>
       </c>
     </row>
     <row r="7">
@@ -2160,7 +2146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2246,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>1520282.7252662426</v>
+        <v>1519927.2796204803</v>
       </c>
       <c r="C4" s="7">
         <v>250000</v>
@@ -2264,7 +2250,7 @@
         <v>2556470.5</v>
       </c>
       <c r="H4" s="7">
-        <v>1517829.7767320566</v>
+        <v>1521645.8887279662</v>
       </c>
       <c r="I4" s="7">
         <v>250000</v>
@@ -2303,7 +2289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2383,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>6821405.5753792245</v>
+        <v>9458464.3975915201</v>
       </c>
       <c r="C4" s="7">
         <v>120914.3515625</v>
@@ -2398,13 +2384,13 @@
         <v>500000</v>
       </c>
       <c r="G4" s="8">
-        <v>930202.1875</v>
+        <v>927010</v>
       </c>
       <c r="H4" s="7">
-        <v>6782799.1977904821</v>
+        <v>9394301.2418644987</v>
       </c>
       <c r="I4" s="7">
-        <v>120914.3515625</v>
+        <v>120581.8125</v>
       </c>
       <c r="J4" s="7">
         <v>201523.921875</v>
@@ -2416,7 +2402,7 @@
         <v>500000</v>
       </c>
       <c r="M4" s="8">
-        <v>930202.5625</v>
+        <v>930000</v>
       </c>
       <c r="N4" s="1">
         <v>834001</v>
@@ -2440,7 +2426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2520,40 +2506,40 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>906798.14155800745</v>
+        <v>868703.25247404724</v>
       </c>
       <c r="C4" s="7">
         <v>55419.078125</v>
       </c>
       <c r="D4" s="7">
-        <v>200000</v>
+        <v>188103.75</v>
       </c>
       <c r="E4" s="7">
-        <v>321051.34375</v>
+        <v>302285.875</v>
       </c>
       <c r="F4" s="7">
-        <v>906857.6875</v>
+        <v>860511.875</v>
       </c>
       <c r="G4" s="8">
-        <v>2015239.25</v>
+        <v>2000000</v>
       </c>
       <c r="H4" s="7">
-        <v>1034146.9053917929</v>
+        <v>881703.5860890263</v>
       </c>
       <c r="I4" s="7">
         <v>55419.078125</v>
       </c>
       <c r="J4" s="7">
-        <v>200000</v>
+        <v>196485.828125</v>
       </c>
       <c r="K4" s="7">
-        <v>332514.46875</v>
+        <v>320000</v>
       </c>
       <c r="L4" s="7">
-        <v>978442.25</v>
+        <v>860511.875</v>
       </c>
       <c r="M4" s="8">
-        <v>2015239.25</v>
+        <v>2000000</v>
       </c>
       <c r="N4" s="1">
         <v>2015239.25</v>

</xml_diff>

<commit_message>
TC actualizacion y Final Keep
Correcciones al do de TC y creacion de DO con las variables a dropear y keep antes de compartir base
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="91">
   <si>
     <t>2019</t>
   </si>
@@ -905,10 +905,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="22">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C4" s="22">
-        <v>1.4713175731525872</v>
+        <v>1.4410375470338643</v>
       </c>
     </row>
     <row r="5" ht="29">
@@ -916,10 +916,10 @@
         <v>62</v>
       </c>
       <c r="B5" s="22">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="C5" s="22">
-        <v>2.6946602744255248</v>
+        <v>2.7860059242654711</v>
       </c>
     </row>
     <row r="6" ht="29">
@@ -927,10 +927,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="22">
-        <v>1528</v>
+        <v>1579</v>
       </c>
       <c r="C6" s="22">
-        <v>12.630186807736814</v>
+        <v>12.641101593147066</v>
       </c>
     </row>
     <row r="7">
@@ -949,10 +949,10 @@
         <v>65</v>
       </c>
       <c r="B8" s="23">
-        <v>1854</v>
+        <v>1927</v>
       </c>
       <c r="C8" s="22">
-        <v>15.324847082162341</v>
+        <v>15.427107517412535</v>
       </c>
     </row>
     <row r="9">
@@ -960,10 +960,10 @@
         <v>66</v>
       </c>
       <c r="B9" s="22">
-        <v>9995</v>
+        <v>10310</v>
       </c>
       <c r="C9" s="22">
-        <v>82.616961481236572</v>
+        <v>82.539428388439674</v>
       </c>
     </row>
     <row r="10">
@@ -971,7 +971,7 @@
         <v>67</v>
       </c>
       <c r="B10" s="25">
-        <v>12098</v>
+        <v>12491</v>
       </c>
       <c r="C10" s="25">
         <v>100</v>
@@ -987,10 +987,10 @@
         <v>69</v>
       </c>
       <c r="B15" s="22">
-        <v>21776</v>
+        <v>22499</v>
       </c>
       <c r="C15" s="22">
-        <v>369.96262317363232</v>
+        <v>370.04934210526318</v>
       </c>
     </row>
     <row r="16" ht="29">
@@ -1001,7 +1001,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="22">
-        <v>0.11892626571525654</v>
+        <v>0.1151315789473684</v>
       </c>
     </row>
     <row r="17" ht="29">
@@ -1012,7 +1012,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="22">
-        <v>0.3058103975535168</v>
+        <v>0.2960526315789474</v>
       </c>
     </row>
     <row r="18">
@@ -1034,7 +1034,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="22">
-        <v>0.42473666326877335</v>
+        <v>0.41118421052631576</v>
       </c>
     </row>
     <row r="20">
@@ -1042,10 +1042,10 @@
         <v>66</v>
       </c>
       <c r="B20" s="22">
-        <v>5797</v>
+        <v>5990</v>
       </c>
       <c r="C20" s="22">
-        <v>98.487937478763172</v>
+        <v>98.51973684210526</v>
       </c>
     </row>
     <row r="21" ht="29">
@@ -1053,7 +1053,7 @@
         <v>72</v>
       </c>
       <c r="B21" s="25">
-        <v>5886</v>
+        <v>6080</v>
       </c>
       <c r="C21" s="25">
         <v>100</v>
@@ -1072,7 +1072,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="22">
-        <v>1.8382352941176472</v>
+        <v>1.7201834862385321</v>
       </c>
     </row>
     <row r="27" ht="29">
@@ -1080,10 +1080,10 @@
         <v>75</v>
       </c>
       <c r="B27" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" s="22">
-        <v>1.9607843137254901</v>
+        <v>1.9495412844036699</v>
       </c>
     </row>
     <row r="28">
@@ -1094,7 +1094,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="22">
-        <v>0.24509803921568626</v>
+        <v>0.22935779816513763</v>
       </c>
     </row>
     <row r="29">
@@ -1102,10 +1102,10 @@
         <v>76</v>
       </c>
       <c r="B29" s="23">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="22">
-        <v>2.2058823529411766</v>
+        <v>2.1788990825688073</v>
       </c>
     </row>
     <row r="30">
@@ -1113,10 +1113,10 @@
         <v>66</v>
       </c>
       <c r="B30" s="22">
-        <v>783</v>
+        <v>838</v>
       </c>
       <c r="C30" s="22">
-        <v>95.955882352941174</v>
+        <v>96.100917431192656</v>
       </c>
     </row>
     <row r="31">
@@ -1124,7 +1124,7 @@
         <v>77</v>
       </c>
       <c r="B31" s="25">
-        <v>816</v>
+        <v>872</v>
       </c>
       <c r="C31" s="25">
         <v>100</v>
@@ -1140,10 +1140,10 @@
         <v>79</v>
       </c>
       <c r="B36" s="22">
-        <v>23602</v>
+        <v>24291</v>
       </c>
       <c r="C36" s="22">
-        <v>317.829248586049</v>
+        <v>315.9599375650364</v>
       </c>
     </row>
     <row r="37" ht="29">
@@ -1151,10 +1151,10 @@
         <v>80</v>
       </c>
       <c r="B37" s="22">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C37" s="22">
-        <v>0.60597899272825206</v>
+        <v>0.70239334027055156</v>
       </c>
     </row>
     <row r="38">
@@ -1169,10 +1169,10 @@
         <v>76</v>
       </c>
       <c r="B39" s="23">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C39" s="22">
-        <v>0.60597899272825206</v>
+        <v>0.70239334027055156</v>
       </c>
     </row>
     <row r="40">
@@ -1180,10 +1180,10 @@
         <v>66</v>
       </c>
       <c r="B40" s="22">
-        <v>7375</v>
+        <v>7627</v>
       </c>
       <c r="C40" s="22">
-        <v>99.313223808241318</v>
+        <v>99.206555671175849</v>
       </c>
     </row>
     <row r="41" ht="29">
@@ -1191,7 +1191,7 @@
         <v>81</v>
       </c>
       <c r="B41" s="25">
-        <v>7426</v>
+        <v>7688</v>
       </c>
       <c r="C41" s="25">
         <v>100</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="4" s="13" customFormat="true" ht="12">
       <c r="B4" s="14">
-        <v>31.445523193096008</v>
+        <v>31.551634665282823</v>
       </c>
       <c r="C4" s="14">
         <v>48</v>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="5">
-        <v>68.554476806903992</v>
+        <v>68.448365334717181</v>
       </c>
       <c r="C5" s="5">
         <v>52</v>
@@ -1275,7 +1275,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="5">
-        <v>0.37756202804746497</v>
+        <v>0.36325895173845357</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="5">
-        <v>12.513484358144552</v>
+        <v>12.454592631032693</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -1299,7 +1299,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="5">
-        <v>22.491909385113267</v>
+        <v>22.625843279709393</v>
       </c>
       <c r="C9" s="5">
         <v>0</v>
@@ -1311,7 +1311,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="5">
-        <v>23.247033441208199</v>
+        <v>23.196678775298391</v>
       </c>
       <c r="C10" s="5">
         <v>4</v>
@@ -1323,7 +1323,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="5">
-        <v>19.741100323624593</v>
+        <v>19.615983393876494</v>
       </c>
       <c r="C11" s="5">
         <v>16</v>
@@ -1335,7 +1335,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="5">
-        <v>14.724919093851133</v>
+        <v>14.737934613388687</v>
       </c>
       <c r="C12" s="5">
         <v>36</v>
@@ -1347,7 +1347,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="5">
-        <v>6.9039913700107869</v>
+        <v>7.0057083549558907</v>
       </c>
       <c r="C13" s="5">
         <v>44</v>
@@ -1367,7 +1367,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="5">
-        <v>23.408845738942826</v>
+        <v>23.456149455111571</v>
       </c>
       <c r="C15" s="5">
         <v>36</v>
@@ -1379,7 +1379,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="5">
-        <v>33.117583603020492</v>
+        <v>33.004670472236633</v>
       </c>
       <c r="C16" s="5">
         <v>20</v>
@@ -1391,7 +1391,7 @@
         <v>54</v>
       </c>
       <c r="B17" s="5">
-        <v>29.935275080906148</v>
+        <v>29.9429164504411</v>
       </c>
       <c r="C17" s="5">
         <v>8</v>
@@ -1403,7 +1403,7 @@
         <v>58</v>
       </c>
       <c r="B18" s="5">
-        <v>10.841423948220065</v>
+        <v>10.949662688116243</v>
       </c>
       <c r="C18" s="5">
         <v>12</v>
@@ -1415,7 +1415,7 @@
         <v>55</v>
       </c>
       <c r="B19" s="5">
-        <v>2.535059331175836</v>
+        <v>2.4909185262065385</v>
       </c>
       <c r="C19" s="5">
         <v>24</v>
@@ -1427,7 +1427,7 @@
         <v>56</v>
       </c>
       <c r="B20" s="5">
-        <v>0.16181229773462785</v>
+        <v>0.15568240788790866</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -1447,7 +1447,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="5">
-        <v>0.37756202804746497</v>
+        <v>0.36325895173845357</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -1459,7 +1459,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="17">
-        <v>0.16181229773462785</v>
+        <v>0.15568240788790866</v>
       </c>
       <c r="C23" s="17">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="5">
-        <v>26.375404530744333</v>
+        <v>26.777374156720292</v>
       </c>
       <c r="C24" s="5">
         <v>48</v>
@@ -1483,7 +1483,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="5">
-        <v>48.2740021574973</v>
+        <v>48.209652309289055</v>
       </c>
       <c r="C25" s="5">
         <v>16</v>
@@ -1495,7 +1495,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="5">
-        <v>5.2319309600862995</v>
+        <v>5.1894135962636225</v>
       </c>
       <c r="C26" s="5">
         <v>4</v>
@@ -1507,7 +1507,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="5">
-        <v>14.347357065803667</v>
+        <v>14.011416709911781</v>
       </c>
       <c r="C27" s="5">
         <v>20</v>
@@ -1519,7 +1519,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="5">
-        <v>0.3236245954692557</v>
+        <v>0.31136481577581732</v>
       </c>
       <c r="C28" s="5">
         <v>0</v>
@@ -1531,7 +1531,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="5">
-        <v>4.9083063646170437</v>
+        <v>4.9818370524130771</v>
       </c>
       <c r="C29" s="5">
         <v>12</v>
@@ -1551,7 +1551,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="5">
-        <v>4.4768069039913696</v>
+        <v>4.4628956927867147</v>
       </c>
       <c r="C31" s="5">
         <v>0</v>
@@ -1563,7 +1563,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="5">
-        <v>3.8834951456310676</v>
+        <v>4.3072132848988067</v>
       </c>
       <c r="C32" s="5">
         <v>0</v>
@@ -1575,7 +1575,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="5">
-        <v>11.596548004314995</v>
+        <v>11.572392319667877</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
@@ -1587,7 +1587,7 @@
         <v>39</v>
       </c>
       <c r="B34" s="5">
-        <v>72.545846817691469</v>
+        <v>72.288531395952262</v>
       </c>
       <c r="C34" s="5">
         <v>4</v>
@@ -1599,7 +1599,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5">
-        <v>0.3236245954692557</v>
+        <v>0.36325895173845357</v>
       </c>
       <c r="C35" s="5">
         <v>0</v>
@@ -1611,7 +1611,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="5">
-        <v>4.1531823085221147</v>
+        <v>4.0477426050856256</v>
       </c>
       <c r="C36" s="5">
         <v>0</v>
@@ -1623,7 +1623,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="5">
-        <v>2.8586839266450914</v>
+        <v>2.7503892060197197</v>
       </c>
       <c r="C37" s="5">
         <v>0</v>
@@ -1635,7 +1635,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="5">
-        <v>0.16181229773462785</v>
+        <v>0.20757654385054489</v>
       </c>
       <c r="C38" s="5">
         <v>92</v>
@@ -1655,7 +1655,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="5">
-        <v>17.637540453074433</v>
+        <v>18.266735858847948</v>
       </c>
       <c r="C40" s="5">
         <v>0</v>
@@ -1667,7 +1667,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="17">
-        <v>0.70118662351672068</v>
+        <v>0.67462376751427089</v>
       </c>
       <c r="C41" s="17">
         <v>0</v>
@@ -1679,7 +1679,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5">
-        <v>1.8338727076591153</v>
+        <v>1.7644006227296314</v>
       </c>
       <c r="C42" s="5">
         <v>4</v>
@@ -1692,7 +1692,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="5">
-        <v>1.2405609492988134</v>
+        <v>1.2454592631032693</v>
       </c>
       <c r="C43" s="5">
         <v>0</v>
@@ -1704,7 +1704,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="5">
-        <v>6.1488673139158578</v>
+        <v>6.123508043591074</v>
       </c>
       <c r="C44" s="5">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="5">
-        <v>20.819848975188783</v>
+        <v>20.550077841203944</v>
       </c>
       <c r="C45" s="5">
         <v>0</v>
@@ -1728,7 +1728,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="5">
-        <v>12.459546925566343</v>
+        <v>12.817851582771148</v>
       </c>
       <c r="C46" s="5">
         <v>0</v>
@@ -1740,7 +1740,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="5">
-        <v>2.9665587918015102</v>
+        <v>2.9060716139076286</v>
       </c>
       <c r="C47" s="5">
         <v>0</v>
@@ -1752,7 +1752,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="5">
-        <v>6.0409924487594395</v>
+        <v>6.0716139076284374</v>
       </c>
       <c r="C48" s="5">
         <v>0</v>
@@ -1764,7 +1764,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="5">
-        <v>29.989212513484357</v>
+        <v>29.372080954852102</v>
       </c>
       <c r="C49" s="5">
         <v>4</v>
@@ -1776,7 +1776,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="5">
-        <v>0.16181229773462785</v>
+        <v>0.20757654385054489</v>
       </c>
       <c r="C50" s="5">
         <v>92</v>
@@ -1796,7 +1796,7 @@
         <v>37</v>
       </c>
       <c r="B52" s="5">
-        <v>19.579288025889969</v>
+        <v>19.564089257913857</v>
       </c>
       <c r="C52" s="5">
         <v>16</v>
@@ -1808,7 +1808,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="17">
-        <v>80.420711974110034</v>
+        <v>80.435910742086151</v>
       </c>
       <c r="C53" s="17">
         <v>84</v>
@@ -2108,40 +2108,40 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>2028753.8251743021</v>
+        <v>2035627.05475047</v>
       </c>
       <c r="C4" s="7">
-        <v>251904.90625</v>
+        <v>252179.71875</v>
       </c>
       <c r="D4" s="7">
-        <v>453428.84375</v>
+        <v>453923.5</v>
       </c>
       <c r="E4" s="7">
-        <v>1000000</v>
+        <v>1008718.875</v>
       </c>
       <c r="F4" s="7">
         <v>2653803.75</v>
       </c>
       <c r="G4" s="8">
-        <v>4030478.5</v>
+        <v>4034875.5</v>
       </c>
       <c r="H4" s="7">
-        <v>2032165.1573092239</v>
+        <v>2074505.4833767149</v>
       </c>
       <c r="I4" s="7">
-        <v>251904.90625</v>
+        <v>252179.71875</v>
       </c>
       <c r="J4" s="7">
-        <v>468543.125</v>
+        <v>467037.0625</v>
       </c>
       <c r="K4" s="7">
-        <v>1000309.25</v>
+        <v>1006662.8125</v>
       </c>
       <c r="L4" s="7">
-        <v>2618299.75</v>
+        <v>2653803.75</v>
       </c>
       <c r="M4" s="8">
-        <v>4101364.75</v>
+        <v>4102169.25</v>
       </c>
     </row>
     <row r="7">
@@ -2246,40 +2246,40 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>1520282.7252662426</v>
+        <v>1527225.5785855504</v>
       </c>
       <c r="C4" s="7">
         <v>250000</v>
       </c>
       <c r="D4" s="7">
-        <v>251904.90625</v>
+        <v>252179.71875</v>
       </c>
       <c r="E4" s="7">
         <v>2203803.75</v>
       </c>
       <c r="F4" s="7">
-        <v>2455708.75</v>
+        <v>2455983.5</v>
       </c>
       <c r="G4" s="8">
-        <v>2556470.5</v>
+        <v>2556855.5</v>
       </c>
       <c r="H4" s="7">
-        <v>1517829.7767320566</v>
+        <v>1525197.7617169488</v>
       </c>
       <c r="I4" s="7">
         <v>250000</v>
       </c>
       <c r="J4" s="7">
-        <v>251904.90625</v>
+        <v>252179.71875</v>
       </c>
       <c r="K4" s="7">
         <v>2203803.75</v>
       </c>
       <c r="L4" s="7">
-        <v>2455708.75</v>
+        <v>2455983.5</v>
       </c>
       <c r="M4" s="8">
-        <v>2556470.5</v>
+        <v>2556855.5</v>
       </c>
       <c r="N4" s="1">
         <v>2556470.5</v>
@@ -2383,13 +2383,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>6821405.5753792245</v>
+        <v>9813130.2602175437</v>
       </c>
       <c r="C4" s="7">
-        <v>120914.3515625</v>
+        <v>121046.265625</v>
       </c>
       <c r="D4" s="7">
-        <v>201523.921875</v>
+        <v>201743.78125</v>
       </c>
       <c r="E4" s="7">
         <v>300000</v>
@@ -2398,16 +2398,16 @@
         <v>500000</v>
       </c>
       <c r="G4" s="8">
-        <v>930202.1875</v>
+        <v>942000</v>
       </c>
       <c r="H4" s="7">
-        <v>6782799.1977904821</v>
+        <v>9747674.9574410859</v>
       </c>
       <c r="I4" s="7">
-        <v>120914.3515625</v>
+        <v>120932.375</v>
       </c>
       <c r="J4" s="7">
-        <v>201523.921875</v>
+        <v>201743.78125</v>
       </c>
       <c r="K4" s="7">
         <v>300000</v>
@@ -2416,7 +2416,7 @@
         <v>500000</v>
       </c>
       <c r="M4" s="8">
-        <v>930202.5625</v>
+        <v>944749.9375</v>
       </c>
       <c r="N4" s="1">
         <v>834001</v>
@@ -2520,40 +2520,40 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>906798.14155800745</v>
+        <v>873729.6433604639</v>
       </c>
       <c r="C4" s="7">
-        <v>55419.078125</v>
+        <v>50435.9453125</v>
       </c>
       <c r="D4" s="7">
-        <v>200000</v>
+        <v>191656.59375</v>
       </c>
       <c r="E4" s="7">
-        <v>321051.34375</v>
+        <v>302615.65625</v>
       </c>
       <c r="F4" s="7">
-        <v>906857.6875</v>
+        <v>860816.1875</v>
       </c>
       <c r="G4" s="8">
-        <v>2015239.25</v>
+        <v>2000000</v>
       </c>
       <c r="H4" s="7">
-        <v>1034146.9053917929</v>
+        <v>972859.7013830659</v>
       </c>
       <c r="I4" s="7">
-        <v>55419.078125</v>
+        <v>55479.5390625</v>
       </c>
       <c r="J4" s="7">
-        <v>200000</v>
+        <v>196700.1875</v>
       </c>
       <c r="K4" s="7">
-        <v>332514.46875</v>
+        <v>310968.96875</v>
       </c>
       <c r="L4" s="7">
-        <v>978442.25</v>
+        <v>870713.125</v>
       </c>
       <c r="M4" s="8">
-        <v>2015239.25</v>
+        <v>2017437.75</v>
       </c>
       <c r="N4" s="1">
         <v>2015239.25</v>

</xml_diff>

<commit_message>
Arreglos en la parte main
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -1,14 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb563583\GitHub\VEN\data_management\management\4. income imputation\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09DCB80-4004-41E3-AD9F-FD7DFE04CABF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="91">
   <si>
     <t>2019</t>
   </si>
@@ -303,7 +297,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -565,14 +559,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -872,7 +858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView showGridLines="false" tabSelected="true" workbookViewId="0">
@@ -904,10 +890,10 @@
       <c r="A4" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4" s="5">
         <v>186</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4" s="5">
         <v>1.4365152919369786</v>
       </c>
     </row>
@@ -915,10 +901,10 @@
       <c r="A5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5" s="5">
         <v>356</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5" s="5">
         <v>2.7494593759654</v>
       </c>
     </row>
@@ -926,10 +912,10 @@
       <c r="A6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6" s="5">
         <v>1671</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6" s="5">
         <v>12.905468025949954</v>
       </c>
     </row>
@@ -937,10 +923,10 @@
       <c r="A7" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="0">
-        <v>0</v>
-      </c>
-      <c r="C7" s="0">
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -948,10 +934,10 @@
       <c r="A8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8" s="5">
         <v>2027</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8" s="5">
         <v>15.654927401915353</v>
       </c>
     </row>
@@ -959,10 +945,10 @@
       <c r="A9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9" s="5">
         <v>10658</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9" s="5">
         <v>82.313870868087733</v>
       </c>
     </row>
@@ -970,10 +956,10 @@
       <c r="A10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10" s="5">
         <v>12948</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10" s="5">
         <v>100</v>
       </c>
     </row>
@@ -986,10 +972,10 @@
       <c r="A15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15" s="5">
         <v>23404</v>
       </c>
-      <c r="C15" s="0">
+      <c r="C15" s="5">
         <v>374.16466826538766</v>
       </c>
     </row>
@@ -997,10 +983,10 @@
       <c r="A16" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16" s="5">
         <v>7</v>
       </c>
-      <c r="C16" s="0">
+      <c r="C16" s="5">
         <v>0.11191047162270183</v>
       </c>
     </row>
@@ -1008,10 +994,10 @@
       <c r="A17" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17" s="5">
         <v>18</v>
       </c>
-      <c r="C17" s="0">
+      <c r="C17" s="5">
         <v>0.28776978417266186</v>
       </c>
     </row>
@@ -1019,10 +1005,10 @@
       <c r="A18" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="0">
-        <v>0</v>
-      </c>
-      <c r="C18" s="0">
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1030,10 +1016,10 @@
       <c r="A19" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19" s="5">
         <v>25</v>
       </c>
-      <c r="C19" s="0">
+      <c r="C19" s="5">
         <v>0.3996802557953637</v>
       </c>
     </row>
@@ -1041,10 +1027,10 @@
       <c r="A20" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20" s="5">
         <v>6160</v>
       </c>
-      <c r="C20" s="0">
+      <c r="C20" s="5">
         <v>98.481215027977626</v>
       </c>
     </row>
@@ -1052,10 +1038,10 @@
       <c r="A21" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21" s="5">
         <v>6255</v>
       </c>
-      <c r="C21" s="0">
+      <c r="C21" s="5">
         <v>100</v>
       </c>
     </row>
@@ -1068,10 +1054,10 @@
       <c r="A26" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="0">
+      <c r="B26" s="5">
         <v>15</v>
       </c>
-      <c r="C26" s="0">
+      <c r="C26" s="5">
         <v>1.6816143497757847</v>
       </c>
     </row>
@@ -1079,10 +1065,10 @@
       <c r="A27" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="0">
+      <c r="B27" s="5">
         <v>20</v>
       </c>
-      <c r="C27" s="0">
+      <c r="C27" s="5">
         <v>2.2421524663677128</v>
       </c>
     </row>
@@ -1090,10 +1076,10 @@
       <c r="A28" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="0">
+      <c r="B28" s="5">
         <v>2</v>
       </c>
-      <c r="C28" s="0">
+      <c r="C28" s="5">
         <v>0.22421524663677131</v>
       </c>
     </row>
@@ -1101,10 +1087,10 @@
       <c r="A29" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="0">
+      <c r="B29" s="5">
         <v>22</v>
       </c>
-      <c r="C29" s="0">
+      <c r="C29" s="5">
         <v>2.4663677130044843</v>
       </c>
     </row>
@@ -1112,10 +1098,10 @@
       <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="0">
+      <c r="B30" s="5">
         <v>855</v>
       </c>
-      <c r="C30" s="0">
+      <c r="C30" s="5">
         <v>95.852017937219742</v>
       </c>
     </row>
@@ -1123,10 +1109,10 @@
       <c r="A31" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="0">
+      <c r="B31" s="5">
         <v>892</v>
       </c>
-      <c r="C31" s="0">
+      <c r="C31" s="5">
         <v>100</v>
       </c>
     </row>
@@ -1139,10 +1125,10 @@
       <c r="A36" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="0">
+      <c r="B36" s="5">
         <v>25088</v>
       </c>
-      <c r="C36" s="0">
+      <c r="C36" s="5">
         <v>314.26781911562068</v>
       </c>
     </row>
@@ -1150,10 +1136,10 @@
       <c r="A37" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="0">
+      <c r="B37" s="5">
         <v>57</v>
       </c>
-      <c r="C37" s="0">
+      <c r="C37" s="5">
         <v>0.71401728673431042</v>
       </c>
     </row>
@@ -1161,17 +1147,17 @@
       <c r="A38" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="0">
+      <c r="B39" s="5">
         <v>57</v>
       </c>
-      <c r="C39" s="0">
+      <c r="C39" s="5">
         <v>0.71401728673431042</v>
       </c>
     </row>
@@ -1179,10 +1165,10 @@
       <c r="A40" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="0">
+      <c r="B40" s="5">
         <v>7919</v>
       </c>
-      <c r="C40" s="0">
+      <c r="C40" s="5">
         <v>99.19829637980709</v>
       </c>
     </row>
@@ -1190,10 +1176,10 @@
       <c r="A41" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="0">
+      <c r="B41" s="5">
         <v>7983</v>
       </c>
-      <c r="C41" s="0">
+      <c r="C41" s="5">
         <v>100</v>
       </c>
     </row>
@@ -1208,7 +1194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showGridLines="false" workbookViewId="0">
@@ -1232,42 +1218,42 @@
     </row>
     <row r="2" s="11" customFormat="true" ht="15.5">
       <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>8</v>
-      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="12">
+        <v>31.277750370004931</v>
+      </c>
+      <c r="C3" s="12">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" s="13" customFormat="true" ht="12">
       <c r="B4" s="14">
-        <v>31.551634665282823</v>
+        <v>68.722249629995076</v>
       </c>
       <c r="C4" s="14">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5">
-        <v>68.448365334717181</v>
-      </c>
-      <c r="C5" s="5">
-        <v>52</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="5">
+        <v>0.34533793783917122</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7">
@@ -1275,7 +1261,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="5">
-        <v>0.36325895173845357</v>
+        <v>12.530833744449927</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -1287,7 +1273,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="5">
-        <v>12.454592631032693</v>
+        <v>22.792303897385299</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -1299,10 +1285,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="5">
-        <v>22.625843279709393</v>
+        <v>23.038973852984707</v>
       </c>
       <c r="C9" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -1311,10 +1297,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="5">
-        <v>23.196678775298391</v>
+        <v>19.980266403552047</v>
       </c>
       <c r="C10" s="5">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D10" s="5"/>
     </row>
@@ -1323,10 +1309,10 @@
         <v>18</v>
       </c>
       <c r="B11" s="5">
-        <v>19.615983393876494</v>
+        <v>14.50419338924519</v>
       </c>
       <c r="C11" s="5">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -1335,10 +1321,10 @@
         <v>19</v>
       </c>
       <c r="B12" s="5">
-        <v>14.737934613388687</v>
+        <v>6.8080907745436612</v>
       </c>
       <c r="C12" s="5">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -1346,20 +1332,20 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="5">
-        <v>7.0057083549558907</v>
-      </c>
-      <c r="C13" s="5">
-        <v>44</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="5">
+        <v>24.124321657622101</v>
+      </c>
+      <c r="C14" s="5">
+        <v>36</v>
+      </c>
       <c r="D14" s="5"/>
     </row>
     <row r="15">
@@ -1367,10 +1353,10 @@
         <v>22</v>
       </c>
       <c r="B15" s="5">
-        <v>23.456149455111571</v>
+        <v>32.807104094721261</v>
       </c>
       <c r="C15" s="5">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -1379,10 +1365,10 @@
         <v>59</v>
       </c>
       <c r="B16" s="5">
-        <v>33.004670472236633</v>
+        <v>29.551060680809076</v>
       </c>
       <c r="C16" s="5">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -1391,10 +1377,10 @@
         <v>54</v>
       </c>
       <c r="B17" s="5">
-        <v>29.9429164504411</v>
+        <v>10.853478046373951</v>
       </c>
       <c r="C17" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D17" s="5"/>
     </row>
@@ -1403,10 +1389,10 @@
         <v>58</v>
       </c>
       <c r="B18" s="5">
-        <v>10.949662688116243</v>
+        <v>2.5160335471139614</v>
       </c>
       <c r="C18" s="5">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5"/>
     </row>
@@ -1415,10 +1401,10 @@
         <v>55</v>
       </c>
       <c r="B19" s="5">
-        <v>2.4909185262065385</v>
+        <v>0.1480019733596448</v>
       </c>
       <c r="C19" s="5">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D19" s="5"/>
     </row>
@@ -1426,20 +1412,20 @@
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="5">
-        <v>0.15568240788790866</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="5">
+        <v>0.34533793783917122</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22">
@@ -1447,7 +1433,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="5">
-        <v>0.36325895173845357</v>
+        <v>0.1480019733596448</v>
       </c>
       <c r="C22" s="5">
         <v>0</v>
@@ -1459,10 +1445,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="17">
-        <v>0.15568240788790866</v>
+        <v>26.985693142575233</v>
       </c>
       <c r="C23" s="17">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D23" s="17"/>
     </row>
@@ -1471,10 +1457,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="5">
-        <v>26.777374156720292</v>
+        <v>48.001973359644794</v>
       </c>
       <c r="C24" s="5">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="D24" s="5"/>
     </row>
@@ -1483,10 +1469,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="5">
-        <v>48.209652309289055</v>
+        <v>5.1307350764676869</v>
       </c>
       <c r="C25" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D25" s="5"/>
     </row>
@@ -1495,10 +1481,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="5">
-        <v>5.1894135962636225</v>
+        <v>14.208189442525901</v>
       </c>
       <c r="C26" s="5">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D26" s="5"/>
     </row>
@@ -1507,10 +1493,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="5">
-        <v>14.011416709911781</v>
+        <v>0.39467192895905284</v>
       </c>
       <c r="C27" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D27" s="5"/>
     </row>
@@ -1519,10 +1505,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="5">
-        <v>0.31136481577581732</v>
+        <v>4.7853971386285155</v>
       </c>
       <c r="C28" s="5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D28" s="5"/>
     </row>
@@ -1530,20 +1516,20 @@
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="5">
-        <v>4.9818370524130771</v>
-      </c>
-      <c r="C29" s="5">
-        <v>12</v>
-      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="5">
+        <v>4.3413912185495809</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
       <c r="D30" s="5"/>
     </row>
     <row r="31">
@@ -1551,7 +1537,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="5">
-        <v>4.4628956927867147</v>
+        <v>4.1440552540700546</v>
       </c>
       <c r="C31" s="5">
         <v>0</v>
@@ -1563,10 +1549,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="5">
-        <v>4.3072132848988067</v>
+        <v>11.001480019733597</v>
       </c>
       <c r="C32" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D32" s="5"/>
     </row>
@@ -1575,7 +1561,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="5">
-        <v>11.572392319667877</v>
+        <v>73.162308830784411</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
@@ -1587,10 +1573,10 @@
         <v>39</v>
       </c>
       <c r="B34" s="5">
-        <v>72.288531395952262</v>
+        <v>0.39467192895905284</v>
       </c>
       <c r="C34" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D34" s="5"/>
     </row>
@@ -1599,7 +1585,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5">
-        <v>0.36325895173845357</v>
+        <v>4.0453872718302915</v>
       </c>
       <c r="C35" s="5">
         <v>0</v>
@@ -1611,7 +1597,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="5">
-        <v>4.0477426050856256</v>
+        <v>2.7133695115934877</v>
       </c>
       <c r="C36" s="5">
         <v>0</v>
@@ -1623,10 +1609,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="5">
-        <v>2.7503892060197197</v>
+        <v>0.19733596447952642</v>
       </c>
       <c r="C37" s="5">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="D37" s="5"/>
     </row>
@@ -1634,20 +1620,20 @@
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="5">
-        <v>0.20757654385054489</v>
-      </c>
-      <c r="C38" s="5">
-        <v>92</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="B39" s="5">
+        <v>18.697582634435125</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
       <c r="D39" s="5"/>
     </row>
     <row r="40">
@@ -1655,7 +1641,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="5">
-        <v>18.266735858847948</v>
+        <v>0.64134188455846086</v>
       </c>
       <c r="C40" s="5">
         <v>0</v>
@@ -1667,10 +1653,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="17">
-        <v>0.67462376751427089</v>
+        <v>1.6773556980759743</v>
       </c>
       <c r="C41" s="17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D41" s="17"/>
     </row>
@@ -1679,10 +1665,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="5">
-        <v>1.7644006227296314</v>
+        <v>1.1840157868771584</v>
       </c>
       <c r="C42" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="18"/>
@@ -1692,7 +1678,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="5">
-        <v>1.2454592631032693</v>
+        <v>5.920078934385792</v>
       </c>
       <c r="C43" s="5">
         <v>0</v>
@@ -1704,7 +1690,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="5">
-        <v>6.123508043591074</v>
+        <v>20.720276270350272</v>
       </c>
       <c r="C44" s="5">
         <v>0</v>
@@ -1716,7 +1702,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="5">
-        <v>20.550077841203944</v>
+        <v>12.530833744449927</v>
       </c>
       <c r="C45" s="5">
         <v>0</v>
@@ -1728,7 +1714,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="5">
-        <v>12.817851582771148</v>
+        <v>2.8120374938332513</v>
       </c>
       <c r="C46" s="5">
         <v>0</v>
@@ -1740,7 +1726,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="5">
-        <v>2.9060716139076286</v>
+        <v>5.8214109521460289</v>
       </c>
       <c r="C47" s="5">
         <v>0</v>
@@ -1752,10 +1738,10 @@
         <v>48</v>
       </c>
       <c r="B48" s="5">
-        <v>6.0716139076284374</v>
+        <v>29.797730636408488</v>
       </c>
       <c r="C48" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D48" s="5"/>
     </row>
@@ -1764,10 +1750,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="5">
-        <v>29.372080954852102</v>
+        <v>0.19733596447952642</v>
       </c>
       <c r="C49" s="5">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="D49" s="5"/>
     </row>
@@ -1775,20 +1761,20 @@
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="5">
-        <v>0.20757654385054489</v>
-      </c>
-      <c r="C50" s="5">
-        <v>92</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
+      <c r="B51" s="5">
+        <v>18.894918598914654</v>
+      </c>
+      <c r="C51" s="5">
+        <v>16</v>
+      </c>
       <c r="D51" s="5"/>
     </row>
     <row r="52">
@@ -1796,10 +1782,10 @@
         <v>37</v>
       </c>
       <c r="B52" s="5">
-        <v>19.564089257913857</v>
+        <v>81.105081401085343</v>
       </c>
       <c r="C52" s="5">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D52" s="5"/>
     </row>
@@ -1808,10 +1794,10 @@
         <v>53</v>
       </c>
       <c r="B53" s="17">
-        <v>80.435910742086151</v>
+        <v>0</v>
       </c>
       <c r="C53" s="17">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="D53" s="17"/>
     </row>
@@ -1819,12 +1805,8 @@
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="5">
-        <v>0</v>
-      </c>
-      <c r="C54" s="5">
-        <v>0</v>
-      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
@@ -2028,7 +2010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2108,40 +2090,40 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>2035627.05475047</v>
+        <v>2013340.0766250594</v>
       </c>
       <c r="C4" s="7">
-        <v>252179.71875</v>
+        <v>251904.90625</v>
       </c>
       <c r="D4" s="7">
-        <v>453923.5</v>
+        <v>454765.71875</v>
       </c>
       <c r="E4" s="7">
-        <v>1008718.875</v>
+        <v>1000000</v>
       </c>
       <c r="F4" s="7">
         <v>2653803.75</v>
       </c>
       <c r="G4" s="8">
-        <v>4034875.5</v>
+        <v>4030478.5</v>
       </c>
       <c r="H4" s="7">
-        <v>2074505.4833767149</v>
+        <v>2018915.0637623686</v>
       </c>
       <c r="I4" s="7">
-        <v>252179.71875</v>
+        <v>251904.90625</v>
       </c>
       <c r="J4" s="7">
-        <v>467037.0625</v>
+        <v>473581.21875</v>
       </c>
       <c r="K4" s="7">
-        <v>1006662.8125</v>
+        <v>1000000</v>
       </c>
       <c r="L4" s="7">
-        <v>2653803.75</v>
+        <v>2616927.75</v>
       </c>
       <c r="M4" s="8">
-        <v>4102169.25</v>
+        <v>4042826.25</v>
       </c>
     </row>
     <row r="7">
@@ -2160,7 +2142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2246,40 +2228,40 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>1527225.5785855504</v>
+        <v>1519927.2796204803</v>
       </c>
       <c r="C4" s="7">
         <v>250000</v>
       </c>
       <c r="D4" s="7">
-        <v>252179.71875</v>
+        <v>251904.90625</v>
       </c>
       <c r="E4" s="7">
         <v>2203803.75</v>
       </c>
       <c r="F4" s="7">
-        <v>2455983.5</v>
+        <v>2455708.75</v>
       </c>
       <c r="G4" s="8">
-        <v>2556855.5</v>
+        <v>2556470.5</v>
       </c>
       <c r="H4" s="7">
-        <v>1525197.7617169488</v>
+        <v>1519518.541647075</v>
       </c>
       <c r="I4" s="7">
         <v>250000</v>
       </c>
       <c r="J4" s="7">
-        <v>252179.71875</v>
+        <v>251904.90625</v>
       </c>
       <c r="K4" s="7">
         <v>2203803.75</v>
       </c>
       <c r="L4" s="7">
-        <v>2455983.5</v>
+        <v>2455708.75</v>
       </c>
       <c r="M4" s="8">
-        <v>2556855.5</v>
+        <v>2556470.5</v>
       </c>
       <c r="N4" s="1">
         <v>2556470.5</v>
@@ -2303,7 +2285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2383,13 +2365,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>9813130.2602175437</v>
+        <v>9458464.3975915201</v>
       </c>
       <c r="C4" s="7">
-        <v>121046.265625</v>
+        <v>120914.3515625</v>
       </c>
       <c r="D4" s="7">
-        <v>201743.78125</v>
+        <v>201523.921875</v>
       </c>
       <c r="E4" s="7">
         <v>300000</v>
@@ -2398,16 +2380,16 @@
         <v>500000</v>
       </c>
       <c r="G4" s="8">
-        <v>942000</v>
+        <v>927010</v>
       </c>
       <c r="H4" s="7">
-        <v>9747674.9574410859</v>
+        <v>9394301.2418644987</v>
       </c>
       <c r="I4" s="7">
-        <v>120932.375</v>
+        <v>120581.8125</v>
       </c>
       <c r="J4" s="7">
-        <v>201743.78125</v>
+        <v>201523.921875</v>
       </c>
       <c r="K4" s="7">
         <v>300000</v>
@@ -2416,7 +2398,7 @@
         <v>500000</v>
       </c>
       <c r="M4" s="8">
-        <v>944749.9375</v>
+        <v>930000</v>
       </c>
       <c r="N4" s="1">
         <v>834001</v>
@@ -2440,7 +2422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2520,40 +2502,40 @@
         <v>0</v>
       </c>
       <c r="B4" s="7">
-        <v>873729.6433604639</v>
+        <v>868703.25247404724</v>
       </c>
       <c r="C4" s="7">
-        <v>50435.9453125</v>
+        <v>55419.078125</v>
       </c>
       <c r="D4" s="7">
-        <v>191656.59375</v>
+        <v>188103.75</v>
       </c>
       <c r="E4" s="7">
-        <v>302615.65625</v>
+        <v>302285.875</v>
       </c>
       <c r="F4" s="7">
-        <v>860816.1875</v>
+        <v>860511.875</v>
       </c>
       <c r="G4" s="8">
         <v>2000000</v>
       </c>
       <c r="H4" s="7">
-        <v>972859.7013830659</v>
+        <v>874224.21238739789</v>
       </c>
       <c r="I4" s="7">
-        <v>55479.5390625</v>
+        <v>55419.078125</v>
       </c>
       <c r="J4" s="7">
-        <v>196700.1875</v>
+        <v>188103.75</v>
       </c>
       <c r="K4" s="7">
-        <v>310968.96875</v>
+        <v>310067.53125</v>
       </c>
       <c r="L4" s="7">
-        <v>870713.125</v>
+        <v>866552.875</v>
       </c>
       <c r="M4" s="8">
-        <v>2017437.75</v>
+        <v>2000000</v>
       </c>
       <c r="N4" s="1">
         <v>2015239.25</v>

</xml_diff>

<commit_message>
MAIN RUNING DE PUNTA A PUNTA
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -890,43 +890,43 @@
       <c r="A4" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="0">
         <v>186</v>
       </c>
-      <c r="C4" s="5">
-        <v>1.4365152919369786</v>
+      <c r="C4" s="0">
+        <v>1.4347423634680654</v>
       </c>
     </row>
     <row r="5" ht="29">
       <c r="A5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="0">
         <v>356</v>
       </c>
-      <c r="C5" s="5">
-        <v>2.7494593759654</v>
+      <c r="C5" s="0">
+        <v>2.7460660290033938</v>
       </c>
     </row>
     <row r="6" ht="29">
       <c r="A6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="5">
-        <v>1671</v>
-      </c>
-      <c r="C6" s="5">
-        <v>12.905468025949954</v>
+      <c r="B6" s="0">
+        <v>1675</v>
+      </c>
+      <c r="C6" s="0">
+        <v>12.920394939833384</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="0">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0">
         <v>0</v>
       </c>
     </row>
@@ -934,32 +934,32 @@
       <c r="A8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="5">
-        <v>2027</v>
-      </c>
-      <c r="C8" s="5">
-        <v>15.654927401915353</v>
+      <c r="B8" s="0">
+        <v>2031</v>
+      </c>
+      <c r="C8" s="0">
+        <v>15.666460968836779</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="5">
-        <v>10658</v>
-      </c>
-      <c r="C9" s="5">
-        <v>82.313870868087733</v>
+      <c r="B9" s="0">
+        <v>10670</v>
+      </c>
+      <c r="C9" s="0">
+        <v>82.304844183893849</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="5">
-        <v>12948</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="0">
+        <v>12964</v>
+      </c>
+      <c r="C10" s="0">
         <v>100</v>
       </c>
     </row>
@@ -972,43 +972,43 @@
       <c r="A15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="5">
-        <v>23404</v>
-      </c>
-      <c r="C15" s="5">
-        <v>374.16466826538766</v>
+      <c r="B15" s="0">
+        <v>23442</v>
+      </c>
+      <c r="C15" s="0">
+        <v>374.59252157238734</v>
       </c>
     </row>
     <row r="16" ht="29">
       <c r="A16" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="0">
         <v>7</v>
       </c>
-      <c r="C16" s="5">
-        <v>0.11191047162270183</v>
+      <c r="C16" s="0">
+        <v>0.11185682326621924</v>
       </c>
     </row>
     <row r="17" ht="29">
       <c r="A17" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="0">
         <v>18</v>
       </c>
-      <c r="C17" s="5">
-        <v>0.28776978417266186</v>
+      <c r="C17" s="0">
+        <v>0.28763183125599234</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B18" s="0">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1016,32 +1016,32 @@
       <c r="A19" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="0">
         <v>25</v>
       </c>
-      <c r="C19" s="5">
-        <v>0.3996802557953637</v>
+      <c r="C19" s="0">
+        <v>0.39948865452221155</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="5">
-        <v>6160</v>
-      </c>
-      <c r="C20" s="5">
-        <v>98.481215027977626</v>
+      <c r="B20" s="0">
+        <v>6163</v>
+      </c>
+      <c r="C20" s="0">
+        <v>98.4819431128156</v>
       </c>
     </row>
     <row r="21" ht="29">
       <c r="A21" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="5">
-        <v>6255</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B21" s="0">
+        <v>6258</v>
+      </c>
+      <c r="C21" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1054,10 +1054,10 @@
       <c r="A26" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="0">
         <v>15</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="0">
         <v>1.6816143497757847</v>
       </c>
     </row>
@@ -1065,10 +1065,10 @@
       <c r="A27" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="0">
         <v>20</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="0">
         <v>2.2421524663677128</v>
       </c>
     </row>
@@ -1076,10 +1076,10 @@
       <c r="A28" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="0">
         <v>2</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="0">
         <v>0.22421524663677131</v>
       </c>
     </row>
@@ -1087,10 +1087,10 @@
       <c r="A29" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="0">
         <v>22</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="0">
         <v>2.4663677130044843</v>
       </c>
     </row>
@@ -1098,10 +1098,10 @@
       <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="0">
         <v>855</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="0">
         <v>95.852017937219742</v>
       </c>
     </row>
@@ -1109,10 +1109,10 @@
       <c r="A31" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="0">
         <v>892</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1125,61 +1125,61 @@
       <c r="A36" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="5">
-        <v>25088</v>
-      </c>
-      <c r="C36" s="5">
-        <v>314.26781911562068</v>
+      <c r="B36" s="0">
+        <v>25113</v>
+      </c>
+      <c r="C36" s="0">
+        <v>313.95174396799604</v>
       </c>
     </row>
     <row r="37" ht="29">
       <c r="A37" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="0">
         <v>57</v>
       </c>
-      <c r="C37" s="5">
-        <v>0.71401728673431042</v>
+      <c r="C37" s="0">
+        <v>0.71258907363420432</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
     </row>
     <row r="39">
       <c r="A39" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="0">
         <v>57</v>
       </c>
-      <c r="C39" s="5">
-        <v>0.71401728673431042</v>
+      <c r="C39" s="0">
+        <v>0.71258907363420432</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="5">
-        <v>7919</v>
-      </c>
-      <c r="C40" s="5">
-        <v>99.19829637980709</v>
+      <c r="B40" s="0">
+        <v>7935</v>
+      </c>
+      <c r="C40" s="0">
+        <v>99.199899987498441</v>
       </c>
     </row>
     <row r="41" ht="29">
       <c r="A41" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="5">
-        <v>7983</v>
-      </c>
-      <c r="C41" s="5">
+      <c r="B41" s="0">
+        <v>7999</v>
+      </c>
+      <c r="C41" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1218,22 +1218,22 @@
     </row>
     <row r="2" s="11" customFormat="true" ht="15.5">
       <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
     </row>
     <row r="3">
-      <c r="B3" s="12">
-        <v>31.277750370004931</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B3" s="0">
+        <v>31.314623338257014</v>
+      </c>
+      <c r="C3" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="4" s="13" customFormat="true" ht="12">
-      <c r="B4" s="14">
-        <v>68.722249629995076</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="0">
+        <v>68.685376661742978</v>
+      </c>
+      <c r="C4" s="0">
         <v>52</v>
       </c>
     </row>
@@ -1241,17 +1241,17 @@
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5">
-        <v>0.34533793783917122</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="0">
+        <v>0.34465780403741997</v>
+      </c>
+      <c r="C6" s="0">
         <v>0</v>
       </c>
       <c r="D6" s="5"/>
@@ -1260,10 +1260,10 @@
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5">
-        <v>12.530833744449927</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="0">
+        <v>12.506154603643527</v>
+      </c>
+      <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7" s="5"/>
@@ -1272,10 +1272,10 @@
       <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5">
-        <v>22.792303897385299</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="0">
+        <v>22.796651895617924</v>
+      </c>
+      <c r="C8" s="0">
         <v>0</v>
       </c>
       <c r="D8" s="5"/>
@@ -1284,10 +1284,10 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5">
-        <v>23.038973852984707</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="0">
+        <v>23.141309699655345</v>
+      </c>
+      <c r="C9" s="0">
         <v>4</v>
       </c>
       <c r="D9" s="5"/>
@@ -1296,10 +1296,10 @@
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5">
-        <v>19.980266403552047</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="0">
+        <v>19.940915805022154</v>
+      </c>
+      <c r="C10" s="0">
         <v>16</v>
       </c>
       <c r="D10" s="5"/>
@@ -1308,10 +1308,10 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5">
-        <v>14.50419338924519</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="0">
+        <v>14.47562776957164</v>
+      </c>
+      <c r="C11" s="0">
         <v>36</v>
       </c>
       <c r="D11" s="5"/>
@@ -1320,10 +1320,10 @@
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="5">
-        <v>6.8080907745436612</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="0">
+        <v>6.7946824224519951</v>
+      </c>
+      <c r="C12" s="0">
         <v>44</v>
       </c>
       <c r="D12" s="5"/>
@@ -1332,18 +1332,18 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5">
-        <v>24.124321657622101</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="0">
+        <v>24.175283111767602</v>
+      </c>
+      <c r="C14" s="0">
         <v>36</v>
       </c>
       <c r="D14" s="5"/>
@@ -1352,10 +1352,10 @@
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="5">
-        <v>32.807104094721261</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="0">
+        <v>32.791728212703106</v>
+      </c>
+      <c r="C15" s="0">
         <v>20</v>
       </c>
       <c r="D15" s="5"/>
@@ -1364,10 +1364,10 @@
       <c r="A16" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="5">
-        <v>29.551060680809076</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="0">
+        <v>29.542097488921716</v>
+      </c>
+      <c r="C16" s="0">
         <v>8</v>
       </c>
       <c r="D16" s="5"/>
@@ -1376,10 +1376,10 @@
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="5">
-        <v>10.853478046373951</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B17" s="0">
+        <v>10.832102412604629</v>
+      </c>
+      <c r="C17" s="0">
         <v>12</v>
       </c>
       <c r="D17" s="5"/>
@@ -1388,10 +1388,10 @@
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="5">
-        <v>2.5160335471139614</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B18" s="0">
+        <v>2.5110782865583459</v>
+      </c>
+      <c r="C18" s="0">
         <v>24</v>
       </c>
       <c r="D18" s="5"/>
@@ -1400,10 +1400,10 @@
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="5">
-        <v>0.1480019733596448</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B19" s="0">
+        <v>0.14771048744460857</v>
+      </c>
+      <c r="C19" s="0">
         <v>0</v>
       </c>
       <c r="D19" s="5"/>
@@ -1412,18 +1412,18 @@
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="5">
-        <v>0.34533793783917122</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B21" s="0">
+        <v>0.34465780403741997</v>
+      </c>
+      <c r="C21" s="0">
         <v>0</v>
       </c>
       <c r="D21" s="5"/>
@@ -1432,10 +1432,10 @@
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="5">
-        <v>0.1480019733596448</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B22" s="0">
+        <v>0.14771048744460857</v>
+      </c>
+      <c r="C22" s="0">
         <v>0</v>
       </c>
       <c r="D22" s="5"/>
@@ -1444,10 +1444,10 @@
       <c r="A23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="17">
-        <v>26.985693142575233</v>
-      </c>
-      <c r="C23" s="17">
+      <c r="B23" s="0">
+        <v>26.981782373215164</v>
+      </c>
+      <c r="C23" s="0">
         <v>48</v>
       </c>
       <c r="D23" s="17"/>
@@ -1456,10 +1456,10 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5">
-        <v>48.001973359644794</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B24" s="0">
+        <v>48.005908419497786</v>
+      </c>
+      <c r="C24" s="0">
         <v>16</v>
       </c>
       <c r="D24" s="5"/>
@@ -1468,10 +1468,10 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5">
-        <v>5.1307350764676869</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="B25" s="0">
+        <v>5.1206302314130969</v>
+      </c>
+      <c r="C25" s="0">
         <v>4</v>
       </c>
       <c r="D25" s="5"/>
@@ -1480,10 +1480,10 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5">
-        <v>14.208189442525901</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B26" s="0">
+        <v>14.229443623830626</v>
+      </c>
+      <c r="C26" s="0">
         <v>20</v>
       </c>
       <c r="D26" s="5"/>
@@ -1492,10 +1492,10 @@
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="5">
-        <v>0.39467192895905284</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="B27" s="0">
+        <v>0.3938946331856229</v>
+      </c>
+      <c r="C27" s="0">
         <v>0</v>
       </c>
       <c r="D27" s="5"/>
@@ -1504,10 +1504,10 @@
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="5">
-        <v>4.7853971386285155</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="B28" s="0">
+        <v>4.7759724273756774</v>
+      </c>
+      <c r="C28" s="0">
         <v>12</v>
       </c>
       <c r="D28" s="5"/>
@@ -1516,18 +1516,18 @@
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
       <c r="D29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="5">
-        <v>4.3413912185495809</v>
-      </c>
-      <c r="C30" s="5">
+      <c r="B30" s="0">
+        <v>4.3328409650418518</v>
+      </c>
+      <c r="C30" s="0">
         <v>0</v>
       </c>
       <c r="D30" s="5"/>
@@ -1536,10 +1536,10 @@
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="5">
-        <v>4.1440552540700546</v>
-      </c>
-      <c r="C31" s="5">
+      <c r="B31" s="0">
+        <v>4.1358936484490396</v>
+      </c>
+      <c r="C31" s="0">
         <v>0</v>
       </c>
       <c r="D31" s="5"/>
@@ -1548,10 +1548,10 @@
       <c r="A32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="5">
-        <v>11.001480019733597</v>
-      </c>
-      <c r="C32" s="5">
+      <c r="B32" s="0">
+        <v>10.979812900049236</v>
+      </c>
+      <c r="C32" s="0">
         <v>4</v>
       </c>
       <c r="D32" s="5"/>
@@ -1560,10 +1560,10 @@
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="5">
-        <v>73.162308830784411</v>
-      </c>
-      <c r="C33" s="5">
+      <c r="B33" s="0">
+        <v>73.215164943377644</v>
+      </c>
+      <c r="C33" s="0">
         <v>4</v>
       </c>
       <c r="D33" s="5"/>
@@ -1572,10 +1572,10 @@
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="5">
-        <v>0.39467192895905284</v>
-      </c>
-      <c r="C34" s="5">
+      <c r="B34" s="0">
+        <v>0.3938946331856229</v>
+      </c>
+      <c r="C34" s="0">
         <v>0</v>
       </c>
       <c r="D34" s="5"/>
@@ -1584,10 +1584,10 @@
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="5">
-        <v>4.0453872718302915</v>
-      </c>
-      <c r="C35" s="5">
+      <c r="B35" s="0">
+        <v>4.0374199901526335</v>
+      </c>
+      <c r="C35" s="0">
         <v>0</v>
       </c>
       <c r="D35" s="5"/>
@@ -1596,10 +1596,10 @@
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5">
-        <v>2.7133695115934877</v>
-      </c>
-      <c r="C36" s="5">
+      <c r="B36" s="0">
+        <v>2.7080256031511571</v>
+      </c>
+      <c r="C36" s="0">
         <v>0</v>
       </c>
       <c r="D36" s="5"/>
@@ -1608,10 +1608,10 @@
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="5">
-        <v>0.19733596447952642</v>
-      </c>
-      <c r="C37" s="5">
+      <c r="B37" s="0">
+        <v>0.19694731659281145</v>
+      </c>
+      <c r="C37" s="0">
         <v>92</v>
       </c>
       <c r="D37" s="5"/>
@@ -1620,18 +1620,18 @@
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="5">
-        <v>18.697582634435125</v>
-      </c>
-      <c r="C39" s="5">
+      <c r="B39" s="0">
+        <v>18.660758247168882</v>
+      </c>
+      <c r="C39" s="0">
         <v>0</v>
       </c>
       <c r="D39" s="5"/>
@@ -1640,10 +1640,10 @@
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="5">
-        <v>0.64134188455846086</v>
-      </c>
-      <c r="C40" s="5">
+      <c r="B40" s="0">
+        <v>0.64007877892663712</v>
+      </c>
+      <c r="C40" s="0">
         <v>0</v>
       </c>
       <c r="D40" s="5"/>
@@ -1652,10 +1652,10 @@
       <c r="A41" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="17">
-        <v>1.6773556980759743</v>
-      </c>
-      <c r="C41" s="17">
+      <c r="B41" s="0">
+        <v>1.674052191038897</v>
+      </c>
+      <c r="C41" s="0">
         <v>4</v>
       </c>
       <c r="D41" s="17"/>
@@ -1664,10 +1664,10 @@
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="5">
-        <v>1.1840157868771584</v>
-      </c>
-      <c r="C42" s="5">
+      <c r="B42" s="0">
+        <v>1.1816838995568686</v>
+      </c>
+      <c r="C42" s="0">
         <v>0</v>
       </c>
       <c r="D42" s="5"/>
@@ -1677,10 +1677,10 @@
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="5">
-        <v>5.920078934385792</v>
-      </c>
-      <c r="C43" s="5">
+      <c r="B43" s="0">
+        <v>5.9084194977843421</v>
+      </c>
+      <c r="C43" s="0">
         <v>0</v>
       </c>
       <c r="D43" s="5"/>
@@ -1689,10 +1689,10 @@
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="5">
-        <v>20.720276270350272</v>
-      </c>
-      <c r="C44" s="5">
+      <c r="B44" s="0">
+        <v>20.728705071393403</v>
+      </c>
+      <c r="C44" s="0">
         <v>0</v>
       </c>
       <c r="D44" s="5"/>
@@ -1701,10 +1701,10 @@
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="5">
-        <v>12.530833744449927</v>
-      </c>
-      <c r="C45" s="5">
+      <c r="B45" s="0">
+        <v>12.506154603643527</v>
+      </c>
+      <c r="C45" s="0">
         <v>0</v>
       </c>
       <c r="D45" s="5"/>
@@ -1713,10 +1713,10 @@
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="5">
-        <v>2.8120374938332513</v>
-      </c>
-      <c r="C46" s="5">
+      <c r="B46" s="0">
+        <v>2.8064992614475628</v>
+      </c>
+      <c r="C46" s="0">
         <v>0</v>
       </c>
       <c r="D46" s="5"/>
@@ -1725,10 +1725,10 @@
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="5">
-        <v>5.8214109521460289</v>
-      </c>
-      <c r="C47" s="5">
+      <c r="B47" s="0">
+        <v>5.8099458394879369</v>
+      </c>
+      <c r="C47" s="0">
         <v>0</v>
       </c>
       <c r="D47" s="5"/>
@@ -1737,10 +1737,10 @@
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="5">
-        <v>29.797730636408488</v>
-      </c>
-      <c r="C48" s="5">
+      <c r="B48" s="0">
+        <v>29.886755292959133</v>
+      </c>
+      <c r="C48" s="0">
         <v>4</v>
       </c>
       <c r="D48" s="5"/>
@@ -1749,10 +1749,10 @@
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="5">
-        <v>0.19733596447952642</v>
-      </c>
-      <c r="C49" s="5">
+      <c r="B49" s="0">
+        <v>0.19694731659281145</v>
+      </c>
+      <c r="C49" s="0">
         <v>92</v>
       </c>
       <c r="D49" s="5"/>
@@ -1761,18 +1761,18 @@
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="5">
-        <v>18.894918598914654</v>
-      </c>
-      <c r="C51" s="5">
+      <c r="B51" s="0">
+        <v>18.906942392909897</v>
+      </c>
+      <c r="C51" s="0">
         <v>16</v>
       </c>
       <c r="D51" s="5"/>
@@ -1781,10 +1781,10 @@
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="5">
-        <v>81.105081401085343</v>
-      </c>
-      <c r="C52" s="5">
+      <c r="B52" s="0">
+        <v>81.093057607090103</v>
+      </c>
+      <c r="C52" s="0">
         <v>84</v>
       </c>
       <c r="D52" s="5"/>
@@ -1793,10 +1793,10 @@
       <c r="A53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="17">
-        <v>0</v>
-      </c>
-      <c r="C53" s="17">
+      <c r="B53" s="0">
+        <v>0</v>
+      </c>
+      <c r="C53" s="0">
         <v>0</v>
       </c>
       <c r="D53" s="17"/>
@@ -1805,199 +1805,199 @@
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="B54" s="0"/>
+      <c r="C54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
     </row>
     <row r="56">
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
     </row>
     <row r="57">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
     </row>
     <row r="58">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
     </row>
     <row r="59">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
     </row>
     <row r="60">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
+      <c r="B60" s="0"/>
+      <c r="C60" s="0"/>
     </row>
     <row r="61">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="B61" s="0"/>
+      <c r="C61" s="0"/>
     </row>
     <row r="62">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="B62" s="0"/>
+      <c r="C62" s="0"/>
     </row>
     <row r="63">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
     </row>
     <row r="64">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="B64" s="0"/>
+      <c r="C64" s="0"/>
     </row>
     <row r="65">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
     </row>
     <row r="66">
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
     </row>
     <row r="67">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="B67" s="0"/>
+      <c r="C67" s="0"/>
     </row>
     <row r="68">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="B68" s="0"/>
+      <c r="C68" s="0"/>
     </row>
     <row r="69">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="B69" s="0"/>
+      <c r="C69" s="0"/>
     </row>
     <row r="70">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="B70" s="0"/>
+      <c r="C70" s="0"/>
     </row>
     <row r="71">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="B71" s="0"/>
+      <c r="C71" s="0"/>
     </row>
     <row r="72">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="B72" s="0"/>
+      <c r="C72" s="0"/>
     </row>
     <row r="73">
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="B73" s="0"/>
+      <c r="C73" s="0"/>
     </row>
     <row r="74">
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="B74" s="0"/>
+      <c r="C74" s="0"/>
     </row>
     <row r="75">
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="B75" s="0"/>
+      <c r="C75" s="0"/>
     </row>
     <row r="76">
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="B76" s="0"/>
+      <c r="C76" s="0"/>
     </row>
     <row r="77">
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="B77" s="0"/>
+      <c r="C77" s="0"/>
     </row>
     <row r="78">
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="B78" s="0"/>
+      <c r="C78" s="0"/>
     </row>
     <row r="79">
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="B79" s="0"/>
+      <c r="C79" s="0"/>
     </row>
     <row r="80">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="B80" s="0"/>
+      <c r="C80" s="0"/>
     </row>
     <row r="81">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="B81" s="0"/>
+      <c r="C81" s="0"/>
     </row>
     <row r="82">
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
+      <c r="B82" s="0"/>
+      <c r="C82" s="0"/>
     </row>
     <row r="83">
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="B83" s="0"/>
+      <c r="C83" s="0"/>
     </row>
     <row r="84">
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
+      <c r="B84" s="0"/>
+      <c r="C84" s="0"/>
     </row>
     <row r="85">
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
+      <c r="B85" s="0"/>
+      <c r="C85" s="0"/>
     </row>
     <row r="86">
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
+      <c r="B86" s="0"/>
+      <c r="C86" s="0"/>
     </row>
     <row r="87">
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
+      <c r="B87" s="0"/>
+      <c r="C87" s="0"/>
     </row>
     <row r="88">
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
+      <c r="B88" s="0"/>
+      <c r="C88" s="0"/>
     </row>
     <row r="89">
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
+      <c r="B89" s="0"/>
+      <c r="C89" s="0"/>
     </row>
     <row r="90">
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
+      <c r="B90" s="0"/>
+      <c r="C90" s="0"/>
     </row>
     <row r="91">
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="B91" s="0"/>
+      <c r="C91" s="0"/>
     </row>
     <row r="92">
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
+      <c r="B92" s="0"/>
+      <c r="C92" s="0"/>
     </row>
     <row r="93">
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
+      <c r="B93" s="0"/>
+      <c r="C93" s="0"/>
     </row>
     <row r="94">
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="B94" s="0"/>
+      <c r="C94" s="0"/>
     </row>
     <row r="95">
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
+      <c r="B95" s="0"/>
+      <c r="C95" s="0"/>
     </row>
     <row r="96">
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="B96" s="0"/>
+      <c r="C96" s="0"/>
     </row>
     <row r="97">
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
+      <c r="B97" s="0"/>
+      <c r="C97" s="0"/>
     </row>
     <row r="98">
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="B98" s="0"/>
+      <c r="C98" s="0"/>
     </row>
     <row r="99">
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="B99" s="0"/>
+      <c r="C99" s="0"/>
     </row>
     <row r="100">
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="B100" s="0"/>
+      <c r="C100" s="0"/>
     </row>
     <row r="101">
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="B101" s="0"/>
+      <c r="C101" s="0"/>
     </row>
     <row r="102">
       <c r="B102" s="1"/>
@@ -2047,39 +2047,41 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>5</v>
+      <c r="A3" s="0">
+        <v>2012673.0515710998</v>
+      </c>
+      <c r="B3" s="0">
+        <v>251904.90625</v>
+      </c>
+      <c r="C3" s="0">
+        <v>457207.40625</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1000000</v>
+      </c>
+      <c r="E3" s="0">
+        <v>2653803.75</v>
+      </c>
+      <c r="F3" s="0">
+        <v>4025439.875</v>
+      </c>
+      <c r="G3" s="0">
+        <v>2023749.1836360358</v>
+      </c>
+      <c r="H3" s="0">
+        <v>251904.90625</v>
+      </c>
+      <c r="I3" s="0">
+        <v>474420.875</v>
+      </c>
+      <c r="J3" s="0">
+        <v>1007619.5625</v>
+      </c>
+      <c r="K3" s="0">
+        <v>2627037.25</v>
+      </c>
+      <c r="L3" s="0">
+        <v>4042826.25</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2179,39 +2181,41 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>5</v>
+      <c r="A3" s="0">
+        <v>1520036.1149338242</v>
+      </c>
+      <c r="B3" s="0">
+        <v>250000</v>
+      </c>
+      <c r="C3" s="0">
+        <v>251904.90625</v>
+      </c>
+      <c r="D3" s="0">
+        <v>2203803.75</v>
+      </c>
+      <c r="E3" s="0">
+        <v>2455708.75</v>
+      </c>
+      <c r="F3" s="0">
+        <v>2556470.5</v>
+      </c>
+      <c r="G3" s="0">
+        <v>1518346.8019720076</v>
+      </c>
+      <c r="H3" s="0">
+        <v>250000</v>
+      </c>
+      <c r="I3" s="0">
+        <v>251904.90625</v>
+      </c>
+      <c r="J3" s="0">
+        <v>2203803.75</v>
+      </c>
+      <c r="K3" s="0">
+        <v>2455708.75</v>
+      </c>
+      <c r="L3" s="0">
+        <v>2556470.5</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2316,39 +2320,41 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>5</v>
+      <c r="A3" s="0">
+        <v>9440112.9962030239</v>
+      </c>
+      <c r="B3" s="0">
+        <v>120914.3515625</v>
+      </c>
+      <c r="C3" s="0">
+        <v>201523.921875</v>
+      </c>
+      <c r="D3" s="0">
+        <v>300000</v>
+      </c>
+      <c r="E3" s="0">
+        <v>500000</v>
+      </c>
+      <c r="F3" s="0">
+        <v>925000</v>
+      </c>
+      <c r="G3" s="0">
+        <v>9376206.6523581576</v>
+      </c>
+      <c r="H3" s="0">
+        <v>120914.3515625</v>
+      </c>
+      <c r="I3" s="0">
+        <v>201523.921875</v>
+      </c>
+      <c r="J3" s="0">
+        <v>300000</v>
+      </c>
+      <c r="K3" s="0">
+        <v>500000</v>
+      </c>
+      <c r="L3" s="0">
+        <v>927010</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2453,39 +2459,41 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>5</v>
+      <c r="A3" s="0">
+        <v>868703.25247404724</v>
+      </c>
+      <c r="B3" s="0">
+        <v>55419.078125</v>
+      </c>
+      <c r="C3" s="0">
+        <v>188103.75</v>
+      </c>
+      <c r="D3" s="0">
+        <v>302285.875</v>
+      </c>
+      <c r="E3" s="0">
+        <v>860511.875</v>
+      </c>
+      <c r="F3" s="0">
+        <v>2000000</v>
+      </c>
+      <c r="G3" s="0">
+        <v>878768.4105995202</v>
+      </c>
+      <c r="H3" s="0">
+        <v>55419.078125</v>
+      </c>
+      <c r="I3" s="0">
+        <v>188103.75</v>
+      </c>
+      <c r="J3" s="0">
+        <v>310067.53125</v>
+      </c>
+      <c r="K3" s="0">
+        <v>868189.0625</v>
+      </c>
+      <c r="L3" s="0">
+        <v>2000000</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Ultimos cambios y chau
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -2047,41 +2047,41 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="0">
+      <c r="A3" s="1">
         <v>2012673.0515710998</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="1">
         <v>251904.90625</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="1">
         <v>457207.40625</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3" s="1">
         <v>1000000</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3" s="1">
         <v>2653803.75</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3" s="1">
         <v>4025439.875</v>
       </c>
-      <c r="G3" s="0">
-        <v>2007264.9413285896</v>
-      </c>
-      <c r="H3" s="0">
-        <v>251904.90625</v>
-      </c>
-      <c r="I3" s="0">
-        <v>480000</v>
-      </c>
-      <c r="J3" s="0">
-        <v>1007619.5625</v>
-      </c>
-      <c r="K3" s="0">
-        <v>2618299.75</v>
-      </c>
-      <c r="L3" s="0">
-        <v>4030478.5</v>
+      <c r="G3" s="1">
+        <v>2086523.0645192461</v>
+      </c>
+      <c r="H3" s="1">
+        <v>272057.28125</v>
+      </c>
+      <c r="I3" s="1">
+        <v>500000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1051825.375</v>
+      </c>
+      <c r="K3" s="1">
+        <v>2653803.75</v>
+      </c>
+      <c r="L3" s="1">
+        <v>4203804</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2181,40 +2181,40 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="0">
+      <c r="A3" s="1">
         <v>1520036.1149338242</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="1">
         <v>250000</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="1">
         <v>251904.90625</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3" s="1">
         <v>2203803.75</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3" s="1">
         <v>2455708.75</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3" s="1">
         <v>2556470.5</v>
       </c>
-      <c r="G3" s="0">
-        <v>1518878.9943882769</v>
-      </c>
-      <c r="H3" s="0">
+      <c r="G3" s="1">
+        <v>1517206.8609697653</v>
+      </c>
+      <c r="H3" s="1">
         <v>250000</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3" s="1">
         <v>251904.90625</v>
       </c>
-      <c r="J3" s="0">
+      <c r="J3" s="1">
         <v>2203803.75</v>
       </c>
-      <c r="K3" s="0">
+      <c r="K3" s="1">
         <v>2455708.75</v>
       </c>
-      <c r="L3" s="0">
+      <c r="L3" s="1">
         <v>2556470.5</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -2320,40 +2320,40 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="0">
+      <c r="A3" s="1">
         <v>9440112.9962030239</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="1">
         <v>120914.3515625</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="1">
         <v>201523.921875</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3" s="1">
         <v>300000</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3" s="1">
         <v>500000</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3" s="1">
         <v>925000</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3" s="1">
         <v>9376206.6523581576</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3" s="1">
         <v>120914.3515625</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3" s="1">
         <v>201523.921875</v>
       </c>
-      <c r="J3" s="0">
+      <c r="J3" s="1">
         <v>300000</v>
       </c>
-      <c r="K3" s="0">
+      <c r="K3" s="1">
         <v>500000</v>
       </c>
-      <c r="L3" s="0">
+      <c r="L3" s="1">
         <v>927010</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -2459,40 +2459,40 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="0">
+      <c r="A3" s="1">
         <v>868703.25247404724</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3" s="1">
         <v>55419.078125</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="1">
         <v>188103.75</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3" s="1">
         <v>302285.875</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3" s="1">
         <v>860511.875</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3" s="1">
         <v>2000000</v>
       </c>
-      <c r="G3" s="0">
-        <v>916495.06942844694</v>
-      </c>
-      <c r="H3" s="0">
-        <v>60000</v>
-      </c>
-      <c r="I3" s="0">
-        <v>196485.828125</v>
-      </c>
-      <c r="J3" s="0">
-        <v>320000</v>
-      </c>
-      <c r="K3" s="0">
+      <c r="G3" s="1">
+        <v>900469.5648963952</v>
+      </c>
+      <c r="H3" s="1">
+        <v>55419.078125</v>
+      </c>
+      <c r="I3" s="1">
+        <v>188103.75</v>
+      </c>
+      <c r="J3" s="1">
+        <v>308593.96875</v>
+      </c>
+      <c r="K3" s="1">
         <v>860511.875</v>
       </c>
-      <c r="L3" s="0">
+      <c r="L3" s="1">
         <v>2000000</v>
       </c>
       <c r="M3" s="4" t="s">

</xml_diff>

<commit_message>
Arreglando sort y agegroup
Por ahora solo 2 vueltas de imputación
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -890,10 +890,10 @@
       <c r="A4" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4" s="5">
         <v>186</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4" s="5">
         <v>1.4347423634680654</v>
       </c>
     </row>
@@ -901,10 +901,10 @@
       <c r="A5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5" s="5">
         <v>356</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5" s="5">
         <v>2.7460660290033938</v>
       </c>
     </row>
@@ -912,10 +912,10 @@
       <c r="A6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6" s="5">
         <v>1675</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6" s="5">
         <v>12.920394939833384</v>
       </c>
     </row>
@@ -923,10 +923,10 @@
       <c r="A7" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="0">
-        <v>0</v>
-      </c>
-      <c r="C7" s="0">
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -934,10 +934,10 @@
       <c r="A8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8" s="5">
         <v>2031</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8" s="5">
         <v>15.666460968836779</v>
       </c>
     </row>
@@ -945,10 +945,10 @@
       <c r="A9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9" s="5">
         <v>10670</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9" s="5">
         <v>82.304844183893849</v>
       </c>
     </row>
@@ -956,10 +956,10 @@
       <c r="A10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10" s="5">
         <v>12964</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10" s="5">
         <v>100</v>
       </c>
     </row>
@@ -972,10 +972,10 @@
       <c r="A15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15" s="5">
         <v>23442</v>
       </c>
-      <c r="C15" s="0">
+      <c r="C15" s="5">
         <v>374.59252157238734</v>
       </c>
     </row>
@@ -983,10 +983,10 @@
       <c r="A16" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16" s="5">
         <v>7</v>
       </c>
-      <c r="C16" s="0">
+      <c r="C16" s="5">
         <v>0.11185682326621924</v>
       </c>
     </row>
@@ -994,10 +994,10 @@
       <c r="A17" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17" s="5">
         <v>18</v>
       </c>
-      <c r="C17" s="0">
+      <c r="C17" s="5">
         <v>0.28763183125599234</v>
       </c>
     </row>
@@ -1005,10 +1005,10 @@
       <c r="A18" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="0">
-        <v>0</v>
-      </c>
-      <c r="C18" s="0">
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1016,10 +1016,10 @@
       <c r="A19" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19" s="5">
         <v>25</v>
       </c>
-      <c r="C19" s="0">
+      <c r="C19" s="5">
         <v>0.39948865452221155</v>
       </c>
     </row>
@@ -1027,10 +1027,10 @@
       <c r="A20" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20" s="5">
         <v>6163</v>
       </c>
-      <c r="C20" s="0">
+      <c r="C20" s="5">
         <v>98.4819431128156</v>
       </c>
     </row>
@@ -1038,10 +1038,10 @@
       <c r="A21" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21" s="5">
         <v>6258</v>
       </c>
-      <c r="C21" s="0">
+      <c r="C21" s="5">
         <v>100</v>
       </c>
     </row>
@@ -1054,10 +1054,10 @@
       <c r="A26" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="0">
+      <c r="B26" s="5">
         <v>15</v>
       </c>
-      <c r="C26" s="0">
+      <c r="C26" s="5">
         <v>1.6816143497757847</v>
       </c>
     </row>
@@ -1065,10 +1065,10 @@
       <c r="A27" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="0">
+      <c r="B27" s="5">
         <v>20</v>
       </c>
-      <c r="C27" s="0">
+      <c r="C27" s="5">
         <v>2.2421524663677128</v>
       </c>
     </row>
@@ -1076,10 +1076,10 @@
       <c r="A28" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="0">
+      <c r="B28" s="5">
         <v>2</v>
       </c>
-      <c r="C28" s="0">
+      <c r="C28" s="5">
         <v>0.22421524663677131</v>
       </c>
     </row>
@@ -1087,10 +1087,10 @@
       <c r="A29" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="0">
+      <c r="B29" s="5">
         <v>22</v>
       </c>
-      <c r="C29" s="0">
+      <c r="C29" s="5">
         <v>2.4663677130044843</v>
       </c>
     </row>
@@ -1098,10 +1098,10 @@
       <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="0">
+      <c r="B30" s="5">
         <v>855</v>
       </c>
-      <c r="C30" s="0">
+      <c r="C30" s="5">
         <v>95.852017937219742</v>
       </c>
     </row>
@@ -1109,10 +1109,10 @@
       <c r="A31" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="0">
+      <c r="B31" s="5">
         <v>892</v>
       </c>
-      <c r="C31" s="0">
+      <c r="C31" s="5">
         <v>100</v>
       </c>
     </row>
@@ -1125,10 +1125,10 @@
       <c r="A36" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="0">
+      <c r="B36" s="5">
         <v>25113</v>
       </c>
-      <c r="C36" s="0">
+      <c r="C36" s="5">
         <v>313.95174396799604</v>
       </c>
     </row>
@@ -1136,10 +1136,10 @@
       <c r="A37" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="0">
+      <c r="B37" s="5">
         <v>57</v>
       </c>
-      <c r="C37" s="0">
+      <c r="C37" s="5">
         <v>0.71258907363420432</v>
       </c>
     </row>
@@ -1147,17 +1147,17 @@
       <c r="A38" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="0">
+      <c r="B39" s="5">
         <v>57</v>
       </c>
-      <c r="C39" s="0">
+      <c r="C39" s="5">
         <v>0.71258907363420432</v>
       </c>
     </row>
@@ -1165,10 +1165,10 @@
       <c r="A40" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="0">
+      <c r="B40" s="5">
         <v>7935</v>
       </c>
-      <c r="C40" s="0">
+      <c r="C40" s="5">
         <v>99.199899987498441</v>
       </c>
     </row>
@@ -1176,10 +1176,10 @@
       <c r="A41" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="0">
+      <c r="B41" s="5">
         <v>7999</v>
       </c>
-      <c r="C41" s="0">
+      <c r="C41" s="5">
         <v>100</v>
       </c>
     </row>
@@ -1218,22 +1218,22 @@
     </row>
     <row r="2" s="11" customFormat="true" ht="15.5">
       <c r="A2" s="9"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3">
-      <c r="B3" s="0">
+      <c r="B3" s="1">
         <v>31.314623338257014</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="1">
         <v>48</v>
       </c>
     </row>
     <row r="4" s="13" customFormat="true" ht="12">
-      <c r="B4" s="0">
+      <c r="B4" s="1">
         <v>68.685376661742978</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4" s="1">
         <v>52</v>
       </c>
     </row>
@@ -1241,17 +1241,17 @@
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6" s="1">
         <v>0.34465780403741997</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="D6" s="5"/>
@@ -1260,10 +1260,10 @@
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7" s="1">
         <v>12.506154603643527</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" s="5"/>
@@ -1272,10 +1272,10 @@
       <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8" s="1">
         <v>22.796651895617924</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" s="5"/>
@@ -1284,10 +1284,10 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9" s="1">
         <v>23.141309699655345</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9" s="1">
         <v>4</v>
       </c>
       <c r="D9" s="5"/>
@@ -1296,10 +1296,10 @@
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10" s="1">
         <v>19.940915805022154</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10" s="1">
         <v>16</v>
       </c>
       <c r="D10" s="5"/>
@@ -1308,10 +1308,10 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11" s="1">
         <v>14.47562776957164</v>
       </c>
-      <c r="C11" s="0">
+      <c r="C11" s="1">
         <v>36</v>
       </c>
       <c r="D11" s="5"/>
@@ -1320,10 +1320,10 @@
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12" s="1">
         <v>6.7946824224519951</v>
       </c>
-      <c r="C12" s="0">
+      <c r="C12" s="1">
         <v>44</v>
       </c>
       <c r="D12" s="5"/>
@@ -1332,18 +1332,18 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14" s="1">
         <v>24.175283111767602</v>
       </c>
-      <c r="C14" s="0">
+      <c r="C14" s="1">
         <v>36</v>
       </c>
       <c r="D14" s="5"/>
@@ -1352,10 +1352,10 @@
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15" s="1">
         <v>32.791728212703106</v>
       </c>
-      <c r="C15" s="0">
+      <c r="C15" s="1">
         <v>20</v>
       </c>
       <c r="D15" s="5"/>
@@ -1364,10 +1364,10 @@
       <c r="A16" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16" s="1">
         <v>29.542097488921716</v>
       </c>
-      <c r="C16" s="0">
+      <c r="C16" s="1">
         <v>8</v>
       </c>
       <c r="D16" s="5"/>
@@ -1376,10 +1376,10 @@
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17" s="1">
         <v>10.832102412604629</v>
       </c>
-      <c r="C17" s="0">
+      <c r="C17" s="1">
         <v>12</v>
       </c>
       <c r="D17" s="5"/>
@@ -1388,10 +1388,10 @@
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18" s="1">
         <v>2.5110782865583459</v>
       </c>
-      <c r="C18" s="0">
+      <c r="C18" s="1">
         <v>24</v>
       </c>
       <c r="D18" s="5"/>
@@ -1400,10 +1400,10 @@
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19" s="1">
         <v>0.14771048744460857</v>
       </c>
-      <c r="C19" s="0">
+      <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" s="5"/>
@@ -1412,18 +1412,18 @@
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21" s="1">
         <v>0.34465780403741997</v>
       </c>
-      <c r="C21" s="0">
+      <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="5"/>
@@ -1432,10 +1432,10 @@
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22" s="1">
         <v>0.14771048744460857</v>
       </c>
-      <c r="C22" s="0">
+      <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="5"/>
@@ -1444,10 +1444,10 @@
       <c r="A23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23" s="1">
         <v>26.981782373215164</v>
       </c>
-      <c r="C23" s="0">
+      <c r="C23" s="1">
         <v>48</v>
       </c>
       <c r="D23" s="17"/>
@@ -1456,10 +1456,10 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="0">
+      <c r="B24" s="1">
         <v>48.005908419497786</v>
       </c>
-      <c r="C24" s="0">
+      <c r="C24" s="1">
         <v>16</v>
       </c>
       <c r="D24" s="5"/>
@@ -1468,10 +1468,10 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="0">
+      <c r="B25" s="1">
         <v>5.1206302314130969</v>
       </c>
-      <c r="C25" s="0">
+      <c r="C25" s="1">
         <v>4</v>
       </c>
       <c r="D25" s="5"/>
@@ -1480,10 +1480,10 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="0">
+      <c r="B26" s="1">
         <v>14.229443623830626</v>
       </c>
-      <c r="C26" s="0">
+      <c r="C26" s="1">
         <v>20</v>
       </c>
       <c r="D26" s="5"/>
@@ -1492,10 +1492,10 @@
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="0">
+      <c r="B27" s="1">
         <v>0.3938946331856229</v>
       </c>
-      <c r="C27" s="0">
+      <c r="C27" s="1">
         <v>0</v>
       </c>
       <c r="D27" s="5"/>
@@ -1504,10 +1504,10 @@
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="0">
+      <c r="B28" s="1">
         <v>4.7759724273756774</v>
       </c>
-      <c r="C28" s="0">
+      <c r="C28" s="1">
         <v>12</v>
       </c>
       <c r="D28" s="5"/>
@@ -1516,18 +1516,18 @@
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="0">
+      <c r="B30" s="1">
         <v>4.3328409650418518</v>
       </c>
-      <c r="C30" s="0">
+      <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" s="5"/>
@@ -1536,10 +1536,10 @@
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0">
+      <c r="B31" s="1">
         <v>4.1358936484490396</v>
       </c>
-      <c r="C31" s="0">
+      <c r="C31" s="1">
         <v>0</v>
       </c>
       <c r="D31" s="5"/>
@@ -1548,10 +1548,10 @@
       <c r="A32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="0">
+      <c r="B32" s="1">
         <v>10.979812900049236</v>
       </c>
-      <c r="C32" s="0">
+      <c r="C32" s="1">
         <v>4</v>
       </c>
       <c r="D32" s="5"/>
@@ -1560,10 +1560,10 @@
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="0">
+      <c r="B33" s="1">
         <v>73.215164943377644</v>
       </c>
-      <c r="C33" s="0">
+      <c r="C33" s="1">
         <v>4</v>
       </c>
       <c r="D33" s="5"/>
@@ -1572,10 +1572,10 @@
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="0">
+      <c r="B34" s="1">
         <v>0.3938946331856229</v>
       </c>
-      <c r="C34" s="0">
+      <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" s="5"/>
@@ -1584,10 +1584,10 @@
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="0">
+      <c r="B35" s="1">
         <v>4.0374199901526335</v>
       </c>
-      <c r="C35" s="0">
+      <c r="C35" s="1">
         <v>0</v>
       </c>
       <c r="D35" s="5"/>
@@ -1596,10 +1596,10 @@
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="0">
+      <c r="B36" s="1">
         <v>2.7080256031511571</v>
       </c>
-      <c r="C36" s="0">
+      <c r="C36" s="1">
         <v>0</v>
       </c>
       <c r="D36" s="5"/>
@@ -1608,10 +1608,10 @@
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="0">
+      <c r="B37" s="1">
         <v>0.19694731659281145</v>
       </c>
-      <c r="C37" s="0">
+      <c r="C37" s="1">
         <v>92</v>
       </c>
       <c r="D37" s="5"/>
@@ -1620,18 +1620,18 @@
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="0">
+      <c r="B39" s="1">
         <v>18.660758247168882</v>
       </c>
-      <c r="C39" s="0">
+      <c r="C39" s="1">
         <v>0</v>
       </c>
       <c r="D39" s="5"/>
@@ -1640,10 +1640,10 @@
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="0">
+      <c r="B40" s="1">
         <v>0.64007877892663712</v>
       </c>
-      <c r="C40" s="0">
+      <c r="C40" s="1">
         <v>0</v>
       </c>
       <c r="D40" s="5"/>
@@ -1652,10 +1652,10 @@
       <c r="A41" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="0">
+      <c r="B41" s="1">
         <v>1.674052191038897</v>
       </c>
-      <c r="C41" s="0">
+      <c r="C41" s="1">
         <v>4</v>
       </c>
       <c r="D41" s="17"/>
@@ -1664,10 +1664,10 @@
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="0">
+      <c r="B42" s="1">
         <v>1.1816838995568686</v>
       </c>
-      <c r="C42" s="0">
+      <c r="C42" s="1">
         <v>0</v>
       </c>
       <c r="D42" s="5"/>
@@ -1677,10 +1677,10 @@
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="0">
+      <c r="B43" s="1">
         <v>5.9084194977843421</v>
       </c>
-      <c r="C43" s="0">
+      <c r="C43" s="1">
         <v>0</v>
       </c>
       <c r="D43" s="5"/>
@@ -1689,10 +1689,10 @@
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="0">
+      <c r="B44" s="1">
         <v>20.728705071393403</v>
       </c>
-      <c r="C44" s="0">
+      <c r="C44" s="1">
         <v>0</v>
       </c>
       <c r="D44" s="5"/>
@@ -1701,10 +1701,10 @@
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="0">
+      <c r="B45" s="1">
         <v>12.506154603643527</v>
       </c>
-      <c r="C45" s="0">
+      <c r="C45" s="1">
         <v>0</v>
       </c>
       <c r="D45" s="5"/>
@@ -1713,10 +1713,10 @@
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="0">
+      <c r="B46" s="1">
         <v>2.8064992614475628</v>
       </c>
-      <c r="C46" s="0">
+      <c r="C46" s="1">
         <v>0</v>
       </c>
       <c r="D46" s="5"/>
@@ -1725,10 +1725,10 @@
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="0">
+      <c r="B47" s="1">
         <v>5.8099458394879369</v>
       </c>
-      <c r="C47" s="0">
+      <c r="C47" s="1">
         <v>0</v>
       </c>
       <c r="D47" s="5"/>
@@ -1737,10 +1737,10 @@
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="0">
+      <c r="B48" s="1">
         <v>29.886755292959133</v>
       </c>
-      <c r="C48" s="0">
+      <c r="C48" s="1">
         <v>4</v>
       </c>
       <c r="D48" s="5"/>
@@ -1749,10 +1749,10 @@
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="0">
+      <c r="B49" s="1">
         <v>0.19694731659281145</v>
       </c>
-      <c r="C49" s="0">
+      <c r="C49" s="1">
         <v>92</v>
       </c>
       <c r="D49" s="5"/>
@@ -1761,18 +1761,18 @@
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="0">
+      <c r="B51" s="1">
         <v>18.906942392909897</v>
       </c>
-      <c r="C51" s="0">
+      <c r="C51" s="1">
         <v>16</v>
       </c>
       <c r="D51" s="5"/>
@@ -1781,10 +1781,10 @@
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="0">
+      <c r="B52" s="1">
         <v>81.093057607090103</v>
       </c>
-      <c r="C52" s="0">
+      <c r="C52" s="1">
         <v>84</v>
       </c>
       <c r="D52" s="5"/>
@@ -1793,10 +1793,10 @@
       <c r="A53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="0">
-        <v>0</v>
-      </c>
-      <c r="C53" s="0">
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1">
         <v>0</v>
       </c>
       <c r="D53" s="17"/>
@@ -1805,199 +1805,199 @@
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="0"/>
-      <c r="C54" s="0"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="0"/>
-      <c r="C55" s="0"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
     </row>
     <row r="56">
-      <c r="B56" s="0"/>
-      <c r="C56" s="0"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
     </row>
     <row r="57">
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
     </row>
     <row r="58">
-      <c r="B58" s="0"/>
-      <c r="C58" s="0"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
     </row>
     <row r="59">
-      <c r="B59" s="0"/>
-      <c r="C59" s="0"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
     </row>
     <row r="60">
-      <c r="B60" s="0"/>
-      <c r="C60" s="0"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61">
-      <c r="B61" s="0"/>
-      <c r="C61" s="0"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="62">
-      <c r="B62" s="0"/>
-      <c r="C62" s="0"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
     </row>
     <row r="63">
-      <c r="B63" s="0"/>
-      <c r="C63" s="0"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
     </row>
     <row r="64">
-      <c r="B64" s="0"/>
-      <c r="C64" s="0"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
     </row>
     <row r="65">
-      <c r="B65" s="0"/>
-      <c r="C65" s="0"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
     </row>
     <row r="66">
-      <c r="B66" s="0"/>
-      <c r="C66" s="0"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
     </row>
     <row r="67">
-      <c r="B67" s="0"/>
-      <c r="C67" s="0"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
     </row>
     <row r="68">
-      <c r="B68" s="0"/>
-      <c r="C68" s="0"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
     </row>
     <row r="69">
-      <c r="B69" s="0"/>
-      <c r="C69" s="0"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
     </row>
     <row r="70">
-      <c r="B70" s="0"/>
-      <c r="C70" s="0"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
     </row>
     <row r="71">
-      <c r="B71" s="0"/>
-      <c r="C71" s="0"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
     </row>
     <row r="72">
-      <c r="B72" s="0"/>
-      <c r="C72" s="0"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
     </row>
     <row r="73">
-      <c r="B73" s="0"/>
-      <c r="C73" s="0"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
     </row>
     <row r="74">
-      <c r="B74" s="0"/>
-      <c r="C74" s="0"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
     </row>
     <row r="75">
-      <c r="B75" s="0"/>
-      <c r="C75" s="0"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
     </row>
     <row r="76">
-      <c r="B76" s="0"/>
-      <c r="C76" s="0"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
     </row>
     <row r="77">
-      <c r="B77" s="0"/>
-      <c r="C77" s="0"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
     </row>
     <row r="78">
-      <c r="B78" s="0"/>
-      <c r="C78" s="0"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
     </row>
     <row r="79">
-      <c r="B79" s="0"/>
-      <c r="C79" s="0"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
     </row>
     <row r="80">
-      <c r="B80" s="0"/>
-      <c r="C80" s="0"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
     </row>
     <row r="81">
-      <c r="B81" s="0"/>
-      <c r="C81" s="0"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
     </row>
     <row r="82">
-      <c r="B82" s="0"/>
-      <c r="C82" s="0"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
     </row>
     <row r="83">
-      <c r="B83" s="0"/>
-      <c r="C83" s="0"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
     </row>
     <row r="84">
-      <c r="B84" s="0"/>
-      <c r="C84" s="0"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
     </row>
     <row r="85">
-      <c r="B85" s="0"/>
-      <c r="C85" s="0"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
     </row>
     <row r="86">
-      <c r="B86" s="0"/>
-      <c r="C86" s="0"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
     </row>
     <row r="87">
-      <c r="B87" s="0"/>
-      <c r="C87" s="0"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
     </row>
     <row r="88">
-      <c r="B88" s="0"/>
-      <c r="C88" s="0"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
     </row>
     <row r="89">
-      <c r="B89" s="0"/>
-      <c r="C89" s="0"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
     </row>
     <row r="90">
-      <c r="B90" s="0"/>
-      <c r="C90" s="0"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
     </row>
     <row r="91">
-      <c r="B91" s="0"/>
-      <c r="C91" s="0"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
     </row>
     <row r="92">
-      <c r="B92" s="0"/>
-      <c r="C92" s="0"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
     </row>
     <row r="93">
-      <c r="B93" s="0"/>
-      <c r="C93" s="0"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
     </row>
     <row r="94">
-      <c r="B94" s="0"/>
-      <c r="C94" s="0"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
     </row>
     <row r="95">
-      <c r="B95" s="0"/>
-      <c r="C95" s="0"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
     </row>
     <row r="96">
-      <c r="B96" s="0"/>
-      <c r="C96" s="0"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
     </row>
     <row r="97">
-      <c r="B97" s="0"/>
-      <c r="C97" s="0"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
     </row>
     <row r="98">
-      <c r="B98" s="0"/>
-      <c r="C98" s="0"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
     </row>
     <row r="99">
-      <c r="B99" s="0"/>
-      <c r="C99" s="0"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
     </row>
     <row r="100">
-      <c r="B100" s="0"/>
-      <c r="C100" s="0"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
     </row>
     <row r="101">
-      <c r="B101" s="0"/>
-      <c r="C101" s="0"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
     </row>
     <row r="102">
       <c r="B102" s="1"/>
@@ -2066,7 +2066,7 @@
         <v>4025439.875</v>
       </c>
       <c r="G3" s="1">
-        <v>2086523.0645192461</v>
+        <v>2079811.9578104364</v>
       </c>
       <c r="H3" s="1">
         <v>272057.28125</v>
@@ -2075,7 +2075,7 @@
         <v>500000</v>
       </c>
       <c r="J3" s="1">
-        <v>1051825.375</v>
+        <v>1058000.625</v>
       </c>
       <c r="K3" s="1">
         <v>2653803.75</v>
@@ -2200,7 +2200,7 @@
         <v>2556470.5</v>
       </c>
       <c r="G3" s="1">
-        <v>1517206.8609697653</v>
+        <v>1519250.7368358569</v>
       </c>
       <c r="H3" s="1">
         <v>250000</v>
@@ -2339,7 +2339,7 @@
         <v>925000</v>
       </c>
       <c r="G3" s="1">
-        <v>9376206.6523581576</v>
+        <v>9376485.093861917</v>
       </c>
       <c r="H3" s="1">
         <v>120914.3515625</v>
@@ -2354,7 +2354,7 @@
         <v>500000</v>
       </c>
       <c r="L3" s="1">
-        <v>927010</v>
+        <v>925000</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2478,16 +2478,16 @@
         <v>2000000</v>
       </c>
       <c r="G3" s="1">
-        <v>900469.5648963952</v>
+        <v>918953.52843286539</v>
       </c>
       <c r="H3" s="1">
         <v>55419.078125</v>
       </c>
       <c r="I3" s="1">
-        <v>188103.75</v>
+        <v>200000</v>
       </c>
       <c r="J3" s="1">
-        <v>308593.96875</v>
+        <v>312810.71875</v>
       </c>
       <c r="K3" s="1">
         <v>860511.875</v>

</xml_diff>

<commit_message>
Más arreglos y corriendo - A ver si ya se soluciona el temita...
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -890,43 +890,43 @@
       <c r="A4" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="0">
         <v>186</v>
       </c>
-      <c r="C4" s="5">
-        <v>1.4347423634680654</v>
+      <c r="C4" s="0">
+        <v>1.4345210550670986</v>
       </c>
     </row>
     <row r="5" ht="29">
       <c r="A5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="0">
         <v>356</v>
       </c>
-      <c r="C5" s="5">
-        <v>2.7460660290033938</v>
+      <c r="C5" s="0">
+        <v>2.7456424494832641</v>
       </c>
     </row>
     <row r="6" ht="29">
       <c r="A6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="0">
         <v>1675</v>
       </c>
-      <c r="C6" s="5">
-        <v>12.920394939833384</v>
+      <c r="C6" s="0">
+        <v>12.91840197439457</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="0">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0">
         <v>0</v>
       </c>
     </row>
@@ -934,32 +934,32 @@
       <c r="A8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="0">
         <v>2031</v>
       </c>
-      <c r="C8" s="5">
-        <v>15.666460968836779</v>
+      <c r="C8" s="0">
+        <v>15.664044423877835</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="5">
-        <v>10670</v>
-      </c>
-      <c r="C9" s="5">
-        <v>82.304844183893849</v>
+      <c r="B9" s="0">
+        <v>10672</v>
+      </c>
+      <c r="C9" s="0">
+        <v>82.307573654172444</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="5">
-        <v>12964</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="0">
+        <v>12966</v>
+      </c>
+      <c r="C10" s="0">
         <v>100</v>
       </c>
     </row>
@@ -972,21 +972,21 @@
       <c r="A15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="5">
-        <v>23442</v>
-      </c>
-      <c r="C15" s="5">
-        <v>374.59252157238734</v>
+      <c r="B15" s="0">
+        <v>23447</v>
+      </c>
+      <c r="C15" s="0">
+        <v>374.6724193032918</v>
       </c>
     </row>
     <row r="16" ht="29">
       <c r="A16" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="0">
         <v>7</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="0">
         <v>0.11185682326621924</v>
       </c>
     </row>
@@ -994,10 +994,10 @@
       <c r="A17" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="0">
         <v>18</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="0">
         <v>0.28763183125599234</v>
       </c>
     </row>
@@ -1005,10 +1005,10 @@
       <c r="A18" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B18" s="0">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1016,10 +1016,10 @@
       <c r="A19" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="0">
         <v>25</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="0">
         <v>0.39948865452221155</v>
       </c>
     </row>
@@ -1027,10 +1027,10 @@
       <c r="A20" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="0">
         <v>6163</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="0">
         <v>98.4819431128156</v>
       </c>
     </row>
@@ -1038,10 +1038,10 @@
       <c r="A21" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="0">
         <v>6258</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1054,10 +1054,10 @@
       <c r="A26" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="0">
         <v>15</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="0">
         <v>1.6816143497757847</v>
       </c>
     </row>
@@ -1065,10 +1065,10 @@
       <c r="A27" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="0">
         <v>20</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="0">
         <v>2.2421524663677128</v>
       </c>
     </row>
@@ -1076,10 +1076,10 @@
       <c r="A28" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="0">
         <v>2</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="0">
         <v>0.22421524663677131</v>
       </c>
     </row>
@@ -1087,10 +1087,10 @@
       <c r="A29" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="0">
         <v>22</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="0">
         <v>2.4663677130044843</v>
       </c>
     </row>
@@ -1098,10 +1098,10 @@
       <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="0">
         <v>855</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="0">
         <v>95.852017937219742</v>
       </c>
     </row>
@@ -1109,10 +1109,10 @@
       <c r="A31" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="0">
         <v>892</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1125,61 +1125,61 @@
       <c r="A36" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="5">
-        <v>25113</v>
-      </c>
-      <c r="C36" s="5">
-        <v>313.95174396799604</v>
+      <c r="B36" s="0">
+        <v>25117</v>
+      </c>
+      <c r="C36" s="0">
+        <v>313.96250000000003</v>
       </c>
     </row>
     <row r="37" ht="29">
       <c r="A37" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="0">
         <v>57</v>
       </c>
-      <c r="C37" s="5">
-        <v>0.71258907363420432</v>
+      <c r="C37" s="0">
+        <v>0.71250000000000002</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
     </row>
     <row r="39">
       <c r="A39" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="0">
         <v>57</v>
       </c>
-      <c r="C39" s="5">
-        <v>0.71258907363420432</v>
+      <c r="C39" s="0">
+        <v>0.71250000000000002</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="5">
-        <v>7935</v>
-      </c>
-      <c r="C40" s="5">
-        <v>99.199899987498441</v>
+      <c r="B40" s="0">
+        <v>7936</v>
+      </c>
+      <c r="C40" s="0">
+        <v>99.200000000000003</v>
       </c>
     </row>
     <row r="41" ht="29">
       <c r="A41" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="5">
-        <v>7999</v>
-      </c>
-      <c r="C41" s="5">
+      <c r="B41" s="0">
+        <v>8000</v>
+      </c>
+      <c r="C41" s="0">
         <v>100</v>
       </c>
     </row>
@@ -1218,22 +1218,22 @@
     </row>
     <row r="2" s="11" customFormat="true" ht="15.5">
       <c r="A2" s="9"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
     </row>
     <row r="3">
-      <c r="B3" s="1">
+      <c r="B3" s="0">
         <v>31.314623338257014</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="4" s="13" customFormat="true" ht="12">
-      <c r="B4" s="1">
+      <c r="B4" s="0">
         <v>68.685376661742978</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="0">
         <v>52</v>
       </c>
     </row>
@@ -1241,17 +1241,17 @@
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="0">
         <v>0.34465780403741997</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="0">
         <v>0</v>
       </c>
       <c r="D6" s="5"/>
@@ -1260,10 +1260,10 @@
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="0">
         <v>12.506154603643527</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="0">
         <v>0</v>
       </c>
       <c r="D7" s="5"/>
@@ -1272,10 +1272,10 @@
       <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="0">
         <v>22.796651895617924</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="0">
         <v>0</v>
       </c>
       <c r="D8" s="5"/>
@@ -1284,10 +1284,10 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="0">
         <v>23.141309699655345</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="0">
         <v>4</v>
       </c>
       <c r="D9" s="5"/>
@@ -1296,10 +1296,10 @@
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="0">
         <v>19.940915805022154</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="0">
         <v>16</v>
       </c>
       <c r="D10" s="5"/>
@@ -1308,10 +1308,10 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="0">
         <v>14.47562776957164</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="0">
         <v>36</v>
       </c>
       <c r="D11" s="5"/>
@@ -1320,10 +1320,10 @@
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="0">
         <v>6.7946824224519951</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="0">
         <v>44</v>
       </c>
       <c r="D12" s="5"/>
@@ -1332,18 +1332,18 @@
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="0">
         <v>24.175283111767602</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="0">
         <v>36</v>
       </c>
       <c r="D14" s="5"/>
@@ -1352,10 +1352,10 @@
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="0">
         <v>32.791728212703106</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="0">
         <v>20</v>
       </c>
       <c r="D15" s="5"/>
@@ -1364,10 +1364,10 @@
       <c r="A16" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="0">
         <v>29.542097488921716</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="0">
         <v>8</v>
       </c>
       <c r="D16" s="5"/>
@@ -1376,10 +1376,10 @@
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="0">
         <v>10.832102412604629</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="0">
         <v>12</v>
       </c>
       <c r="D17" s="5"/>
@@ -1388,10 +1388,10 @@
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="0">
         <v>2.5110782865583459</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="0">
         <v>24</v>
       </c>
       <c r="D18" s="5"/>
@@ -1400,10 +1400,10 @@
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="0">
         <v>0.14771048744460857</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="0">
         <v>0</v>
       </c>
       <c r="D19" s="5"/>
@@ -1412,18 +1412,18 @@
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="0">
         <v>0.34465780403741997</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="0">
         <v>0</v>
       </c>
       <c r="D21" s="5"/>
@@ -1432,10 +1432,10 @@
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="0">
         <v>0.14771048744460857</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="0">
         <v>0</v>
       </c>
       <c r="D22" s="5"/>
@@ -1444,10 +1444,10 @@
       <c r="A23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="0">
         <v>26.981782373215164</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="0">
         <v>48</v>
       </c>
       <c r="D23" s="17"/>
@@ -1456,10 +1456,10 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="0">
         <v>48.005908419497786</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="0">
         <v>16</v>
       </c>
       <c r="D24" s="5"/>
@@ -1468,10 +1468,10 @@
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="0">
         <v>5.1206302314130969</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="0">
         <v>4</v>
       </c>
       <c r="D25" s="5"/>
@@ -1480,10 +1480,10 @@
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="0">
         <v>14.229443623830626</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="0">
         <v>20</v>
       </c>
       <c r="D26" s="5"/>
@@ -1492,10 +1492,10 @@
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="0">
         <v>0.3938946331856229</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="0">
         <v>0</v>
       </c>
       <c r="D27" s="5"/>
@@ -1504,10 +1504,10 @@
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="0">
         <v>4.7759724273756774</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="0">
         <v>12</v>
       </c>
       <c r="D28" s="5"/>
@@ -1516,18 +1516,18 @@
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
       <c r="D29" s="5"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="0">
         <v>4.3328409650418518</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="0">
         <v>0</v>
       </c>
       <c r="D30" s="5"/>
@@ -1536,10 +1536,10 @@
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="0">
         <v>4.1358936484490396</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="0">
         <v>0</v>
       </c>
       <c r="D31" s="5"/>
@@ -1548,10 +1548,10 @@
       <c r="A32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="0">
         <v>10.979812900049236</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="0">
         <v>4</v>
       </c>
       <c r="D32" s="5"/>
@@ -1560,10 +1560,10 @@
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="0">
         <v>73.215164943377644</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="0">
         <v>4</v>
       </c>
       <c r="D33" s="5"/>
@@ -1572,10 +1572,10 @@
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="0">
         <v>0.3938946331856229</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="0">
         <v>0</v>
       </c>
       <c r="D34" s="5"/>
@@ -1584,10 +1584,10 @@
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="0">
         <v>4.0374199901526335</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="0">
         <v>0</v>
       </c>
       <c r="D35" s="5"/>
@@ -1596,10 +1596,10 @@
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="0">
         <v>2.7080256031511571</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="0">
         <v>0</v>
       </c>
       <c r="D36" s="5"/>
@@ -1608,10 +1608,10 @@
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="0">
         <v>0.19694731659281145</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="0">
         <v>92</v>
       </c>
       <c r="D37" s="5"/>
@@ -1620,18 +1620,18 @@
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="0">
         <v>18.660758247168882</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="0">
         <v>0</v>
       </c>
       <c r="D39" s="5"/>
@@ -1640,10 +1640,10 @@
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="0">
         <v>0.64007877892663712</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="0">
         <v>0</v>
       </c>
       <c r="D40" s="5"/>
@@ -1652,10 +1652,10 @@
       <c r="A41" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="0">
         <v>1.674052191038897</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="0">
         <v>4</v>
       </c>
       <c r="D41" s="17"/>
@@ -1664,10 +1664,10 @@
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="0">
         <v>1.1816838995568686</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="0">
         <v>0</v>
       </c>
       <c r="D42" s="5"/>
@@ -1677,10 +1677,10 @@
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="0">
         <v>5.9084194977843421</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="0">
         <v>0</v>
       </c>
       <c r="D43" s="5"/>
@@ -1689,10 +1689,10 @@
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="0">
         <v>20.728705071393403</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="0">
         <v>0</v>
       </c>
       <c r="D44" s="5"/>
@@ -1701,10 +1701,10 @@
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="0">
         <v>12.506154603643527</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="0">
         <v>0</v>
       </c>
       <c r="D45" s="5"/>
@@ -1713,10 +1713,10 @@
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="0">
         <v>2.8064992614475628</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="0">
         <v>0</v>
       </c>
       <c r="D46" s="5"/>
@@ -1725,10 +1725,10 @@
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="0">
         <v>5.8099458394879369</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="0">
         <v>0</v>
       </c>
       <c r="D47" s="5"/>
@@ -1737,10 +1737,10 @@
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="0">
         <v>29.886755292959133</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="0">
         <v>4</v>
       </c>
       <c r="D48" s="5"/>
@@ -1749,10 +1749,10 @@
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="0">
         <v>0.19694731659281145</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="0">
         <v>92</v>
       </c>
       <c r="D49" s="5"/>
@@ -1761,18 +1761,18 @@
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="0">
         <v>18.906942392909897</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="0">
         <v>16</v>
       </c>
       <c r="D51" s="5"/>
@@ -1781,10 +1781,10 @@
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="0">
         <v>81.093057607090103</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="0">
         <v>84</v>
       </c>
       <c r="D52" s="5"/>
@@ -1793,10 +1793,10 @@
       <c r="A53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="1">
-        <v>0</v>
-      </c>
-      <c r="C53" s="1">
+      <c r="B53" s="0">
+        <v>0</v>
+      </c>
+      <c r="C53" s="0">
         <v>0</v>
       </c>
       <c r="D53" s="17"/>
@@ -1805,199 +1805,199 @@
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="B54" s="0"/>
+      <c r="C54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
     </row>
     <row r="56">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
     </row>
     <row r="57">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
     </row>
     <row r="58">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
     </row>
     <row r="59">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
     </row>
     <row r="60">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
+      <c r="B60" s="0"/>
+      <c r="C60" s="0"/>
     </row>
     <row r="61">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="B61" s="0"/>
+      <c r="C61" s="0"/>
     </row>
     <row r="62">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="B62" s="0"/>
+      <c r="C62" s="0"/>
     </row>
     <row r="63">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="B63" s="0"/>
+      <c r="C63" s="0"/>
     </row>
     <row r="64">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="B64" s="0"/>
+      <c r="C64" s="0"/>
     </row>
     <row r="65">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
     </row>
     <row r="66">
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="B66" s="0"/>
+      <c r="C66" s="0"/>
     </row>
     <row r="67">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="B67" s="0"/>
+      <c r="C67" s="0"/>
     </row>
     <row r="68">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="B68" s="0"/>
+      <c r="C68" s="0"/>
     </row>
     <row r="69">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="B69" s="0"/>
+      <c r="C69" s="0"/>
     </row>
     <row r="70">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="B70" s="0"/>
+      <c r="C70" s="0"/>
     </row>
     <row r="71">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="B71" s="0"/>
+      <c r="C71" s="0"/>
     </row>
     <row r="72">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="B72" s="0"/>
+      <c r="C72" s="0"/>
     </row>
     <row r="73">
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="B73" s="0"/>
+      <c r="C73" s="0"/>
     </row>
     <row r="74">
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="B74" s="0"/>
+      <c r="C74" s="0"/>
     </row>
     <row r="75">
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="B75" s="0"/>
+      <c r="C75" s="0"/>
     </row>
     <row r="76">
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="B76" s="0"/>
+      <c r="C76" s="0"/>
     </row>
     <row r="77">
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="B77" s="0"/>
+      <c r="C77" s="0"/>
     </row>
     <row r="78">
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="B78" s="0"/>
+      <c r="C78" s="0"/>
     </row>
     <row r="79">
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="B79" s="0"/>
+      <c r="C79" s="0"/>
     </row>
     <row r="80">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="B80" s="0"/>
+      <c r="C80" s="0"/>
     </row>
     <row r="81">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="B81" s="0"/>
+      <c r="C81" s="0"/>
     </row>
     <row r="82">
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
+      <c r="B82" s="0"/>
+      <c r="C82" s="0"/>
     </row>
     <row r="83">
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="B83" s="0"/>
+      <c r="C83" s="0"/>
     </row>
     <row r="84">
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
+      <c r="B84" s="0"/>
+      <c r="C84" s="0"/>
     </row>
     <row r="85">
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
+      <c r="B85" s="0"/>
+      <c r="C85" s="0"/>
     </row>
     <row r="86">
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
+      <c r="B86" s="0"/>
+      <c r="C86" s="0"/>
     </row>
     <row r="87">
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
+      <c r="B87" s="0"/>
+      <c r="C87" s="0"/>
     </row>
     <row r="88">
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
+      <c r="B88" s="0"/>
+      <c r="C88" s="0"/>
     </row>
     <row r="89">
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
+      <c r="B89" s="0"/>
+      <c r="C89" s="0"/>
     </row>
     <row r="90">
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
+      <c r="B90" s="0"/>
+      <c r="C90" s="0"/>
     </row>
     <row r="91">
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="B91" s="0"/>
+      <c r="C91" s="0"/>
     </row>
     <row r="92">
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
+      <c r="B92" s="0"/>
+      <c r="C92" s="0"/>
     </row>
     <row r="93">
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
+      <c r="B93" s="0"/>
+      <c r="C93" s="0"/>
     </row>
     <row r="94">
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="B94" s="0"/>
+      <c r="C94" s="0"/>
     </row>
     <row r="95">
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
+      <c r="B95" s="0"/>
+      <c r="C95" s="0"/>
     </row>
     <row r="96">
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="B96" s="0"/>
+      <c r="C96" s="0"/>
     </row>
     <row r="97">
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
+      <c r="B97" s="0"/>
+      <c r="C97" s="0"/>
     </row>
     <row r="98">
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="B98" s="0"/>
+      <c r="C98" s="0"/>
     </row>
     <row r="99">
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="B99" s="0"/>
+      <c r="C99" s="0"/>
     </row>
     <row r="100">
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="B100" s="0"/>
+      <c r="C100" s="0"/>
     </row>
     <row r="101">
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="B101" s="0"/>
+      <c r="C101" s="0"/>
     </row>
     <row r="102">
       <c r="B102" s="1"/>
@@ -2047,40 +2047,40 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="1">
-        <v>2012673.0515710998</v>
-      </c>
-      <c r="B3" s="1">
-        <v>251904.90625</v>
-      </c>
-      <c r="C3" s="1">
-        <v>457207.40625</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="A3" s="0">
+        <v>2011022.1024419526</v>
+      </c>
+      <c r="B3" s="0">
+        <v>251362.515625</v>
+      </c>
+      <c r="C3" s="0">
+        <v>457400.625</v>
+      </c>
+      <c r="D3" s="0">
         <v>1000000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="0">
         <v>2653803.75</v>
       </c>
-      <c r="F3" s="1">
-        <v>4025439.875</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2079811.9578104364</v>
-      </c>
-      <c r="H3" s="1">
-        <v>272057.28125</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="F3" s="0">
+        <v>4013614</v>
+      </c>
+      <c r="G3" s="0">
+        <v>2078131.1615470054</v>
+      </c>
+      <c r="H3" s="0">
+        <v>271471.53125</v>
+      </c>
+      <c r="I3" s="0">
         <v>500000</v>
       </c>
-      <c r="J3" s="1">
-        <v>1058000.625</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="J3" s="0">
+        <v>1055722.625</v>
+      </c>
+      <c r="K3" s="0">
         <v>2653803.75</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="0">
         <v>4203804</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -2181,41 +2181,41 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="1">
-        <v>1520036.1149338242</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="0">
+        <v>1519751.3009426657</v>
+      </c>
+      <c r="B3" s="0">
         <v>250000</v>
       </c>
-      <c r="C3" s="1">
-        <v>251904.90625</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="0">
+        <v>251362.515625</v>
+      </c>
+      <c r="D3" s="0">
         <v>2203803.75</v>
       </c>
-      <c r="E3" s="1">
-        <v>2455708.75</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2556470.5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1519250.7368358569</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="E3" s="0">
+        <v>2455166.25</v>
+      </c>
+      <c r="F3" s="0">
+        <v>2555711.25</v>
+      </c>
+      <c r="G3" s="0">
+        <v>1519079.3485082455</v>
+      </c>
+      <c r="H3" s="0">
         <v>250000</v>
       </c>
-      <c r="I3" s="1">
-        <v>251904.90625</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="I3" s="0">
+        <v>251362.515625</v>
+      </c>
+      <c r="J3" s="0">
         <v>2203803.75</v>
       </c>
-      <c r="K3" s="1">
-        <v>2455708.75</v>
-      </c>
-      <c r="L3" s="1">
-        <v>2556470.5</v>
+      <c r="K3" s="0">
+        <v>2455166.25</v>
+      </c>
+      <c r="L3" s="0">
+        <v>2555711.25</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2320,40 +2320,40 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="1">
-        <v>9440112.9962030239</v>
-      </c>
-      <c r="B3" s="1">
-        <v>120914.3515625</v>
-      </c>
-      <c r="C3" s="1">
-        <v>201523.921875</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="A3" s="0">
+        <v>9405345.5259445123</v>
+      </c>
+      <c r="B3" s="0">
+        <v>120654.0078125</v>
+      </c>
+      <c r="C3" s="0">
+        <v>201090.015625</v>
+      </c>
+      <c r="D3" s="0">
         <v>300000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="0">
         <v>500000</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="0">
         <v>925000</v>
       </c>
-      <c r="G3" s="1">
-        <v>9376485.093861917</v>
-      </c>
-      <c r="H3" s="1">
-        <v>120914.3515625</v>
-      </c>
-      <c r="I3" s="1">
-        <v>201523.921875</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="G3" s="0">
+        <v>9341970.0548591763</v>
+      </c>
+      <c r="H3" s="0">
+        <v>120654.0078125</v>
+      </c>
+      <c r="I3" s="0">
+        <v>201090.015625</v>
+      </c>
+      <c r="J3" s="0">
         <v>300000</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="0">
         <v>500000</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="0">
         <v>925000</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -2459,40 +2459,40 @@
       <c r="M1" s="29"/>
     </row>
     <row r="3" s="5" customFormat="true">
-      <c r="A3" s="1">
-        <v>868703.25247404724</v>
-      </c>
-      <c r="B3" s="1">
-        <v>55419.078125</v>
-      </c>
-      <c r="C3" s="1">
-        <v>188103.75</v>
-      </c>
-      <c r="D3" s="1">
-        <v>302285.875</v>
-      </c>
-      <c r="E3" s="1">
-        <v>860511.875</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="A3" s="0">
+        <v>868287.75104398548</v>
+      </c>
+      <c r="B3" s="0">
+        <v>55299.75390625</v>
+      </c>
+      <c r="C3" s="0">
+        <v>186483.03125</v>
+      </c>
+      <c r="D3" s="0">
+        <v>301635.03125</v>
+      </c>
+      <c r="E3" s="0">
+        <v>861765.125</v>
+      </c>
+      <c r="F3" s="0">
         <v>2000000</v>
       </c>
-      <c r="G3" s="1">
-        <v>918953.52843286539</v>
-      </c>
-      <c r="H3" s="1">
-        <v>55419.078125</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="G3" s="0">
+        <v>918559.2920356486</v>
+      </c>
+      <c r="H3" s="0">
+        <v>55299.75390625</v>
+      </c>
+      <c r="I3" s="0">
         <v>200000</v>
       </c>
-      <c r="J3" s="1">
-        <v>312810.71875</v>
-      </c>
-      <c r="K3" s="1">
-        <v>860511.875</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="J3" s="0">
+        <v>312137.21875</v>
+      </c>
+      <c r="K3" s="0">
+        <v>861765.125</v>
+      </c>
+      <c r="L3" s="0">
         <v>2000000</v>
       </c>
       <c r="M3" s="4" t="s">

</xml_diff>

<commit_message>
Agregando ,stable y otras cositas
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -2048,13 +2048,13 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>2011022.1024419526</v>
+        <v>2011001.6655145618</v>
       </c>
       <c r="B3" s="0">
-        <v>251362.515625</v>
+        <v>251357.078125</v>
       </c>
       <c r="C3" s="0">
-        <v>457400.625</v>
+        <v>457395.671875</v>
       </c>
       <c r="D3" s="0">
         <v>1000000</v>
@@ -2063,19 +2063,19 @@
         <v>2653803.75</v>
       </c>
       <c r="F3" s="0">
-        <v>4013614</v>
+        <v>4013574.75</v>
       </c>
       <c r="G3" s="0">
-        <v>2078131.1615470054</v>
+        <v>2078110.4379400655</v>
       </c>
       <c r="H3" s="0">
-        <v>271471.53125</v>
+        <v>271465.65625</v>
       </c>
       <c r="I3" s="0">
         <v>500000</v>
       </c>
       <c r="J3" s="0">
-        <v>1055722.625</v>
+        <v>1055699.75</v>
       </c>
       <c r="K3" s="0">
         <v>2653803.75</v>
@@ -2182,40 +2182,40 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>1519751.3009426657</v>
+        <v>1519746.6826208543</v>
       </c>
       <c r="B3" s="0">
         <v>250000</v>
       </c>
       <c r="C3" s="0">
-        <v>251362.515625</v>
+        <v>251357.078125</v>
       </c>
       <c r="D3" s="0">
         <v>2203803.75</v>
       </c>
       <c r="E3" s="0">
-        <v>2455166.25</v>
+        <v>2455160.75</v>
       </c>
       <c r="F3" s="0">
-        <v>2555711.25</v>
+        <v>2555703.75</v>
       </c>
       <c r="G3" s="0">
-        <v>1519079.3485082455</v>
+        <v>1519125.402360185</v>
       </c>
       <c r="H3" s="0">
         <v>250000</v>
       </c>
       <c r="I3" s="0">
-        <v>251362.515625</v>
+        <v>251357.078125</v>
       </c>
       <c r="J3" s="0">
         <v>2203803.75</v>
       </c>
       <c r="K3" s="0">
-        <v>2455166.25</v>
+        <v>2455160.75</v>
       </c>
       <c r="L3" s="0">
-        <v>2555711.25</v>
+        <v>2555703.75</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2321,13 +2321,13 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>9405345.5259445123</v>
+        <v>9405235.5827523023</v>
       </c>
       <c r="B3" s="0">
-        <v>120654.0078125</v>
+        <v>120651.3984375</v>
       </c>
       <c r="C3" s="0">
-        <v>201090.015625</v>
+        <v>201085.671875</v>
       </c>
       <c r="D3" s="0">
         <v>300000</v>
@@ -2336,16 +2336,16 @@
         <v>500000</v>
       </c>
       <c r="F3" s="0">
-        <v>925000</v>
+        <v>924994.0625</v>
       </c>
       <c r="G3" s="0">
-        <v>9341970.0548591763</v>
+        <v>9341860.8559432384</v>
       </c>
       <c r="H3" s="0">
-        <v>120654.0078125</v>
+        <v>120651.3984375</v>
       </c>
       <c r="I3" s="0">
-        <v>201090.015625</v>
+        <v>201085.671875</v>
       </c>
       <c r="J3" s="0">
         <v>300000</v>
@@ -2354,7 +2354,7 @@
         <v>500000</v>
       </c>
       <c r="L3" s="0">
-        <v>925000</v>
+        <v>924994.0625</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2460,37 +2460,37 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>868287.75104398548</v>
+        <v>868275.70093919628</v>
       </c>
       <c r="B3" s="0">
-        <v>55299.75390625</v>
+        <v>55298.55859375</v>
       </c>
       <c r="C3" s="0">
-        <v>186483.03125</v>
+        <v>186483.921875</v>
       </c>
       <c r="D3" s="0">
-        <v>301635.03125</v>
+        <v>301628.5</v>
       </c>
       <c r="E3" s="0">
-        <v>861765.125</v>
+        <v>861750.875</v>
       </c>
       <c r="F3" s="0">
         <v>2000000</v>
       </c>
       <c r="G3" s="0">
-        <v>918559.2920356486</v>
+        <v>918546.60322865273</v>
       </c>
       <c r="H3" s="0">
-        <v>55299.75390625</v>
+        <v>55298.55859375</v>
       </c>
       <c r="I3" s="0">
         <v>200000</v>
       </c>
       <c r="J3" s="0">
-        <v>312137.21875</v>
+        <v>312130.46875</v>
       </c>
       <c r="K3" s="0">
-        <v>861765.125</v>
+        <v>861750.875</v>
       </c>
       <c r="L3" s="0">
         <v>2000000</v>

</xml_diff>

<commit_message>
Solucionado hasta pobreza + empezar ponderas
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -2048,13 +2048,13 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>2011001.6655145618</v>
+        <v>2011022.1024419526</v>
       </c>
       <c r="B3" s="0">
-        <v>251357.078125</v>
+        <v>251362.515625</v>
       </c>
       <c r="C3" s="0">
-        <v>457395.671875</v>
+        <v>457400.625</v>
       </c>
       <c r="D3" s="0">
         <v>1000000</v>
@@ -2063,19 +2063,19 @@
         <v>2653803.75</v>
       </c>
       <c r="F3" s="0">
-        <v>4013574.75</v>
+        <v>4013614</v>
       </c>
       <c r="G3" s="0">
-        <v>2078110.4379400655</v>
+        <v>2078131.1615470054</v>
       </c>
       <c r="H3" s="0">
-        <v>271465.65625</v>
+        <v>271471.53125</v>
       </c>
       <c r="I3" s="0">
         <v>500000</v>
       </c>
       <c r="J3" s="0">
-        <v>1055699.75</v>
+        <v>1055722.625</v>
       </c>
       <c r="K3" s="0">
         <v>2653803.75</v>
@@ -2182,40 +2182,40 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>1519746.6826208543</v>
+        <v>1519751.3009426657</v>
       </c>
       <c r="B3" s="0">
         <v>250000</v>
       </c>
       <c r="C3" s="0">
-        <v>251357.078125</v>
+        <v>251362.515625</v>
       </c>
       <c r="D3" s="0">
         <v>2203803.75</v>
       </c>
       <c r="E3" s="0">
-        <v>2455160.75</v>
+        <v>2455166.25</v>
       </c>
       <c r="F3" s="0">
-        <v>2555703.75</v>
+        <v>2555711.25</v>
       </c>
       <c r="G3" s="0">
-        <v>1519125.402360185</v>
+        <v>1519110.1494611988</v>
       </c>
       <c r="H3" s="0">
         <v>250000</v>
       </c>
       <c r="I3" s="0">
-        <v>251357.078125</v>
+        <v>251362.515625</v>
       </c>
       <c r="J3" s="0">
         <v>2203803.75</v>
       </c>
       <c r="K3" s="0">
-        <v>2455160.75</v>
+        <v>2455166.25</v>
       </c>
       <c r="L3" s="0">
-        <v>2555703.75</v>
+        <v>2555711.25</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2321,13 +2321,13 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>9405235.5827523023</v>
+        <v>9405345.5259445123</v>
       </c>
       <c r="B3" s="0">
-        <v>120651.3984375</v>
+        <v>120654.0078125</v>
       </c>
       <c r="C3" s="0">
-        <v>201085.671875</v>
+        <v>201090.015625</v>
       </c>
       <c r="D3" s="0">
         <v>300000</v>
@@ -2336,16 +2336,16 @@
         <v>500000</v>
       </c>
       <c r="F3" s="0">
-        <v>924994.0625</v>
+        <v>925000</v>
       </c>
       <c r="G3" s="0">
-        <v>9341860.8559432384</v>
+        <v>9341970.0548591763</v>
       </c>
       <c r="H3" s="0">
-        <v>120651.3984375</v>
+        <v>120654.0078125</v>
       </c>
       <c r="I3" s="0">
-        <v>201085.671875</v>
+        <v>201090.015625</v>
       </c>
       <c r="J3" s="0">
         <v>300000</v>
@@ -2354,7 +2354,7 @@
         <v>500000</v>
       </c>
       <c r="L3" s="0">
-        <v>924994.0625</v>
+        <v>925000</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2460,37 +2460,37 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="0">
-        <v>868275.70093919628</v>
+        <v>868287.75104398548</v>
       </c>
       <c r="B3" s="0">
-        <v>55298.55859375</v>
+        <v>55299.75390625</v>
       </c>
       <c r="C3" s="0">
-        <v>186483.921875</v>
+        <v>186483.03125</v>
       </c>
       <c r="D3" s="0">
-        <v>301628.5</v>
+        <v>301635.03125</v>
       </c>
       <c r="E3" s="0">
-        <v>861750.875</v>
+        <v>861765.125</v>
       </c>
       <c r="F3" s="0">
         <v>2000000</v>
       </c>
       <c r="G3" s="0">
-        <v>918546.60322865273</v>
+        <v>918559.2920356486</v>
       </c>
       <c r="H3" s="0">
-        <v>55298.55859375</v>
+        <v>55299.75390625</v>
       </c>
       <c r="I3" s="0">
         <v>200000</v>
       </c>
       <c r="J3" s="0">
-        <v>312130.46875</v>
+        <v>312137.21875</v>
       </c>
       <c r="K3" s="0">
-        <v>861750.875</v>
+        <v>861765.125</v>
       </c>
       <c r="L3" s="0">
         <v>2000000</v>

</xml_diff>

<commit_message>
Arreglito en CEDLAS para que corra
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -924,10 +924,10 @@
         <v>64</v>
       </c>
       <c r="B7" s="0">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0">
-        <v>0</v>
+        <v>0.30849915162733299</v>
       </c>
     </row>
     <row r="8">
@@ -935,10 +935,10 @@
         <v>65</v>
       </c>
       <c r="B8" s="0">
-        <v>2338</v>
+        <v>2378</v>
       </c>
       <c r="C8" s="0">
-        <v>18.031775412617616</v>
+        <v>18.34027456424495</v>
       </c>
     </row>
     <row r="9">
@@ -1006,10 +1006,10 @@
         <v>64</v>
       </c>
       <c r="B18" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>0.095877277085330767</v>
       </c>
     </row>
     <row r="19">
@@ -1017,10 +1017,10 @@
         <v>65</v>
       </c>
       <c r="B19" s="0">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C19" s="0">
-        <v>2.6366251198465962</v>
+        <v>2.7325023969319271</v>
       </c>
     </row>
     <row r="20">
@@ -1223,18 +1223,18 @@
     </row>
     <row r="3">
       <c r="B3" s="0">
-        <v>33.019674935842602</v>
+        <v>33.052985702270817</v>
       </c>
       <c r="C3" s="0">
-        <v>54.54545454545454</v>
+        <v>54.970760233918128</v>
       </c>
     </row>
     <row r="4" s="13" customFormat="true" ht="12">
       <c r="B4" s="0">
-        <v>66.980325064157398</v>
+        <v>66.947014297729183</v>
       </c>
       <c r="C4" s="0">
-        <v>45.454545454545453</v>
+        <v>45.029239766081872</v>
       </c>
     </row>
     <row r="5">
@@ -1249,10 +1249,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="0">
-        <v>0.34217279726261762</v>
+        <v>0.33641715727502103</v>
       </c>
       <c r="C6" s="0">
-        <v>0.60606060606060608</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -1261,7 +1261,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="0">
-        <v>12.446535500427716</v>
+        <v>12.363330529857022</v>
       </c>
       <c r="C7" s="0">
         <v>0</v>
@@ -1273,7 +1273,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="0">
-        <v>22.369546621043625</v>
+        <v>22.329688814129518</v>
       </c>
       <c r="C8" s="0">
         <v>0</v>
@@ -1285,10 +1285,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="0">
-        <v>23.096663815226691</v>
+        <v>23.25483599663583</v>
       </c>
       <c r="C9" s="0">
-        <v>1.2121212121212122</v>
+        <v>1.1695906432748537</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -1297,10 +1297,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="0">
-        <v>20.658682634730539</v>
+        <v>20.647603027754418</v>
       </c>
       <c r="C10" s="0">
-        <v>4.8484848484848486</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="D10" s="5"/>
     </row>
@@ -1309,10 +1309,10 @@
         <v>18</v>
       </c>
       <c r="B11" s="0">
-        <v>14.456800684345595</v>
+        <v>14.507989907485284</v>
       </c>
       <c r="C11" s="0">
-        <v>39.393939393939391</v>
+        <v>39.1812865497076</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -1321,10 +1321,10 @@
         <v>19</v>
       </c>
       <c r="B12" s="0">
-        <v>6.6295979469632158</v>
+        <v>6.5601345668629101</v>
       </c>
       <c r="C12" s="0">
-        <v>53.939393939393945</v>
+        <v>53.801169590643269</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -1341,10 +1341,10 @@
         <v>21</v>
       </c>
       <c r="B14" s="0">
-        <v>24.208725406330199</v>
+        <v>24.516400336417156</v>
       </c>
       <c r="C14" s="0">
-        <v>38.787878787878789</v>
+        <v>38.011695906432749</v>
       </c>
       <c r="D14" s="5"/>
     </row>
@@ -1353,10 +1353,10 @@
         <v>22</v>
       </c>
       <c r="B15" s="0">
-        <v>32.720273738237807</v>
+        <v>32.506307821698904</v>
       </c>
       <c r="C15" s="0">
-        <v>15.151515151515152</v>
+        <v>15.789473684210526</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -1365,10 +1365,10 @@
         <v>59</v>
       </c>
       <c r="B16" s="0">
-        <v>29.170230966638151</v>
+        <v>29.100084104289319</v>
       </c>
       <c r="C16" s="0">
-        <v>9.6969696969696972</v>
+        <v>9.9415204678362574</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -1377,10 +1377,10 @@
         <v>54</v>
       </c>
       <c r="B17" s="0">
-        <v>11.035072711719419</v>
+        <v>10.933557611438182</v>
       </c>
       <c r="C17" s="0">
-        <v>12.121212121212121</v>
+        <v>12.865497076023392</v>
       </c>
       <c r="D17" s="5"/>
     </row>
@@ -1389,10 +1389,10 @@
         <v>58</v>
       </c>
       <c r="B18" s="0">
-        <v>2.737382378100941</v>
+        <v>2.8174936921783011</v>
       </c>
       <c r="C18" s="0">
-        <v>23.636363636363637</v>
+        <v>22.807017543859647</v>
       </c>
       <c r="D18" s="5"/>
     </row>
@@ -1401,10 +1401,10 @@
         <v>55</v>
       </c>
       <c r="B19" s="0">
-        <v>0.12831479897348161</v>
+        <v>0.12615643397813289</v>
       </c>
       <c r="C19" s="0">
-        <v>0.60606060606060608</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D19" s="5"/>
     </row>
@@ -1421,7 +1421,7 @@
         <v>57</v>
       </c>
       <c r="B21" s="0">
-        <v>0.29940119760479045</v>
+        <v>0.29436501261564341</v>
       </c>
       <c r="C21" s="0">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>37</v>
       </c>
       <c r="B22" s="0">
-        <v>0.12831479897348161</v>
+        <v>0.12615643397813289</v>
       </c>
       <c r="C22" s="0">
-        <v>0.60606060606060608</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D22" s="5"/>
     </row>
@@ -1445,10 +1445,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="0">
-        <v>26.860564585115483</v>
+        <v>26.703111858704791</v>
       </c>
       <c r="C23" s="0">
-        <v>50.303030303030305</v>
+        <v>49.122807017543856</v>
       </c>
       <c r="D23" s="17"/>
     </row>
@@ -1457,10 +1457,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="0">
-        <v>46.963216424294266</v>
+        <v>46.761984861227923</v>
       </c>
       <c r="C24" s="0">
-        <v>23.030303030303031</v>
+        <v>23.391812865497073</v>
       </c>
       <c r="D24" s="5"/>
     </row>
@@ -1469,10 +1469,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="0">
-        <v>5.7313943541488452</v>
+        <v>5.9714045416316228</v>
       </c>
       <c r="C25" s="0">
-        <v>7.878787878787878</v>
+        <v>8.1871345029239766</v>
       </c>
       <c r="D25" s="5"/>
     </row>
@@ -1481,10 +1481,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="0">
-        <v>14.713430282292558</v>
+        <v>14.760302775441547</v>
       </c>
       <c r="C26" s="0">
-        <v>9.0909090909090917</v>
+        <v>8.7719298245614024</v>
       </c>
       <c r="D26" s="5"/>
     </row>
@@ -1493,7 +1493,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="0">
-        <v>0.5988023952095809</v>
+        <v>0.67283431455004206</v>
       </c>
       <c r="C27" s="0">
         <v>0</v>
@@ -1505,10 +1505,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="0">
-        <v>4.7048759623609921</v>
+        <v>4.7098402018502945</v>
       </c>
       <c r="C28" s="0">
-        <v>9.0909090909090917</v>
+        <v>9.9415204678362574</v>
       </c>
       <c r="D28" s="5"/>
     </row>
@@ -1525,10 +1525,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="0">
-        <v>9.1103507271171953</v>
+        <v>9.3355761143818334</v>
       </c>
       <c r="C30" s="0">
-        <v>9.0909090909090917</v>
+        <v>8.7719298245614024</v>
       </c>
       <c r="D30" s="5"/>
     </row>
@@ -1537,10 +1537,10 @@
         <v>37</v>
       </c>
       <c r="B31" s="0">
-        <v>6.5440547476475626</v>
+        <v>6.9386038687973093</v>
       </c>
       <c r="C31" s="0">
-        <v>3.0303030303030303</v>
+        <v>2.9239766081871341</v>
       </c>
       <c r="D31" s="5"/>
     </row>
@@ -1549,10 +1549,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="0">
-        <v>9.9230111206159108</v>
+        <v>9.9663582842724967</v>
       </c>
       <c r="C32" s="0">
-        <v>3.0303030303030303</v>
+        <v>2.9239766081871341</v>
       </c>
       <c r="D32" s="5"/>
     </row>
@@ -1561,10 +1561,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="0">
-        <v>67.536355859709147</v>
+        <v>66.904962153069803</v>
       </c>
       <c r="C33" s="0">
-        <v>10.303030303030303</v>
+        <v>12.280701754385964</v>
       </c>
       <c r="D33" s="5"/>
     </row>
@@ -1573,7 +1573,7 @@
         <v>39</v>
       </c>
       <c r="B34" s="0">
-        <v>0.4704875962360992</v>
+        <v>0.50462573591253157</v>
       </c>
       <c r="C34" s="0">
         <v>0</v>
@@ -1585,7 +1585,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="0">
-        <v>3.721129170230967</v>
+        <v>3.7005887300252311</v>
       </c>
       <c r="C35" s="0">
         <v>0</v>
@@ -1597,10 +1597,10 @@
         <v>33</v>
       </c>
       <c r="B36" s="0">
-        <v>2.3524379811804961</v>
+        <v>2.3128679562657695</v>
       </c>
       <c r="C36" s="0">
-        <v>1.8181818181818181</v>
+        <v>1.7543859649122806</v>
       </c>
       <c r="D36" s="5"/>
     </row>
@@ -1609,10 +1609,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="0">
-        <v>0.34217279726261762</v>
+        <v>0.33641715727502103</v>
       </c>
       <c r="C37" s="0">
-        <v>72.727272727272734</v>
+        <v>71.345029239766077</v>
       </c>
       <c r="D37" s="5"/>
     </row>
@@ -1629,10 +1629,10 @@
         <v>36</v>
       </c>
       <c r="B39" s="0">
-        <v>18.006843455945251</v>
+        <v>18.040370058873005</v>
       </c>
       <c r="C39" s="0">
-        <v>6.0606060606060606</v>
+        <v>5.8479532163742682</v>
       </c>
       <c r="D39" s="5"/>
     </row>
@@ -1641,10 +1641,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="0">
-        <v>0.5988023952095809</v>
+        <v>0.58873002523128681</v>
       </c>
       <c r="C40" s="0">
-        <v>0.60606060606060608</v>
+        <v>1.1695906432748537</v>
       </c>
       <c r="D40" s="5"/>
     </row>
@@ -1653,10 +1653,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="0">
-        <v>1.6680923866552608</v>
+        <v>1.808242220353238</v>
       </c>
       <c r="C41" s="0">
-        <v>0.60606060606060608</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D41" s="17"/>
     </row>
@@ -1665,10 +1665,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="0">
-        <v>1.4114627887082978</v>
+        <v>1.3877207737594619</v>
       </c>
       <c r="C42" s="0">
-        <v>0.60606060606060608</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="18"/>
@@ -1678,10 +1678,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="0">
-        <v>5.7313943541488452</v>
+        <v>5.6349873843566023</v>
       </c>
       <c r="C43" s="0">
-        <v>2.4242424242424243</v>
+        <v>2.3391812865497075</v>
       </c>
       <c r="D43" s="5"/>
     </row>
@@ -1690,10 +1690,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="0">
-        <v>20.273738237810093</v>
+        <v>20.142977291841884</v>
       </c>
       <c r="C44" s="0">
-        <v>1.2121212121212122</v>
+        <v>1.7543859649122806</v>
       </c>
       <c r="D44" s="5"/>
     </row>
@@ -1702,10 +1702,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="0">
-        <v>11.676646706586826</v>
+        <v>11.606391925988225</v>
       </c>
       <c r="C45" s="0">
-        <v>2.4242424242424243</v>
+        <v>2.3391812865497075</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -1714,10 +1714,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="0">
-        <v>3.20786997433704</v>
+        <v>3.280067283431455</v>
       </c>
       <c r="C46" s="0">
-        <v>0.60606060606060608</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D46" s="5"/>
     </row>
@@ -1726,10 +1726,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="0">
-        <v>8.8109495295124027</v>
+        <v>8.9571068124474351</v>
       </c>
       <c r="C47" s="0">
-        <v>6.666666666666667</v>
+        <v>7.0175438596491224</v>
       </c>
       <c r="D47" s="5"/>
     </row>
@@ -1738,10 +1738,10 @@
         <v>48</v>
       </c>
       <c r="B48" s="0">
-        <v>28.272027373823782</v>
+        <v>28.216989066442387</v>
       </c>
       <c r="C48" s="0">
-        <v>6.0606060606060606</v>
+        <v>6.4327485380116958</v>
       </c>
       <c r="D48" s="5"/>
     </row>
@@ -1750,10 +1750,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="0">
-        <v>0.34217279726261762</v>
+        <v>0.33641715727502103</v>
       </c>
       <c r="C49" s="0">
-        <v>72.727272727272734</v>
+        <v>71.345029239766077</v>
       </c>
       <c r="D49" s="5"/>
     </row>
@@ -1770,10 +1770,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="0">
-        <v>19.674935842600512</v>
+        <v>19.638351555929354</v>
       </c>
       <c r="C51" s="0">
-        <v>10.303030303030303</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="D51" s="5"/>
     </row>
@@ -1782,10 +1782,10 @@
         <v>37</v>
       </c>
       <c r="B52" s="0">
-        <v>80.325064157399481</v>
+        <v>80.361648444070639</v>
       </c>
       <c r="C52" s="0">
-        <v>89.696969696969703</v>
+        <v>89.473684210526315</v>
       </c>
       <c r="D52" s="5"/>
     </row>
@@ -2066,7 +2066,7 @@
         <v>4000000</v>
       </c>
       <c r="G3" s="0">
-        <v>2123473.3427020512</v>
+        <v>2122992.6601368403</v>
       </c>
       <c r="H3" s="0">
         <v>280000</v>
@@ -2081,7 +2081,7 @@
         <v>2653558.75</v>
       </c>
       <c r="L3" s="0">
-        <v>4271499</v>
+        <v>4268412</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2200,7 +2200,7 @@
         <v>2553613.25</v>
       </c>
       <c r="G3" s="0">
-        <v>1536925.2511139384</v>
+        <v>1541093.4671792437</v>
       </c>
       <c r="H3" s="0">
         <v>249863.890625</v>

</xml_diff>

<commit_message>
Última corrida (ESPEREMOS FINAL)
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -2066,22 +2066,22 @@
         <v>4000000</v>
       </c>
       <c r="G3" s="0">
-        <v>2109222.6644164398</v>
+        <v>2080805.9128611058</v>
       </c>
       <c r="H3" s="0">
-        <v>280000</v>
+        <v>299415.71875</v>
       </c>
       <c r="I3" s="0">
-        <v>499026.21875</v>
+        <v>538948.3125</v>
       </c>
       <c r="J3" s="0">
-        <v>1089033.8125</v>
+        <v>1461299</v>
       </c>
       <c r="K3" s="0">
-        <v>2652927.25</v>
+        <v>2653803.75</v>
       </c>
       <c r="L3" s="0">
-        <v>4256624</v>
+        <v>3880000</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2200,7 +2200,7 @@
         <v>2553122</v>
       </c>
       <c r="G3" s="0">
-        <v>1540915.8860893724</v>
+        <v>1542192.2846315436</v>
       </c>
       <c r="H3" s="0">
         <v>249513.109375</v>
@@ -2339,7 +2339,7 @@
         <v>917000</v>
       </c>
       <c r="G3" s="0">
-        <v>9105352.5361602288</v>
+        <v>9105707.0312418621</v>
       </c>
       <c r="H3" s="0">
         <v>122509.8828125</v>
@@ -2354,7 +2354,7 @@
         <v>499026.21875</v>
       </c>
       <c r="L3" s="0">
-        <v>930000</v>
+        <v>900764.8125</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>
@@ -2478,22 +2478,22 @@
         <v>1996104.875</v>
       </c>
       <c r="G3" s="0">
-        <v>844363.77948566957</v>
+        <v>866425.13373399491</v>
       </c>
       <c r="H3" s="0">
-        <v>57697.703125</v>
+        <v>60000</v>
       </c>
       <c r="I3" s="0">
-        <v>189183.28125</v>
+        <v>199610.484375</v>
       </c>
       <c r="J3" s="0">
-        <v>300000</v>
+        <v>349318.34375</v>
       </c>
       <c r="K3" s="0">
-        <v>856780.4375</v>
+        <v>945916.4375</v>
       </c>
       <c r="L3" s="0">
-        <v>1996104.875</v>
+        <v>2000000</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Analizo problemas renta imputada
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb550905\Github\VEN\data_management\management\4. income imputation\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1DB2FA-FD56-4370-A325-851A963B1601}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233CECE-24FF-4E3D-9BD6-E21EE701AC21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missing_values" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,19 @@
     <sheet name="labor_beneimp_stochastic_reg" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
-  <si>
-    <t>2019</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>p90</t>
   </si>
@@ -39,9 +44,6 @@
     <t>Imputing missing values</t>
   </si>
   <si>
-    <t>Profile of employed with missing values in labor income</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
@@ -183,9 +185,6 @@
     <t>Convive</t>
   </si>
   <si>
-    <t>Estados civil</t>
-  </si>
-  <si>
     <t>Monetary labor income</t>
   </si>
   <si>
@@ -273,10 +272,34 @@
     <t>kd_bene1</t>
   </si>
   <si>
-    <t>p99</t>
-  </si>
-  <si>
     <t>Missing values: outliers (not included)</t>
+  </si>
+  <si>
+    <t>Estado civil</t>
+  </si>
+  <si>
+    <t>Labor income%</t>
+  </si>
+  <si>
+    <t>Pensions%</t>
+  </si>
+  <si>
+    <t>Profile missing values</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p50</t>
+  </si>
+  <si>
+    <t>p75</t>
   </si>
 </sst>
 </file>
@@ -343,13 +366,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <name val="Calibri Light"/>
@@ -377,8 +393,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,18 +407,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -447,15 +461,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -519,17 +524,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -537,47 +539,57 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -891,361 +903,361 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="34.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="B1" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>77</v>
+      <c r="B1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8">
+      <c r="A4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="16">
+        <v>186</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1.4345210550670986</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8">
+      <c r="A5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="18">
+        <v>356</v>
+      </c>
+      <c r="C5" s="19">
+        <v>2.7456424494832641</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8">
+      <c r="A6" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.8">
-      <c r="A4" s="17" t="s">
+      <c r="B6" s="20">
+        <v>1675</v>
+      </c>
+      <c r="C6" s="21">
+        <v>12.91840197439457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="22">
-        <v>186</v>
-      </c>
-      <c r="C4" s="23">
-        <v>1.4345210550670986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8">
-      <c r="A5" s="17" t="s">
+      <c r="B7" s="22">
+        <v>43</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0.331636587999383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="24">
-        <v>356</v>
-      </c>
-      <c r="C5" s="25">
-        <v>2.7456424494832641</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8">
-      <c r="A6" s="17" t="s">
+      <c r="B8" s="24">
+        <v>2074</v>
+      </c>
+      <c r="C8" s="25">
+        <v>15.995681011877217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="26">
-        <v>1675</v>
-      </c>
-      <c r="C6" s="27">
-        <v>12.91840197439457</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="17" t="s">
+      <c r="B9" s="16">
+        <v>10672</v>
+      </c>
+      <c r="C9" s="17">
+        <v>82.307573654172444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="28">
-        <v>43</v>
-      </c>
-      <c r="C7" s="29">
-        <v>0.331636587999383</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="17" t="s">
+      <c r="B10" s="26">
+        <v>12966</v>
+      </c>
+      <c r="C10" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" s="28"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" s="28"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="30">
-        <v>2074</v>
-      </c>
-      <c r="C8" s="31">
-        <v>15.995681011877217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="17" t="s">
+      <c r="C13" s="28"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="1:3" ht="28.8">
+      <c r="A15" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="22">
-        <v>10672</v>
-      </c>
-      <c r="C9" s="23">
-        <v>82.307573654172444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="18" t="s">
+      <c r="B15" s="16">
+        <v>23447</v>
+      </c>
+      <c r="C15" s="17">
+        <v>374.6724193032918</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8">
+      <c r="A16" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="32">
-        <v>12966</v>
-      </c>
-      <c r="C10" s="33">
+      <c r="B16" s="18">
+        <v>7</v>
+      </c>
+      <c r="C16" s="19">
+        <v>0.11185682326621924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8">
+      <c r="A17" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="20">
+        <v>18</v>
+      </c>
+      <c r="C17" s="21">
+        <v>0.28763183125599234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="22">
+        <v>7</v>
+      </c>
+      <c r="C18" s="23">
+        <v>0.11185682326621924</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="24">
+        <v>32</v>
+      </c>
+      <c r="C19" s="25">
+        <v>0.51134547778843076</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="16">
+        <v>6163</v>
+      </c>
+      <c r="C20" s="17">
+        <v>98.4819431128156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29.4" customHeight="1">
+      <c r="A21" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="26">
+        <v>6258</v>
+      </c>
+      <c r="C21" s="27">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="C11" s="34"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="C12" s="34"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="34"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="C14" s="34"/>
-    </row>
-    <row r="15" spans="1:3" ht="28.8">
-      <c r="A15" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="22">
-        <v>23447</v>
-      </c>
-      <c r="C15" s="23">
-        <v>374.6724193032918</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8">
-      <c r="A16" s="17" t="s">
+    <row r="22" spans="1:3">
+      <c r="C22" s="28"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="C23" s="28"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="24">
-        <v>7</v>
-      </c>
-      <c r="C16" s="25">
-        <v>0.11185682326621924</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8">
-      <c r="A17" s="17" t="s">
+      <c r="C24" s="28"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="C25" s="28"/>
+    </row>
+    <row r="26" spans="1:3" ht="28.8">
+      <c r="A26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="26">
-        <v>18</v>
-      </c>
-      <c r="C17" s="27">
-        <v>0.28763183125599234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="17" t="s">
+      <c r="B26" s="16">
+        <v>15</v>
+      </c>
+      <c r="C26" s="17">
+        <v>1.6816143497757847</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.8">
+      <c r="A27" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="18">
+        <v>20</v>
+      </c>
+      <c r="C27" s="19">
+        <v>2.2421524663677128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="22">
+        <v>2</v>
+      </c>
+      <c r="C28" s="23">
+        <v>0.22421524663677131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="29">
+        <v>22</v>
+      </c>
+      <c r="C29" s="30">
+        <v>2.4663677130044843</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="16">
+        <v>855</v>
+      </c>
+      <c r="C30" s="17">
+        <v>95.852017937219742</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="32">
+        <v>892</v>
+      </c>
+      <c r="C31" s="33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="C32" s="28"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="C33" s="28"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="28"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" s="28"/>
+    </row>
+    <row r="36" spans="1:3" ht="28.8">
+      <c r="A36" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="16">
+        <v>25117</v>
+      </c>
+      <c r="C36" s="17">
+        <v>313.96250000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="28.8">
+      <c r="A37" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="18">
         <v>57</v>
       </c>
-      <c r="B18" s="28">
-        <v>7</v>
-      </c>
-      <c r="C18" s="29">
-        <v>0.11185682326621924</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="30">
-        <v>32</v>
-      </c>
-      <c r="C19" s="31">
-        <v>0.51134547778843076</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="22">
-        <v>6163</v>
-      </c>
-      <c r="C20" s="23">
-        <v>98.4819431128156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29.4" customHeight="1">
-      <c r="A21" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="32">
-        <v>6258</v>
-      </c>
-      <c r="C21" s="33">
+      <c r="C37" s="19">
+        <v>0.71250000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="29">
+        <v>57</v>
+      </c>
+      <c r="C39" s="30">
+        <v>0.71250000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="16">
+        <v>7936</v>
+      </c>
+      <c r="C40" s="17">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="32">
+        <v>8000</v>
+      </c>
+      <c r="C41" s="33">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="C22" s="34"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="C23" s="34"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="34"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="C25" s="34"/>
-    </row>
-    <row r="26" spans="1:3" ht="28.8">
-      <c r="A26" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="22">
-        <v>15</v>
-      </c>
-      <c r="C26" s="23">
-        <v>1.6816143497757847</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="28.8">
-      <c r="A27" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="24">
-        <v>20</v>
-      </c>
-      <c r="C27" s="25">
-        <v>2.2421524663677128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="28">
-        <v>2</v>
-      </c>
-      <c r="C28" s="29">
-        <v>0.22421524663677131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="35">
-        <v>22</v>
-      </c>
-      <c r="C29" s="36">
-        <v>2.4663677130044843</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="22">
-        <v>855</v>
-      </c>
-      <c r="C30" s="23">
-        <v>95.852017937219742</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="38">
-        <v>892</v>
-      </c>
-      <c r="C31" s="39">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="C32" s="34"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="C33" s="34"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="34"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="C35" s="34"/>
-    </row>
-    <row r="36" spans="1:3" ht="28.8">
-      <c r="A36" s="17" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" s="22">
-        <v>25117</v>
-      </c>
-      <c r="C36" s="23">
-        <v>313.96250000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="28.8">
-      <c r="A37" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="24">
-        <v>57</v>
-      </c>
-      <c r="C37" s="25">
-        <v>0.71250000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="35">
-        <v>57</v>
-      </c>
-      <c r="C39" s="36">
-        <v>0.71250000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="22">
-        <v>7936</v>
-      </c>
-      <c r="C40" s="23">
-        <v>99.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="38">
-        <v>8000</v>
-      </c>
-      <c r="C41" s="39">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="20" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1270,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1269,609 +1281,613 @@
     <col min="4" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="15.6">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="15.6">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="43.2">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" ht="15.6">
-      <c r="A2" s="7"/>
-      <c r="B2"/>
-      <c r="C2"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3">
+      <c r="B3" s="34">
         <v>31.3404050144648</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="35">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1">
-      <c r="B4">
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="34">
         <v>68.659594985535193</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="35">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5"/>
-    </row>
-    <row r="6" spans="1:4">
+    <row r="5" spans="1:5">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="B6" s="34">
         <v>0.33751205400192863</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="35">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="B7" s="34">
         <v>12.391513982642238</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="35">
         <v>0</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="34">
         <v>22.709739633558339</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="35">
         <v>0</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="B9" s="34">
         <v>23.288331726133077</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="35">
         <v>3.125</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="B10" s="34">
         <v>19.913211186113791</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="35">
         <v>15.625</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="B11" s="34">
         <v>14.609450337512053</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="35">
         <v>37.5</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="B12" s="34">
         <v>6.750241080038573</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="35">
         <v>43.75</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="B14" s="34">
         <v>24.541947926711668</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="35">
         <v>31.25</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
+        <v>49</v>
+      </c>
+      <c r="B15" s="34">
         <v>32.497589199614275</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="35">
         <v>25</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="34">
         <v>29.411764705882355</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="35">
         <v>9.375</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="34">
         <v>10.752169720347156</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="35">
         <v>15.625</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18">
+        <v>48</v>
+      </c>
+      <c r="B18" s="34">
         <v>2.651880424300868</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="35">
         <v>18.75</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19">
+        <v>28</v>
+      </c>
+      <c r="B19" s="34">
         <v>0.14464802314368372</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="35">
         <v>0</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="B21" s="34">
         <v>0.33751205400192863</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="35">
         <v>0</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="B22" s="34">
         <v>0.14464802314368372</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="35">
         <v>0</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" s="12" customFormat="1">
-      <c r="A23" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" s="8" customFormat="1">
+      <c r="A23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="34">
         <v>26.808100289296043</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="35">
         <v>40.625</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24">
+        <v>18</v>
+      </c>
+      <c r="B24" s="34">
         <v>47.782063645130187</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="35">
         <v>21.875</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25">
+        <v>19</v>
+      </c>
+      <c r="B25" s="34">
         <v>5.4001928640308581</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="35">
         <v>6.25</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="B26" s="34">
         <v>14.271938283510124</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="35">
         <v>15.625</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27">
+        <v>21</v>
+      </c>
+      <c r="B27" s="34">
         <v>0.48216007714561238</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="35">
         <v>0</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28">
+        <v>28</v>
+      </c>
+      <c r="B28" s="34">
         <v>4.7733847637415625</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="35">
         <v>15.625</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29" s="3"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="34">
         <v>4.6769527483124396</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="35">
         <v>0</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="34">
         <v>4.725168756027001</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="35">
         <v>0</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="34">
         <v>11.041465766634524</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="35">
         <v>3.125</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33">
+        <v>24</v>
+      </c>
+      <c r="B33" s="34">
         <v>72.275795564127293</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="35">
         <v>18.75</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34">
+        <v>25</v>
+      </c>
+      <c r="B34" s="34">
         <v>0.43394406943105107</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="35">
         <v>0</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35">
+        <v>26</v>
+      </c>
+      <c r="B35" s="34">
         <v>4.0019286403085825</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="35">
         <v>0</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36">
+        <v>27</v>
+      </c>
+      <c r="B36" s="34">
         <v>2.651880424300868</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="35">
         <v>0</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37">
+        <v>28</v>
+      </c>
+      <c r="B37" s="34">
         <v>0.19286403085824494</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="35">
         <v>78.125</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39">
+        <v>32</v>
+      </c>
+      <c r="B39" s="34">
         <v>18.659594985535197</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="35">
         <v>0</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40">
+        <v>33</v>
+      </c>
+      <c r="B40" s="34">
         <v>0.67502410800385726</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="35">
         <v>3.125</v>
       </c>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" s="12" customFormat="1">
-      <c r="A41" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" s="8" customFormat="1">
+      <c r="A41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="34">
         <v>1.832208293153327</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="35">
         <v>3.125</v>
       </c>
-      <c r="D41" s="13"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42">
+        <v>35</v>
+      </c>
+      <c r="B42" s="34">
         <v>1.1571841851494697</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="35">
         <v>0</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="14"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43">
+        <v>36</v>
+      </c>
+      <c r="B43" s="34">
         <v>5.7859209257473481</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="35">
         <v>3.125</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44">
+        <v>37</v>
+      </c>
+      <c r="B44" s="34">
         <v>20.588235294117645</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="35">
         <v>3.125</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45">
+        <v>39</v>
+      </c>
+      <c r="B45" s="34">
         <v>12.391513982642238</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="35">
         <v>0</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="34">
         <v>2.892960462873674</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="35">
         <v>0</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47">
+        <v>40</v>
+      </c>
+      <c r="B47" s="34">
         <v>6.075216972034716</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="35">
         <v>3.125</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="34">
         <v>29.749276759884282</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="35">
         <v>6.25</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B49">
+        <v>28</v>
+      </c>
+      <c r="B49" s="34">
         <v>0.19286403085824494</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="35">
         <v>78.125</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50" s="3"/>
+      <c r="A50" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51">
+        <v>42</v>
+      </c>
+      <c r="B51" s="34">
         <v>18.900675024108004</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="35">
         <v>15.625</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B52">
+        <v>43</v>
+      </c>
+      <c r="B52" s="34">
         <v>81.099324975891989</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="35">
         <v>84.375</v>
       </c>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" s="12" customFormat="1">
-      <c r="A53" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53">
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" s="8" customFormat="1">
+      <c r="B53" s="34">
         <v>0</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="35">
         <v>0</v>
       </c>
-      <c r="D53" s="13"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="B54"/>
       <c r="C54"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="B55"/>
       <c r="C55"/>
     </row>
@@ -2067,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2085,114 +2101,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1">
-      <c r="A3">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="38"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1">
+      <c r="A3" s="42">
         <v>2006937.0944554566</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="42">
         <v>250056.625</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="42">
         <v>455677.6875</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="42">
         <v>1000000</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="42">
         <v>2653803.75</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="42">
         <v>4000906</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="42">
         <v>2062216.8450810947</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="42">
         <v>300000</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="42">
         <v>500113.28125</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="42">
         <v>1450000</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="42">
         <v>2653803.75</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="42">
         <v>3788069.25</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2013340.0766250594</v>
-      </c>
-      <c r="C4" s="5">
-        <v>251904.90625</v>
-      </c>
-      <c r="D4" s="5">
-        <v>454765.71875</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1000000</v>
-      </c>
-      <c r="F4" s="5">
-        <v>2653803.75</v>
-      </c>
-      <c r="G4" s="6">
-        <v>4030478.5</v>
-      </c>
-      <c r="H4" s="5">
-        <v>2018915.0637623686</v>
-      </c>
-      <c r="I4" s="5">
-        <v>251904.90625</v>
-      </c>
-      <c r="J4" s="5">
-        <v>473581.21875</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1000000</v>
-      </c>
-      <c r="L4" s="5">
-        <v>2616927.75</v>
-      </c>
-      <c r="M4" s="6">
-        <v>4042826.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
-        <v>78</v>
+      <c r="M3" s="39"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="M4" s="38"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="M5" s="38"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2201,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L2" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2219,126 +2238,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-    </row>
-    <row r="3" spans="1:15" s="3" customFormat="1">
-      <c r="A3">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="38"/>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="A3" s="42">
         <v>1518811.1937084021</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="42">
         <v>250000</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="42">
         <v>250056.625</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="42">
         <v>2203803.75</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="42">
         <v>2453860.5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="42">
         <v>2553883</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="42">
         <v>1517850.4823062764</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="42">
         <v>250000</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="42">
         <v>250056.625</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="42">
         <v>2203803.75</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="42">
         <v>2453860.5</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="42">
         <v>2553883</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="3" customFormat="1">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1519927.2796204803</v>
-      </c>
-      <c r="C4" s="5">
-        <v>250000</v>
-      </c>
-      <c r="D4" s="5">
-        <v>251904.90625</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2203803.75</v>
-      </c>
-      <c r="F4" s="5">
-        <v>2455708.75</v>
-      </c>
-      <c r="G4" s="6">
-        <v>2556470.5</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1519518.541647075</v>
-      </c>
-      <c r="I4" s="5">
-        <v>250000</v>
-      </c>
-      <c r="J4" s="5">
-        <v>251904.90625</v>
-      </c>
-      <c r="K4" s="5">
-        <v>2203803.75</v>
-      </c>
-      <c r="L4" s="5">
-        <v>2455708.75</v>
-      </c>
-      <c r="M4" s="6">
-        <v>2556470.5</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2556470.5</v>
-      </c>
-      <c r="O4" s="1">
-        <v>3444074</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="1" t="s">
-        <v>79</v>
+      <c r="M3" s="39"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1">
+      <c r="A4" s="43"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2346,10 +2369,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="L2" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2358,126 +2381,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-    </row>
-    <row r="3" spans="1:15" s="3" customFormat="1">
-      <c r="A3">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="A3" s="42">
         <v>9411043.7327192165</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="42">
         <v>120027.1796875</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="42">
         <v>200045.296875</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="42">
         <v>300000</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="42">
         <v>500000</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="42">
         <v>921868.4375</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="42">
         <v>9348053.9164523259</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="42">
         <v>121000</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="42">
         <v>200045.296875</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="42">
         <v>300000</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="42">
         <v>500000</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="42">
         <v>915853.0625</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="3" customFormat="1">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5">
-        <v>9458464.3975915201</v>
-      </c>
-      <c r="C4" s="5">
-        <v>120914.3515625</v>
-      </c>
-      <c r="D4" s="5">
-        <v>201523.921875</v>
-      </c>
-      <c r="E4" s="5">
-        <v>300000</v>
-      </c>
-      <c r="F4" s="5">
-        <v>500000</v>
-      </c>
-      <c r="G4" s="6">
-        <v>927010</v>
-      </c>
-      <c r="H4" s="5">
-        <v>9394301.2418644987</v>
-      </c>
-      <c r="I4" s="5">
-        <v>120581.8125</v>
-      </c>
-      <c r="J4" s="5">
-        <v>201523.921875</v>
-      </c>
-      <c r="K4" s="5">
-        <v>300000</v>
-      </c>
-      <c r="L4" s="5">
-        <v>500000</v>
-      </c>
-      <c r="M4" s="6">
-        <v>930000</v>
-      </c>
-      <c r="N4" s="1">
-        <v>834001</v>
-      </c>
-      <c r="O4" s="1">
-        <v>2720574</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="1" t="s">
-        <v>80</v>
+      <c r="M3" s="39"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2485,10 +2502,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2497,126 +2514,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-    </row>
-    <row r="3" spans="1:15" s="3" customFormat="1">
-      <c r="A3">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="A3" s="42">
         <v>865994.29392043944</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="42">
         <v>55012.45703125</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="42">
         <v>188868.25</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="42">
         <v>300067.9375</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="42">
         <v>856391.0625</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="42">
         <v>2000000</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="42">
         <v>896981.88475139765</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="42">
         <v>60000</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="42">
         <v>200000</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="42">
         <v>328074.28125</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="42">
         <v>922484.625</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="42">
         <v>2000453</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="3" customFormat="1">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5">
-        <v>868703.25247404724</v>
-      </c>
-      <c r="C4" s="5">
-        <v>55419.078125</v>
-      </c>
-      <c r="D4" s="5">
-        <v>188103.75</v>
-      </c>
-      <c r="E4" s="5">
-        <v>302285.875</v>
-      </c>
-      <c r="F4" s="5">
-        <v>860511.875</v>
-      </c>
-      <c r="G4" s="6">
-        <v>2000000</v>
-      </c>
-      <c r="H4" s="5">
-        <v>874224.21238739789</v>
-      </c>
-      <c r="I4" s="5">
-        <v>55419.078125</v>
-      </c>
-      <c r="J4" s="5">
-        <v>188103.75</v>
-      </c>
-      <c r="K4" s="5">
-        <v>310067.53125</v>
-      </c>
-      <c r="L4" s="5">
-        <v>866552.875</v>
-      </c>
-      <c r="M4" s="6">
-        <v>2000000</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2015239.25</v>
-      </c>
-      <c r="O4" s="1">
-        <v>9631540</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="1" t="s">
-        <v>81</v>
+      <c r="M3" s="39"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Before running everything again
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb550905\Github\VEN\data_management\management\4. income imputation\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233CECE-24FF-4E3D-9BD6-E21EE701AC21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="missing_values" sheetId="1" r:id="rId1"/>
@@ -20,15 +14,7 @@
     <sheet name="nonlabor_imp_stochastic_reg" sheetId="4" r:id="rId5"/>
     <sheet name="labor_beneimp_stochastic_reg" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -305,7 +291,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -526,66 +512,66 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,14 +579,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -900,22 +878,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="false" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" style="1" customWidth="true"/>
+    <col min="2" max="2" width="11.88671875" style="2" customWidth="true"/>
+    <col min="3" max="3" width="12.5546875" style="2" bestFit="true" customWidth="true"/>
     <col min="4" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1">
       <c r="B1" s="10" t="s">
         <v>73</v>
       </c>
@@ -923,78 +901,186 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8">
+    <row r="4" ht="28.8">
       <c r="A4" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="16">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C4" s="17">
-        <v>1.4345210550670986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8">
+        <v>1.3573962671602653</v>
+      </c>
+      <c r="D4" s="1">
+        <v>176</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.3573962671602653</v>
+      </c>
+      <c r="F4" s="1">
+        <v>176</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.3573962671602653</v>
+      </c>
+      <c r="H4" s="1">
+        <v>176</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1.3573962671602653</v>
+      </c>
+    </row>
+    <row r="5" ht="28.8">
       <c r="A5" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="18">
-        <v>356</v>
+        <v>651</v>
       </c>
       <c r="C5" s="19">
-        <v>2.7456424494832641</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8">
+        <v>5.0208236927348455</v>
+      </c>
+      <c r="D5" s="1">
+        <v>651</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5.0208236927348455</v>
+      </c>
+      <c r="F5" s="1">
+        <v>651</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5.0208236927348455</v>
+      </c>
+      <c r="H5" s="1">
+        <v>651</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5.0208236927348455</v>
+      </c>
+    </row>
+    <row r="6" ht="28.8">
       <c r="A6" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="20">
-        <v>1675</v>
+        <v>1687</v>
       </c>
       <c r="C6" s="21">
-        <v>12.91840197439457</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>13.010951719882771</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1687</v>
+      </c>
+      <c r="E6" s="1">
+        <v>13.010951719882771</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1687</v>
+      </c>
+      <c r="G6" s="1">
+        <v>13.010951719882771</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1687</v>
+      </c>
+      <c r="I6" s="1">
+        <v>13.010951719882771</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="22">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="23">
-        <v>0.331636587999383</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>0.31621163041801637</v>
+      </c>
+      <c r="D7" s="1">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.31621163041801637</v>
+      </c>
+      <c r="F7" s="1">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.31621163041801637</v>
+      </c>
+      <c r="H7" s="1">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.31621163041801637</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="24">
-        <v>2074</v>
+        <v>2379</v>
       </c>
       <c r="C8" s="25">
-        <v>15.995681011877217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>18.347987043035634</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2379</v>
+      </c>
+      <c r="E8" s="1">
+        <v>18.347987043035634</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2379</v>
+      </c>
+      <c r="G8" s="1">
+        <v>18.347987043035634</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2379</v>
+      </c>
+      <c r="I8" s="1">
+        <v>18.347987043035634</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="16">
-        <v>10672</v>
+        <v>10377</v>
       </c>
       <c r="C9" s="17">
-        <v>82.307573654172444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>80.032392410920878</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10377</v>
+      </c>
+      <c r="E9" s="1">
+        <v>80.032392410920878</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10377</v>
+      </c>
+      <c r="G9" s="1">
+        <v>80.032392410920878</v>
+      </c>
+      <c r="H9" s="1">
+        <v>10377</v>
+      </c>
+      <c r="I9" s="1">
+        <v>80.032392410920878</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="13" t="s">
         <v>57</v>
       </c>
@@ -1004,23 +1090,41 @@
       <c r="C10" s="27">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="1">
+        <v>12966</v>
+      </c>
+      <c r="E10" s="1">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1">
+        <v>12966</v>
+      </c>
+      <c r="G10" s="1">
+        <v>100</v>
+      </c>
+      <c r="H10" s="1">
+        <v>12966</v>
+      </c>
+      <c r="I10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="C11" s="28"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12">
       <c r="C12" s="28"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13">
       <c r="A13" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="28"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14">
       <c r="C14" s="28"/>
     </row>
-    <row r="15" spans="1:3" ht="28.8">
+    <row r="15" ht="28.8">
       <c r="A15" s="12" t="s">
         <v>59</v>
       </c>
@@ -1030,19 +1134,55 @@
       <c r="C15" s="17">
         <v>374.6724193032918</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8">
+      <c r="D15" s="1">
+        <v>23447</v>
+      </c>
+      <c r="E15" s="1">
+        <v>374.6724193032918</v>
+      </c>
+      <c r="F15" s="1">
+        <v>23447</v>
+      </c>
+      <c r="G15" s="1">
+        <v>374.6724193032918</v>
+      </c>
+      <c r="H15" s="1">
+        <v>23447</v>
+      </c>
+      <c r="I15" s="1">
+        <v>374.6724193032918</v>
+      </c>
+    </row>
+    <row r="16" ht="28.8">
       <c r="A16" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="18">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="C16" s="19">
-        <v>0.11185682326621924</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8">
+        <v>2.348993288590604</v>
+      </c>
+      <c r="D16" s="1">
+        <v>147</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.348993288590604</v>
+      </c>
+      <c r="F16" s="1">
+        <v>147</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2.348993288590604</v>
+      </c>
+      <c r="H16" s="1">
+        <v>147</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2.348993288590604</v>
+      </c>
+    </row>
+    <row r="17" ht="28.8">
       <c r="A17" s="12" t="s">
         <v>61</v>
       </c>
@@ -1052,41 +1192,113 @@
       <c r="C17" s="21">
         <v>0.28763183125599234</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="1">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.28763183125599234</v>
+      </c>
+      <c r="F17" s="1">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.28763183125599234</v>
+      </c>
+      <c r="H17" s="1">
+        <v>18</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.28763183125599234</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="23">
-        <v>0.11185682326621924</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>0.095877277085330767</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.095877277085330767</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.095877277085330767</v>
+      </c>
+      <c r="H18" s="1">
+        <v>6</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.095877277085330767</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="24">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="C19" s="25">
-        <v>0.51134547778843076</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>2.7325023969319271</v>
+      </c>
+      <c r="D19" s="1">
+        <v>171</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2.7325023969319271</v>
+      </c>
+      <c r="F19" s="1">
+        <v>171</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2.7325023969319271</v>
+      </c>
+      <c r="H19" s="1">
+        <v>171</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2.7325023969319271</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="16">
-        <v>6163</v>
+        <v>6024</v>
       </c>
       <c r="C20" s="17">
-        <v>98.4819431128156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29.4" customHeight="1">
+        <v>96.260786193672104</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6024</v>
+      </c>
+      <c r="E20" s="1">
+        <v>96.260786193672104</v>
+      </c>
+      <c r="F20" s="1">
+        <v>6024</v>
+      </c>
+      <c r="G20" s="1">
+        <v>96.260786193672104</v>
+      </c>
+      <c r="H20" s="1">
+        <v>6024</v>
+      </c>
+      <c r="I20" s="1">
+        <v>96.260786193672104</v>
+      </c>
+    </row>
+    <row r="21" ht="29.4" customHeight="true">
       <c r="A21" s="13" t="s">
         <v>62</v>
       </c>
@@ -1096,23 +1308,41 @@
       <c r="C21" s="27">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="1">
+        <v>6258</v>
+      </c>
+      <c r="E21" s="1">
+        <v>100</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6258</v>
+      </c>
+      <c r="G21" s="1">
+        <v>100</v>
+      </c>
+      <c r="H21" s="1">
+        <v>6258</v>
+      </c>
+      <c r="I21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="C22" s="28"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23">
       <c r="C23" s="28"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24">
       <c r="A24" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="28"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25">
       <c r="C25" s="28"/>
     </row>
-    <row r="26" spans="1:3" ht="28.8">
+    <row r="26" ht="28.8">
       <c r="A26" s="12" t="s">
         <v>64</v>
       </c>
@@ -1122,19 +1352,55 @@
       <c r="C26" s="17">
         <v>1.6816143497757847</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="28.8">
+      <c r="D26" s="1">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.6816143497757847</v>
+      </c>
+      <c r="F26" s="1">
+        <v>15</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1.6816143497757847</v>
+      </c>
+      <c r="H26" s="1">
+        <v>15</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1.6816143497757847</v>
+      </c>
+    </row>
+    <row r="27" ht="28.8">
       <c r="A27" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="18">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="C27" s="19">
-        <v>2.2421524663677128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>6.6143497757847527</v>
+      </c>
+      <c r="D27" s="1">
+        <v>59</v>
+      </c>
+      <c r="E27" s="1">
+        <v>6.6143497757847527</v>
+      </c>
+      <c r="F27" s="1">
+        <v>59</v>
+      </c>
+      <c r="G27" s="1">
+        <v>6.6143497757847527</v>
+      </c>
+      <c r="H27" s="1">
+        <v>59</v>
+      </c>
+      <c r="I27" s="1">
+        <v>6.6143497757847527</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="12" t="s">
         <v>54</v>
       </c>
@@ -1144,30 +1410,84 @@
       <c r="C28" s="23">
         <v>0.22421524663677131</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.22421524663677131</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.22421524663677131</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.22421524663677131</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" s="13" t="s">
         <v>66</v>
       </c>
       <c r="B29" s="29">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="C29" s="30">
-        <v>2.4663677130044843</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>6.8385650224215251</v>
+      </c>
+      <c r="D29" s="1">
+        <v>61</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6.8385650224215251</v>
+      </c>
+      <c r="F29" s="1">
+        <v>61</v>
+      </c>
+      <c r="G29" s="1">
+        <v>6.8385650224215251</v>
+      </c>
+      <c r="H29" s="1">
+        <v>61</v>
+      </c>
+      <c r="I29" s="1">
+        <v>6.8385650224215251</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="16">
-        <v>855</v>
+        <v>816</v>
       </c>
       <c r="C30" s="17">
-        <v>95.852017937219742</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>91.479820627802695</v>
+      </c>
+      <c r="D30" s="1">
+        <v>816</v>
+      </c>
+      <c r="E30" s="1">
+        <v>91.479820627802695</v>
+      </c>
+      <c r="F30" s="1">
+        <v>816</v>
+      </c>
+      <c r="G30" s="1">
+        <v>91.479820627802695</v>
+      </c>
+      <c r="H30" s="1">
+        <v>816</v>
+      </c>
+      <c r="I30" s="1">
+        <v>91.479820627802695</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" s="31" t="s">
         <v>67</v>
       </c>
@@ -1177,23 +1497,41 @@
       <c r="C31" s="33">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="1">
+        <v>892</v>
+      </c>
+      <c r="E31" s="1">
+        <v>100</v>
+      </c>
+      <c r="F31" s="1">
+        <v>892</v>
+      </c>
+      <c r="G31" s="1">
+        <v>100</v>
+      </c>
+      <c r="H31" s="1">
+        <v>892</v>
+      </c>
+      <c r="I31" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="C32" s="28"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33">
       <c r="C33" s="28"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34">
       <c r="A34" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C34" s="28"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35">
       <c r="C35" s="28"/>
     </row>
-    <row r="36" spans="1:3" ht="28.8">
+    <row r="36" ht="28.8">
       <c r="A36" s="12" t="s">
         <v>69</v>
       </c>
@@ -1204,47 +1542,51 @@
         <v>313.96250000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="28.8">
+    <row r="37" ht="28.8">
       <c r="A37" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B37" s="18">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="C37" s="19">
-        <v>0.71250000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="23"/>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="B38" s="22">
+        <v>64</v>
+      </c>
+      <c r="C38" s="23">
+        <v>0.80000000000000004</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" s="13" t="s">
         <v>66</v>
       </c>
       <c r="B39" s="29">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="C39" s="30">
-        <v>0.71250000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B40" s="16">
-        <v>7936</v>
+        <v>7753</v>
       </c>
       <c r="C40" s="17">
-        <v>99.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>96.912499999999994</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41" s="31" t="s">
         <v>71</v>
       </c>
@@ -1255,7 +1597,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43">
       <c r="A43" s="15" t="s">
         <v>72</v>
       </c>
@@ -1266,154 +1608,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="false" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="1" customWidth="true"/>
+    <col min="2" max="2" width="8.109375" style="1" customWidth="true"/>
+    <col min="3" max="3" width="8.77734375" style="1" customWidth="true"/>
     <col min="4" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="15.6">
+    <row r="1" s="5" customFormat="true" ht="15.6">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="43.2">
+    <row r="2" s="5" customFormat="true" ht="43.2">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+    </row>
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="34">
-        <v>31.3404050144648</v>
+        <v>33.039092055485497</v>
       </c>
       <c r="C3" s="35">
-        <v>50</v>
+        <v>54.970760233918128</v>
       </c>
       <c r="E3" s="28"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1">
+    <row r="4" s="6" customFormat="true">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="34">
-        <v>68.659594985535193</v>
+        <v>66.960907944514503</v>
       </c>
       <c r="C4" s="35">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>45.029239766081872</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="35"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="34">
-        <v>0.33751205400192863</v>
+        <v>0.33627574611181166</v>
       </c>
       <c r="C6" s="35">
-        <v>0</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D6" s="28"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="34">
-        <v>12.391513982642238</v>
+        <v>12.35813366960908</v>
       </c>
       <c r="C7" s="35">
         <v>0</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="34">
-        <v>22.709739633558339</v>
+        <v>22.320302648171499</v>
       </c>
       <c r="C8" s="35">
         <v>0</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="34">
-        <v>23.288331726133077</v>
+        <v>23.245060949978981</v>
       </c>
       <c r="C9" s="35">
-        <v>3.125</v>
+        <v>1.1695906432748537</v>
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="34">
-        <v>19.913211186113791</v>
+        <v>20.638923917612441</v>
       </c>
       <c r="C10" s="35">
-        <v>15.625</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="34">
-        <v>14.609450337512053</v>
+        <v>14.543926019335856</v>
       </c>
       <c r="C11" s="35">
-        <v>37.5</v>
+        <v>39.1812865497076</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="34">
-        <v>6.750241080038573</v>
+        <v>6.557377049180328</v>
       </c>
       <c r="C12" s="35">
-        <v>43.75</v>
+        <v>53.801169590643269</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13">
       <c r="A13" s="7" t="s">
         <v>80</v>
       </c>
@@ -1421,79 +1759,79 @@
       <c r="C13" s="35"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="34">
-        <v>24.541947926711668</v>
+        <v>24.506094997898277</v>
       </c>
       <c r="C14" s="35">
-        <v>31.25</v>
+        <v>38.011695906432749</v>
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="34">
-        <v>32.497589199614275</v>
+        <v>32.492643968053805</v>
       </c>
       <c r="C15" s="35">
-        <v>25</v>
+        <v>15.789473684210526</v>
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="34">
-        <v>29.411764705882355</v>
+        <v>29.087852038671713</v>
       </c>
       <c r="C16" s="35">
-        <v>9.375</v>
+        <v>9.9415204678362574</v>
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="34">
-        <v>10.752169720347156</v>
+        <v>10.928961748633879</v>
       </c>
       <c r="C17" s="35">
-        <v>15.625</v>
+        <v>12.865497076023392</v>
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="34">
-        <v>2.651880424300868</v>
+        <v>2.8583438419503993</v>
       </c>
       <c r="C18" s="35">
-        <v>18.75</v>
+        <v>22.807017543859647</v>
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="34">
-        <v>0.14464802314368372</v>
+        <v>0.12610340479192939</v>
       </c>
       <c r="C19" s="35">
-        <v>0</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1501,103 +1839,103 @@
       <c r="C20" s="35"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="34">
-        <v>0.33751205400192863</v>
+        <v>0.29424127784783521</v>
       </c>
       <c r="C21" s="35">
         <v>0</v>
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="34">
-        <v>0.14464802314368372</v>
+        <v>0.12610340479192939</v>
       </c>
       <c r="C22" s="35">
-        <v>0</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" s="8" customFormat="1">
+    <row r="23" s="8" customFormat="true">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="34">
-        <v>26.808100289296043</v>
+        <v>26.691887347625055</v>
       </c>
       <c r="C23" s="35">
-        <v>40.625</v>
+        <v>49.122807017543856</v>
       </c>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="34">
-        <v>47.782063645130187</v>
+        <v>46.784363177805801</v>
       </c>
       <c r="C24" s="35">
-        <v>21.875</v>
+        <v>23.391812865497073</v>
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="34">
-        <v>5.4001928640308581</v>
+        <v>5.9688944934846573</v>
       </c>
       <c r="C25" s="35">
-        <v>6.25</v>
+        <v>8.1871345029239766</v>
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="34">
-        <v>14.271938283510124</v>
+        <v>14.754098360655737</v>
       </c>
       <c r="C26" s="35">
-        <v>15.625</v>
+        <v>8.7719298245614024</v>
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="34">
-        <v>0.48216007714561238</v>
+        <v>0.67255149222362332</v>
       </c>
       <c r="C27" s="35">
         <v>0</v>
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="34">
-        <v>4.7733847637415625</v>
+        <v>4.7078604455653634</v>
       </c>
       <c r="C28" s="35">
-        <v>15.625</v>
+        <v>9.9415204678362574</v>
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29">
       <c r="A29" s="7" t="s">
         <v>22</v>
       </c>
@@ -1605,103 +1943,103 @@
       <c r="C29" s="35"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="34">
-        <v>4.6769527483124396</v>
+        <v>9.3316519546027745</v>
       </c>
       <c r="C30" s="35">
-        <v>0</v>
+        <v>8.7719298245614024</v>
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="34">
-        <v>4.725168756027001</v>
+        <v>6.9356872635561162</v>
       </c>
       <c r="C31" s="35">
-        <v>0</v>
+        <v>2.9239766081871341</v>
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="34">
-        <v>11.041465766634524</v>
+        <v>10.004203446826397</v>
       </c>
       <c r="C32" s="35">
-        <v>3.125</v>
+        <v>2.9239766081871341</v>
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="34">
-        <v>72.275795564127293</v>
+        <v>66.876839007986547</v>
       </c>
       <c r="C33" s="35">
-        <v>18.75</v>
+        <v>12.280701754385964</v>
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="34">
-        <v>0.43394406943105107</v>
+        <v>0.50441361916771754</v>
       </c>
       <c r="C34" s="35">
         <v>0</v>
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="34">
-        <v>4.0019286403085825</v>
+        <v>3.6990332072299283</v>
       </c>
       <c r="C35" s="35">
         <v>0</v>
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="34">
-        <v>2.651880424300868</v>
+        <v>2.3118957545187055</v>
       </c>
       <c r="C36" s="35">
-        <v>0</v>
+        <v>1.7543859649122806</v>
       </c>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="34">
-        <v>0.19286403085824494</v>
+        <v>0.33627574611181166</v>
       </c>
       <c r="C37" s="35">
-        <v>78.125</v>
+        <v>71.345029239766077</v>
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38">
       <c r="A38" s="8" t="s">
         <v>31</v>
       </c>
@@ -1709,140 +2047,140 @@
       <c r="C38" s="35"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="34">
-        <v>18.659594985535197</v>
+        <v>18.032786885245901</v>
       </c>
       <c r="C39" s="35">
-        <v>0</v>
+        <v>5.8479532163742682</v>
       </c>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B40" s="34">
-        <v>0.67502410800385726</v>
+        <v>0.58848255569567043</v>
       </c>
       <c r="C40" s="35">
-        <v>3.125</v>
+        <v>1.1695906432748537</v>
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:5" s="8" customFormat="1">
+    <row r="41" s="8" customFormat="true">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="34">
-        <v>1.832208293153327</v>
+        <v>1.807482135350988</v>
       </c>
       <c r="C41" s="35">
-        <v>3.125</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="34">
-        <v>1.1571841851494697</v>
+        <v>1.3871374527112232</v>
       </c>
       <c r="C42" s="35">
-        <v>0</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="34">
-        <v>5.7859209257473481</v>
+        <v>5.6326187473728462</v>
       </c>
       <c r="C43" s="35">
-        <v>3.125</v>
+        <v>2.3391812865497075</v>
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="34">
-        <v>20.588235294117645</v>
+        <v>20.176544766708702</v>
       </c>
       <c r="C44" s="35">
-        <v>3.125</v>
+        <v>1.7543859649122806</v>
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B45" s="34">
-        <v>12.391513982642238</v>
+        <v>11.601513240857503</v>
       </c>
       <c r="C45" s="35">
-        <v>0</v>
+        <v>2.3391812865497075</v>
       </c>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B46" s="34">
-        <v>2.892960462873674</v>
+        <v>3.278688524590164</v>
       </c>
       <c r="C46" s="35">
-        <v>0</v>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="34">
-        <v>6.075216972034716</v>
+        <v>8.9533417402269855</v>
       </c>
       <c r="C47" s="35">
-        <v>3.125</v>
+        <v>7.0175438596491224</v>
       </c>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B48" s="34">
-        <v>29.749276759884282</v>
+        <v>28.205128205128204</v>
       </c>
       <c r="C48" s="35">
-        <v>6.25</v>
+        <v>6.4327485380116958</v>
       </c>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B49" s="34">
-        <v>0.19286403085824494</v>
+        <v>0.33627574611181166</v>
       </c>
       <c r="C49" s="35">
-        <v>78.125</v>
+        <v>71.345029239766077</v>
       </c>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50">
       <c r="A50" s="8" t="s">
         <v>44</v>
       </c>
@@ -1850,31 +2188,31 @@
       <c r="C50" s="35"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="34">
-        <v>18.900675024108004</v>
+        <v>19.630096679277006</v>
       </c>
       <c r="C51" s="35">
-        <v>15.625</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="34">
-        <v>81.099324975891989</v>
+        <v>80.369903320722997</v>
       </c>
       <c r="C52" s="35">
-        <v>84.375</v>
+        <v>89.473684210526315</v>
       </c>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" s="8" customFormat="1">
+    <row r="53" s="8" customFormat="true">
       <c r="B53" s="34">
         <v>0</v>
       </c>
@@ -1883,197 +2221,197 @@
       </c>
       <c r="D53" s="9"/>
     </row>
-    <row r="54" spans="1:4">
-      <c r="B54"/>
-      <c r="C54"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="B55"/>
-      <c r="C55"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="B56"/>
-      <c r="C56"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="B57"/>
-      <c r="C57"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="B58"/>
-      <c r="C58"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="B59"/>
-      <c r="C59"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="B60"/>
-      <c r="C60"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="B61"/>
-      <c r="C61"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="B62"/>
-      <c r="C62"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="B63"/>
-      <c r="C63"/>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="B64"/>
-      <c r="C64"/>
-    </row>
-    <row r="65" spans="2:3">
-      <c r="B65"/>
-      <c r="C65"/>
-    </row>
-    <row r="66" spans="2:3">
-      <c r="B66"/>
-      <c r="C66"/>
-    </row>
-    <row r="67" spans="2:3">
-      <c r="B67"/>
-      <c r="C67"/>
-    </row>
-    <row r="68" spans="2:3">
-      <c r="B68"/>
-      <c r="C68"/>
-    </row>
-    <row r="69" spans="2:3">
-      <c r="B69"/>
-      <c r="C69"/>
-    </row>
-    <row r="70" spans="2:3">
-      <c r="B70"/>
-      <c r="C70"/>
-    </row>
-    <row r="71" spans="2:3">
-      <c r="B71"/>
-      <c r="C71"/>
-    </row>
-    <row r="72" spans="2:3">
-      <c r="B72"/>
-      <c r="C72"/>
-    </row>
-    <row r="73" spans="2:3">
-      <c r="B73"/>
-      <c r="C73"/>
-    </row>
-    <row r="74" spans="2:3">
-      <c r="B74"/>
-      <c r="C74"/>
-    </row>
-    <row r="75" spans="2:3">
-      <c r="B75"/>
-      <c r="C75"/>
-    </row>
-    <row r="76" spans="2:3">
-      <c r="B76"/>
-      <c r="C76"/>
-    </row>
-    <row r="77" spans="2:3">
-      <c r="B77"/>
-      <c r="C77"/>
-    </row>
-    <row r="78" spans="2:3">
-      <c r="B78"/>
-      <c r="C78"/>
-    </row>
-    <row r="79" spans="2:3">
-      <c r="B79"/>
-      <c r="C79"/>
-    </row>
-    <row r="80" spans="2:3">
-      <c r="B80"/>
-      <c r="C80"/>
-    </row>
-    <row r="81" spans="2:3">
-      <c r="B81"/>
-      <c r="C81"/>
-    </row>
-    <row r="82" spans="2:3">
-      <c r="B82"/>
-      <c r="C82"/>
-    </row>
-    <row r="83" spans="2:3">
-      <c r="B83"/>
-      <c r="C83"/>
-    </row>
-    <row r="84" spans="2:3">
-      <c r="B84"/>
-      <c r="C84"/>
-    </row>
-    <row r="85" spans="2:3">
-      <c r="B85"/>
-      <c r="C85"/>
-    </row>
-    <row r="86" spans="2:3">
-      <c r="B86"/>
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="2:3">
-      <c r="B87"/>
-      <c r="C87"/>
-    </row>
-    <row r="88" spans="2:3">
-      <c r="B88"/>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="2:3">
-      <c r="B89"/>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="2:3">
-      <c r="B90"/>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="2:3">
-      <c r="B91"/>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="2:3">
-      <c r="B92"/>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="2:3">
-      <c r="B93"/>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="2:3">
-      <c r="B94"/>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="2:3">
-      <c r="B95"/>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="2:3">
-      <c r="B96"/>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="2:3">
-      <c r="B97"/>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="2:3">
-      <c r="B98"/>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="2:3">
-      <c r="B99"/>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="2:3">
-      <c r="B100"/>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="2:3">
-      <c r="B101"/>
-      <c r="C101"/>
+    <row r="54">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72">
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73">
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77">
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82">
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83">
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89">
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92">
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98">
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99">
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101">
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2082,7 +2420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2092,15 +2430,15 @@
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.77734375" style="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="true" customWidth="true"/>
+    <col min="3" max="4" width="8.77734375" style="1" bestFit="true" customWidth="true"/>
+    <col min="5" max="8" width="9.33203125" style="1" bestFit="true" customWidth="true"/>
+    <col min="9" max="10" width="8.77734375" style="1" bestFit="true" customWidth="true"/>
+    <col min="11" max="13" width="9.33203125" style="1" bestFit="true" customWidth="true"/>
     <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1">
       <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
@@ -2119,7 +2457,7 @@
       <c r="L1" s="40"/>
       <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2">
       <c r="A2" s="41" t="s">
         <v>84</v>
       </c>
@@ -2158,7 +2496,7 @@
       </c>
       <c r="M2" s="38"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1">
+    <row r="3" s="2" customFormat="true">
       <c r="A3" s="42">
         <v>2006937.0944554566</v>
       </c>
@@ -2197,13 +2535,13 @@
       </c>
       <c r="M3" s="39"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4">
       <c r="M4" s="38"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5">
       <c r="M5" s="38"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
@@ -2219,7 +2557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2229,15 +2567,15 @@
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.77734375" style="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="true" customWidth="true"/>
+    <col min="3" max="4" width="8.77734375" style="1" bestFit="true" customWidth="true"/>
+    <col min="5" max="8" width="9.33203125" style="1" bestFit="true" customWidth="true"/>
+    <col min="9" max="10" width="8.77734375" style="1" bestFit="true" customWidth="true"/>
+    <col min="11" max="13" width="9.33203125" style="1" bestFit="true" customWidth="true"/>
     <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1">
       <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
@@ -2256,7 +2594,7 @@
       <c r="L1" s="40"/>
       <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2">
       <c r="A2" s="41" t="s">
         <v>84</v>
       </c>
@@ -2295,7 +2633,7 @@
       </c>
       <c r="M2" s="38"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1">
+    <row r="3" s="2" customFormat="true">
       <c r="A3" s="42">
         <v>1518811.1937084021</v>
       </c>
@@ -2336,7 +2674,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1">
+    <row r="4" s="2" customFormat="true">
       <c r="A4" s="43"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -2353,7 +2691,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
@@ -2368,7 +2706,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2380,7 +2718,7 @@
     <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1">
       <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
@@ -2399,7 +2737,7 @@
       <c r="L1" s="40"/>
       <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2">
       <c r="A2" s="41" t="s">
         <v>84</v>
       </c>
@@ -2440,7 +2778,7 @@
       <c r="N2" s="38"/>
       <c r="O2" s="38"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1">
+    <row r="3" s="2" customFormat="true">
       <c r="A3" s="42">
         <v>9411043.7327192165</v>
       </c>
@@ -2481,12 +2819,12 @@
       <c r="N3" s="38"/>
       <c r="O3" s="38"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4">
       <c r="M4" s="38"/>
       <c r="N4" s="38"/>
       <c r="O4" s="38"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>77</v>
       </c>
@@ -2501,10 +2839,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2513,7 +2851,7 @@
     <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1">
       <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
@@ -2532,7 +2870,7 @@
       <c r="L1" s="40"/>
       <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2">
       <c r="A2" s="41" t="s">
         <v>84</v>
       </c>
@@ -2570,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1">
+    <row r="3" s="2" customFormat="true">
       <c r="A3" s="42">
         <v>865994.29392043944</v>
       </c>
@@ -2611,7 +2949,7 @@
       <c r="N3" s="38"/>
       <c r="O3" s="38"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
New weights, hh without head, miembros, pondera_hh
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -4832,10 +4832,10 @@
         <v>54</v>
       </c>
       <c r="B38" s="0">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="C38" s="0">
-        <v>0.9375</v>
+        <v>1.2749999999999999</v>
       </c>
     </row>
     <row r="39">
@@ -4854,10 +4854,10 @@
         <v>56</v>
       </c>
       <c r="B40" s="0">
-        <v>7861</v>
+        <v>7834</v>
       </c>
       <c r="C40" s="0">
-        <v>98.262500000000003</v>
+        <v>97.924999999999997</v>
       </c>
     </row>
     <row r="41">
@@ -5775,13 +5775,13 @@
     </row>
     <row r="3" s="2" customFormat="true">
       <c r="A3" s="0">
-        <v>2007271.323501125</v>
+        <v>2007357.2352610789</v>
       </c>
       <c r="B3" s="0">
-        <v>250166.609375</v>
+        <v>250197.34375</v>
       </c>
       <c r="C3" s="0">
-        <v>455755.0625</v>
+        <v>455767.578125</v>
       </c>
       <c r="D3" s="0">
         <v>1000000</v>
@@ -5790,25 +5790,25 @@
         <v>2653803.75</v>
       </c>
       <c r="F3" s="0">
-        <v>4002665.5</v>
+        <v>4003157</v>
       </c>
       <c r="G3" s="0">
-        <v>2061953.882068218</v>
+        <v>2079280.2081727833</v>
       </c>
       <c r="H3" s="0">
-        <v>300000</v>
+        <v>270213.125</v>
       </c>
       <c r="I3" s="0">
-        <v>500333.25</v>
+        <v>500000</v>
       </c>
       <c r="J3" s="0">
-        <v>1400000</v>
+        <v>1053030.25</v>
       </c>
       <c r="K3" s="0">
-        <v>2654103.5</v>
+        <v>2653803.75</v>
       </c>
       <c r="L3" s="0">
-        <v>3862057.25</v>
+        <v>4203804</v>
       </c>
       <c r="M3" s="20"/>
     </row>
@@ -5913,40 +5913,40 @@
     </row>
     <row r="3" s="2" customFormat="true">
       <c r="A3" s="0">
-        <v>1518884.0054644204</v>
+        <v>1518900.9281340449</v>
       </c>
       <c r="B3" s="0">
         <v>250000</v>
       </c>
       <c r="C3" s="0">
-        <v>250166.609375</v>
+        <v>250197.34375</v>
       </c>
       <c r="D3" s="0">
         <v>2203803.75</v>
       </c>
       <c r="E3" s="0">
-        <v>2453970.25</v>
+        <v>2454001</v>
       </c>
       <c r="F3" s="0">
-        <v>2554037</v>
+        <v>2554080</v>
       </c>
       <c r="G3" s="0">
-        <v>1518197.6367921263</v>
+        <v>1517309.3726285503</v>
       </c>
       <c r="H3" s="0">
         <v>250000</v>
       </c>
       <c r="I3" s="0">
-        <v>250166.609375</v>
+        <v>250197.34375</v>
       </c>
       <c r="J3" s="0">
         <v>2203803.75</v>
       </c>
       <c r="K3" s="0">
-        <v>2453970.25</v>
+        <v>2454001</v>
       </c>
       <c r="L3" s="0">
-        <v>2554037</v>
+        <v>2554080</v>
       </c>
       <c r="M3" s="20"/>
       <c r="N3" s="1"/>
@@ -6059,40 +6059,40 @@
     </row>
     <row r="3" s="2" customFormat="true">
       <c r="A3" s="0">
-        <v>447445.45137360872</v>
+        <v>434814.74970929569</v>
       </c>
       <c r="B3" s="0">
         <v>120000</v>
       </c>
       <c r="C3" s="0">
-        <v>200133.28125</v>
+        <v>200157.875</v>
       </c>
       <c r="D3" s="0">
         <v>300000</v>
       </c>
       <c r="E3" s="0">
-        <v>500000</v>
+        <v>484000</v>
       </c>
       <c r="F3" s="0">
-        <v>850000</v>
+        <v>840515.125</v>
       </c>
       <c r="G3" s="0">
-        <v>447766.59699393006</v>
+        <v>434861.08810818463</v>
       </c>
       <c r="H3" s="0">
-        <v>120079.96875</v>
+        <v>120094.71875</v>
       </c>
       <c r="I3" s="0">
-        <v>200133.28125</v>
+        <v>200157.875</v>
       </c>
       <c r="J3" s="0">
         <v>300000</v>
       </c>
       <c r="K3" s="0">
-        <v>500000</v>
+        <v>486968.09375</v>
       </c>
       <c r="L3" s="0">
-        <v>850000</v>
+        <v>840515.125</v>
       </c>
       <c r="M3" s="20"/>
       <c r="N3" s="19"/>
@@ -6190,40 +6190,40 @@
     </row>
     <row r="3" s="2" customFormat="true">
       <c r="A3" s="0">
-        <v>866155.67797133105</v>
+        <v>866184.52546126244</v>
       </c>
       <c r="B3" s="0">
-        <v>55036.65234375</v>
+        <v>55043.4140625</v>
       </c>
       <c r="C3" s="0">
-        <v>188828.65625</v>
+        <v>188879.8125</v>
       </c>
       <c r="D3" s="0">
-        <v>300199.9375</v>
+        <v>300236.8125</v>
       </c>
       <c r="E3" s="0">
-        <v>856605.3125</v>
+        <v>856565.625</v>
       </c>
       <c r="F3" s="0">
         <v>2000000</v>
       </c>
       <c r="G3" s="0">
-        <v>897986.15396221553</v>
+        <v>894069.06448190357</v>
       </c>
       <c r="H3" s="0">
         <v>60000</v>
       </c>
       <c r="I3" s="0">
-        <v>200000</v>
+        <v>195153.921875</v>
       </c>
       <c r="J3" s="0">
-        <v>328218.59375</v>
+        <v>310810.9375</v>
       </c>
       <c r="K3" s="0">
-        <v>922291.1875</v>
+        <v>870270.625</v>
       </c>
       <c r="L3" s="0">
-        <v>2001332.875</v>
+        <v>2000000</v>
       </c>
       <c r="M3" s="20"/>
       <c r="N3" s="19"/>

</xml_diff>

<commit_message>
Last corrida of database 5/1
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019.xlsx
@@ -5793,22 +5793,22 @@
         <v>4003157</v>
       </c>
       <c r="G3" s="0">
-        <v>2079280.2081727833</v>
+        <v>2062039.5297215781</v>
       </c>
       <c r="H3" s="0">
-        <v>270213.125</v>
+        <v>300000</v>
       </c>
       <c r="I3" s="0">
-        <v>500000</v>
+        <v>500394.75</v>
       </c>
       <c r="J3" s="0">
-        <v>1053030.25</v>
+        <v>1400000</v>
       </c>
       <c r="K3" s="0">
-        <v>2653803.75</v>
+        <v>2654159</v>
       </c>
       <c r="L3" s="0">
-        <v>4203804</v>
+        <v>3862165</v>
       </c>
       <c r="M3" s="20"/>
     </row>
@@ -5931,7 +5931,7 @@
         <v>2554080</v>
       </c>
       <c r="G3" s="0">
-        <v>1517309.3726285503</v>
+        <v>1518214.4247522387</v>
       </c>
       <c r="H3" s="0">
         <v>250000</v>
@@ -6077,7 +6077,7 @@
         <v>840515.125</v>
       </c>
       <c r="G3" s="0">
-        <v>434861.08810818463</v>
+        <v>435286.01169894467</v>
       </c>
       <c r="H3" s="0">
         <v>120094.71875</v>
@@ -6089,10 +6089,10 @@
         <v>300000</v>
       </c>
       <c r="K3" s="0">
-        <v>486968.09375</v>
+        <v>486977.59375</v>
       </c>
       <c r="L3" s="0">
-        <v>840515.125</v>
+        <v>834000</v>
       </c>
       <c r="M3" s="20"/>
       <c r="N3" s="19"/>
@@ -6208,22 +6208,22 @@
         <v>2000000</v>
       </c>
       <c r="G3" s="0">
-        <v>894069.06448190357</v>
+        <v>898015.88863384188</v>
       </c>
       <c r="H3" s="0">
         <v>60000</v>
       </c>
       <c r="I3" s="0">
-        <v>195153.921875</v>
+        <v>200000</v>
       </c>
       <c r="J3" s="0">
-        <v>310810.9375</v>
+        <v>328258.90625</v>
       </c>
       <c r="K3" s="0">
-        <v>870270.625</v>
+        <v>922541.125</v>
       </c>
       <c r="L3" s="0">
-        <v>2000000</v>
+        <v>2001578.75</v>
       </c>
       <c r="M3" s="20"/>
       <c r="N3" s="19"/>

</xml_diff>